<commit_message>
Changed from Orbital.all(params) Orbital.get(): latter is faster.
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -7,7 +7,8 @@
     <workbookView xWindow="26220" yWindow="860" windowWidth="21600" windowHeight="15260" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId1"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -46,6 +47,18 @@
   </si>
   <si>
     <t>pt_element: construct class for each term</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pt_element: construct pre_class once</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@base.all()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@base.get()</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -89,9 +102,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,16 +435,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.24570099999999978</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(D6:D32)</f>
+        <v>0.3320297999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.0237555966569346E-2</v>
+      </c>
+      <c r="D4">
+        <f>STDEVA(D6:D32)</f>
+        <v>3.7396661477998347E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>8.2366599918475558E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D4/D3</f>
+        <v>0.11263043702100954</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.275005</v>
+      </c>
+      <c r="D6">
+        <v>0.32842199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.23533599999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.37503599999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.224244999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.27442299999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.23674799999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.35225099999999898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.25717099999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.33001699999999901</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -438,7 +586,7 @@
         <v>6</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
pt_element: instead of composing ec class for each span in a term, compose it once (as class_nl, formerly pre_class) and use it repeatedly. Doesn't save any time, but code is more readable. Would it save significant time to include "<span class=" in class_nl?
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -7,8 +7,9 @@
     <workbookView xWindow="26220" yWindow="860" windowWidth="21600" windowHeight="15260" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="db query vs get" sheetId="2" r:id="rId1"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId2"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId1"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId2"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -448,17 +449,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="B1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>8</v>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
@@ -466,11 +473,11 @@
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
-        <v>0.24570099999999978</v>
+        <v>0.44118779999999946</v>
       </c>
       <c r="D3">
         <f>AVERAGE(D6:D32)</f>
-        <v>0.3320297999999996</v>
+        <v>0.45040099999999939</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -479,11 +486,11 @@
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
-        <v>2.0237555966569346E-2</v>
+        <v>2.1336102659575439E-2</v>
       </c>
       <c r="D4">
         <f>STDEVA(D6:D32)</f>
-        <v>3.7396661477998347E-2</v>
+        <v>3.2935379806523481E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -492,11 +499,11 @@
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
-        <v>8.2366599918475558E-2</v>
+        <v>4.8360590795066105E-2</v>
       </c>
       <c r="D5" s="1">
         <f>D4/D3</f>
-        <v>0.11263043702100954</v>
+        <v>7.3124570785863097E-2</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -504,10 +511,10 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>0.275005</v>
+        <v>0.42475299999999999</v>
       </c>
       <c r="D6">
-        <v>0.32842199999999999</v>
+        <v>0.39991199999999999</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -515,10 +522,10 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>0.23533599999999999</v>
+        <v>0.438661999999999</v>
       </c>
       <c r="D7">
-        <v>0.37503599999999998</v>
+        <v>0.45086799999999899</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -526,10 +533,10 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>0.224244999999999</v>
+        <v>0.446709999999999</v>
       </c>
       <c r="D8">
-        <v>0.27442299999999997</v>
+        <v>0.484957999999999</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -537,10 +544,10 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.23674799999999999</v>
+        <v>0.42122699999999902</v>
       </c>
       <c r="D9">
-        <v>0.35225099999999898</v>
+        <v>0.44270900000000002</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -548,10 +555,10 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0.25717099999999998</v>
+        <v>0.47458699999999998</v>
       </c>
       <c r="D10">
-        <v>0.33001699999999901</v>
+        <v>0.47355799999999898</v>
       </c>
     </row>
   </sheetData>
@@ -567,6 +574,139 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.24570099999999978</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(D6:D32)</f>
+        <v>0.3320297999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.0237555966569346E-2</v>
+      </c>
+      <c r="D4">
+        <f>STDEVA(D6:D32)</f>
+        <v>3.7396661477998347E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>8.2366599918475558E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D4/D3</f>
+        <v>0.11263043702100954</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.275005</v>
+      </c>
+      <c r="D6">
+        <v>0.32842199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.23533599999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.37503599999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.224244999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.27442299999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.23674799999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.35225099999999898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.25717099999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.33001699999999901</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>

</xml_diff>

<commit_message>
Changed .all(params) to .get(:id) wherever possible. pt_element.erb has class_nl = '"ec_<%=@orbital.n.to_s+@orbital.l'
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="26220" yWindow="860" windowWidth="21600" windowHeight="15260" tabRatio="500"/>
+    <workbookView xWindow="25040" yWindow="1220" windowWidth="26680" windowHeight="15780" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId1"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId2"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId3"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId1"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId2"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId3"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -60,6 +61,18 @@
   </si>
   <si>
     <t>@base.get()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>class_nl only</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>span_nl (includes &lt;span&gt; tag)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@terms</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,8 +451,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -450,21 +463,21 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>2</v>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -473,11 +486,11 @@
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
-        <v>0.44118779999999946</v>
-      </c>
-      <c r="D3">
+        <v>0.46217180000000002</v>
+      </c>
+      <c r="D3" t="e">
         <f>AVERAGE(D6:D32)</f>
-        <v>0.45040099999999939</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -486,11 +499,11 @@
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
-        <v>2.1336102659575439E-2</v>
-      </c>
-      <c r="D4">
+        <v>4.5992554111507419E-2</v>
+      </c>
+      <c r="D4" t="e">
         <f>STDEVA(D6:D32)</f>
-        <v>3.2935379806523481E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -499,11 +512,11 @@
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
-        <v>4.8360590795066105E-2</v>
-      </c>
-      <c r="D5" s="1">
+        <v>9.9513977511192633E-2</v>
+      </c>
+      <c r="D5" s="1" t="e">
         <f>D4/D3</f>
-        <v>7.3124570785863097E-2</v>
+        <v>#DIV/0!</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -511,10 +524,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>0.42475299999999999</v>
-      </c>
-      <c r="D6">
-        <v>0.39991199999999999</v>
+        <v>0.48859599999999997</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -522,10 +532,7 @@
         <v>2</v>
       </c>
       <c r="B7">
-        <v>0.438661999999999</v>
-      </c>
-      <c r="D7">
-        <v>0.45086799999999899</v>
+        <v>0.48438100000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -533,10 +540,7 @@
         <v>3</v>
       </c>
       <c r="B8">
-        <v>0.446709999999999</v>
-      </c>
-      <c r="D8">
-        <v>0.484957999999999</v>
+        <v>0.39359699999999997</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -544,10 +548,7 @@
         <v>4</v>
       </c>
       <c r="B9">
-        <v>0.42122699999999902</v>
-      </c>
-      <c r="D9">
-        <v>0.44270900000000002</v>
+        <v>0.50655499999999998</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -555,10 +556,7 @@
         <v>5</v>
       </c>
       <c r="B10">
-        <v>0.47458699999999998</v>
-      </c>
-      <c r="D10">
-        <v>0.47355799999999898</v>
+        <v>0.43773000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -577,6 +575,145 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.44118779999999946</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(D6:D32)</f>
+        <v>0.45040099999999939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.1336102659575439E-2</v>
+      </c>
+      <c r="D4">
+        <f>STDEVA(D6:D32)</f>
+        <v>3.2935379806523481E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>4.8360590795066105E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D4/D3</f>
+        <v>7.3124570785863097E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.42475299999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.39991199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.438661999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.45086799999999899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.446709999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.484957999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.42122699999999902</v>
+      </c>
+      <c r="D9">
+        <v>0.44270900000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.47458699999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.47355799999999898</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B31" sqref="B31"/>
     </sheetView>
@@ -706,7 +843,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>

</xml_diff>

<commit_message>
pt_element_home.erb: tried making this custom, stripped-down version of element.erb to see if would speed up processing & loading of home page. Helped only a little bit, ~100 ms (which is within the standard deviations)...
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,13 +4,15 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25040" yWindow="1220" windowWidth="26680" windowHeight="15780" tabRatio="500"/>
+    <workbookView xWindow="25600" yWindow="6240" windowWidth="20120" windowHeight="12940" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="span_ec" sheetId="5" r:id="rId1"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId2"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId3"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId4"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId1"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId2"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId3"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId4"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId5"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId6"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -73,6 +75,50 @@
   </si>
   <si>
     <t>@terms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pt_element.erb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>custom pt_element_home.erb</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delta</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total Sinatra time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>file size (k)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>times in s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ms</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -116,10 +162,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -127,6 +180,208 @@
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="1"/>
+  <c:lang val="en-US"/>
+  <c:style val="18"/>
+  <c:chart>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'custom pt_element_home total'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>pt_element.erb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="0.068"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'custom pt_element_home total'!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>@terms</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>total Sinatra time</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>onload</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'custom pt_element_home total'!$B$3:$D$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.4537816</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1975714</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.572</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'custom pt_element_home total'!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>custom pt_element_home.erb</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:errBars>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="1"/>
+            <c:val val="0.114"/>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'custom pt_element_home total'!$B$2:$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>@terms</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>total Sinatra time</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>onload</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'custom pt_element_home total'!$F$3:$H$3</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.4372596</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.1572868</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.474</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:axId val="460167944"/>
+        <c:axId val="460171112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="460167944"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="b"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="460171112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="460171112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="460167944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>296333</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>33867</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>634999</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>67734</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -449,10 +704,573 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="11" width="2.85546875" customWidth="1"/>
+    <col min="12" max="12" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.5703125" customWidth="1"/>
+    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F2" s="2" t="str">
+        <f t="array" ref="F2:I2">B2:E2</f>
+        <v>@terms</v>
+      </c>
+      <c r="G2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="H2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="I2" t="str">
+        <v>file size (k)</v>
+      </c>
+      <c r="M2" s="2" t="str">
+        <f t="array" ref="M2:P2">B2:E2</f>
+        <v>@terms</v>
+      </c>
+      <c r="N2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="O2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="P2" t="str">
+        <v>file size (k)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.45378159999999956</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:I3" si="0">AVERAGE(C6:C32)</f>
+        <v>1.1975714</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>2.5720000000000001</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>134.80000000000001</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>0.43725959999999964</v>
+      </c>
+      <c r="G3">
+        <f t="shared" si="0"/>
+        <v>1.1572868000000001</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>2.4740000000000002</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>69.7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>16</v>
+      </c>
+      <c r="M3">
+        <f>B3-F3</f>
+        <v>1.6521999999999926E-2</v>
+      </c>
+      <c r="N3">
+        <f t="shared" ref="N3:P3" si="1">C3-G3</f>
+        <v>4.0284599999999893E-2</v>
+      </c>
+      <c r="O3">
+        <f t="shared" si="1"/>
+        <v>9.7999999999999865E-2</v>
+      </c>
+      <c r="P3">
+        <f t="shared" si="1"/>
+        <v>65.100000000000009</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.0870108895260892E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:H4" si="2">STDEVA(C6:C32)</f>
+        <v>4.3157184561784891E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="2"/>
+        <v>6.8337398253059706E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="2"/>
+        <v>2.5346738297066202E-2</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>3.5277761461013364E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="2"/>
+        <v>0.11458621208504334</v>
+      </c>
+      <c r="L4" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="7">
+        <f>M3*1000</f>
+        <v>16.521999999999927</v>
+      </c>
+      <c r="N4" s="7">
+        <f t="shared" ref="N4:P4" si="3">N3*1000</f>
+        <v>40.284599999999891</v>
+      </c>
+      <c r="O4" s="7">
+        <f t="shared" si="3"/>
+        <v>97.999999999999858</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>4.5991527411558583E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:H5" si="4">C4/C3</f>
+        <v>3.6037253863765363E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="4"/>
+        <v>2.656975048719273E-2</v>
+      </c>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <f t="shared" si="4"/>
+        <v>5.7967253999834933E-2</v>
+      </c>
+      <c r="G5" s="1">
+        <f t="shared" si="4"/>
+        <v>3.0483162394156195E-2</v>
+      </c>
+      <c r="H5" s="1">
+        <f t="shared" si="4"/>
+        <v>4.6316173033566423E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.43260199999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.2069000000000001</v>
+      </c>
+      <c r="D6">
+        <v>2.59</v>
+      </c>
+      <c r="E6">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.44712800000000003</v>
+      </c>
+      <c r="G6">
+        <v>1.1972499999999999</v>
+      </c>
+      <c r="H6">
+        <v>2.67</v>
+      </c>
+      <c r="I6">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.46669099999999902</v>
+      </c>
+      <c r="C7">
+        <v>1.2588010000000001</v>
+      </c>
+      <c r="D7">
+        <v>2.66</v>
+      </c>
+      <c r="F7">
+        <v>0.440271999999999</v>
+      </c>
+      <c r="G7">
+        <v>1.1428370000000001</v>
+      </c>
+      <c r="H7">
+        <v>2.37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.44835399999999997</v>
+      </c>
+      <c r="C8">
+        <v>1.138239</v>
+      </c>
+      <c r="D8">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="F8">
+        <v>0.44775199999999898</v>
+      </c>
+      <c r="G8">
+        <v>1.18065</v>
+      </c>
+      <c r="H8">
+        <v>2.44</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.43822799999999901</v>
+      </c>
+      <c r="C9">
+        <v>1.1958789999999999</v>
+      </c>
+      <c r="D9">
+        <v>2.56</v>
+      </c>
+      <c r="F9">
+        <v>0.39332299999999998</v>
+      </c>
+      <c r="G9">
+        <v>1.1060909999999999</v>
+      </c>
+      <c r="H9">
+        <v>2.4300000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.48303299999999999</v>
+      </c>
+      <c r="C10">
+        <v>1.1880379999999999</v>
+      </c>
+      <c r="D10">
+        <v>2.58</v>
+      </c>
+      <c r="F10">
+        <v>0.45782299999999998</v>
+      </c>
+      <c r="G10">
+        <v>1.1596059999999999</v>
+      </c>
+      <c r="H10">
+        <v>2.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="F1:I1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:J12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="B1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.46217180000000002</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(E6:E32)</f>
+        <v>0.44876379999999949</v>
+      </c>
+      <c r="H3">
+        <f>B3-E3</f>
+        <v>1.3408000000000531E-2</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>4.5992554111507419E-2</v>
+      </c>
+      <c r="E4">
+        <f>STDEVA(E6:E32)</f>
+        <v>2.4783456724196181E-2</v>
+      </c>
+      <c r="H4">
+        <f>H3*1000</f>
+        <v>13.408000000000531</v>
+      </c>
+      <c r="I4">
+        <f>I3*1000</f>
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>9.9513977511192633E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f>E4/E3</f>
+        <v>5.5226060400139693E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.48859599999999997</v>
+      </c>
+      <c r="E6">
+        <v>0.45363399999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.48438100000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.44280399999999898</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.39359699999999997</v>
+      </c>
+      <c r="E8">
+        <v>0.42095300000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.50655499999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.48777599999999899</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.43773000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.43865199999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <mergeCells count="2">
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="B1:C1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -488,9 +1306,9 @@
         <f>AVERAGE(B6:B32)</f>
         <v>0.46217180000000002</v>
       </c>
-      <c r="D3" t="e">
+      <c r="D3">
         <f>AVERAGE(D6:D32)</f>
-        <v>#DIV/0!</v>
+        <v>0.47046542857142815</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -501,9 +1319,9 @@
         <f>STDEVA(B6:B32)</f>
         <v>4.5992554111507419E-2</v>
       </c>
-      <c r="D4" t="e">
+      <c r="D4">
         <f>STDEVA(D6:D32)</f>
-        <v>#DIV/0!</v>
+        <v>4.7567555847296966E-2</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -514,9 +1332,9 @@
         <f>B4/B3</f>
         <v>9.9513977511192633E-2</v>
       </c>
-      <c r="D5" s="1" t="e">
+      <c r="D5" s="1">
         <f>D4/D3</f>
-        <v>#DIV/0!</v>
+        <v>0.10110744160678546</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -526,6 +1344,9 @@
       <c r="B6">
         <v>0.48859599999999997</v>
       </c>
+      <c r="D6">
+        <v>0.45848599999999901</v>
+      </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
@@ -534,6 +1355,9 @@
       <c r="B7">
         <v>0.48438100000000001</v>
       </c>
+      <c r="D7">
+        <v>0.47763599999999901</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
@@ -542,6 +1366,9 @@
       <c r="B8">
         <v>0.39359699999999997</v>
       </c>
+      <c r="D8">
+        <v>0.56508999999999998</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9">
@@ -550,6 +1377,9 @@
       <c r="B9">
         <v>0.50655499999999998</v>
       </c>
+      <c r="D9">
+        <v>0.42804599999999998</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
@@ -558,8 +1388,28 @@
       <c r="B10">
         <v>0.43773000000000001</v>
       </c>
+      <c r="D10">
+        <v>0.41930800000000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>0.473713</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0.47097899999999898</v>
+      </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -571,7 +1421,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -699,6 +1549,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -710,7 +1561,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -832,6 +1683,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -843,7 +1695,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1032,6 +1884,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Trying to optimize time of loading (building and transferring) home page. Found that removing span tags from electron configs reduces file size and time of running pt_element (including apparently non-term time, which seems odd).
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,15 +4,16 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="6240" windowWidth="20120" windowHeight="12940" tabRatio="500"/>
+    <workbookView xWindow="25520" yWindow="-520" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId1"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId2"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId3"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId4"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId5"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId6"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId1"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId2"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId3"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId4"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId5"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId6"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -119,6 +120,22 @@
   </si>
   <si>
     <t>ms</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>non-Sinatra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>term_spans = true</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>in e config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>term_spans = false</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -254,7 +271,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'custom pt_element_home total'!$F$1</c:f>
+              <c:f>'custom pt_element_home total'!$H$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -288,7 +305,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'custom pt_element_home total'!$F$3:$H$3</c:f>
+              <c:f>'custom pt_element_home total'!$H$3:$J$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -359,7 +376,7 @@
       <xdr:rowOff>33867</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>634999</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>67734</xdr:rowOff>
@@ -704,10 +721,535 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:P17"/>
+  <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="20" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f t="array" ref="I2:N2">B2:G2</f>
+        <v>@terms</v>
+      </c>
+      <c r="J2" t="str">
+        <v>in e config</v>
+      </c>
+      <c r="K2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="L2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="M2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="N2" t="str">
+        <v>file size (k)</v>
+      </c>
+      <c r="Q2" s="2" t="str">
+        <f t="array" ref="Q2:V2">B2:G2</f>
+        <v>@terms</v>
+      </c>
+      <c r="R2" t="str">
+        <v>in e config</v>
+      </c>
+      <c r="S2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="T2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="U2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="V2" t="str">
+        <v>file size (k)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.5009969999999998</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(C6:C32)</f>
+        <v>0.95898819999999974</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:M3" si="0">AVERAGE(D6:D32)</f>
+        <v>1.3245984</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>3.0500000000000003</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1.7254016000000001</v>
+      </c>
+      <c r="G3">
+        <v>67.3</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>0.55348319999999984</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>1.1211011999999978</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>1.4813308000000001</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:M3" si="1">AVERAGE(L6:L32)</f>
+        <v>3.468</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
+        <v>1.9866692000000001</v>
+      </c>
+      <c r="N3">
+        <v>106.7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3">
+        <f>B3-I3</f>
+        <v>-5.2486200000000038E-2</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:U3" si="2">C3-J3</f>
+        <v>-0.16211299999999806</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="2"/>
+        <v>-0.1567324000000001</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="2"/>
+        <v>-0.41799999999999971</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="2"/>
+        <v>-0.26126760000000004</v>
+      </c>
+      <c r="V3">
+        <f>G3-N3</f>
+        <v>-39.400000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>5.3914485354123132E-2</v>
+      </c>
+      <c r="C4">
+        <f>STDEVA(C6:C32)</f>
+        <v>7.1833464563531013E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:L4" si="3">STDEVA(D6:D32)</f>
+        <v>9.4934143127222176E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>0.29824486584013271</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>0.22816090053140187</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>9.7315476406376278E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.19036480990902901</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>0.24516197712777557</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:M4" si="4">STDEVA(L6:L32)</f>
+        <v>0.43677225186589419</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>0.33879452626806195</v>
+      </c>
+      <c r="P4" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q4" s="7">
+        <f>Q3*1000</f>
+        <v>-52.486200000000039</v>
+      </c>
+      <c r="R4" s="7">
+        <f t="shared" ref="R4:U4" si="5">R3*1000</f>
+        <v>-162.11299999999807</v>
+      </c>
+      <c r="S4" s="7">
+        <f t="shared" si="5"/>
+        <v>-156.7324000000001</v>
+      </c>
+      <c r="T4" s="7">
+        <f t="shared" si="5"/>
+        <v>-417.99999999999972</v>
+      </c>
+      <c r="U4" s="7">
+        <f t="shared" si="5"/>
+        <v>-261.26760000000002</v>
+      </c>
+      <c r="V4" s="7"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>0.10761438761933335</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C4/C3</f>
+        <v>7.4905472834317491E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:M5" si="6">D4/D3</f>
+        <v>7.1670132718884588E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="6"/>
+        <v>9.7785201914797601E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.13223640254616773</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.17582372221302525</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.16980162888865821</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.16550116768501374</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" ref="L5" si="7">L4/L3</f>
+        <v>0.12594355590135356</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" ref="M5" si="8">M4/M3</f>
+        <v>0.17053394005809419</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.51501599999999903</v>
+      </c>
+      <c r="C6">
+        <v>0.92809899999999901</v>
+      </c>
+      <c r="D6">
+        <v>1.246054</v>
+      </c>
+      <c r="E6">
+        <v>2.9</v>
+      </c>
+      <c r="F6">
+        <f>E6-D6</f>
+        <v>1.6539459999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.69593300000000002</v>
+      </c>
+      <c r="J6">
+        <v>1.4183220000000001</v>
+      </c>
+      <c r="K6">
+        <v>1.857729</v>
+      </c>
+      <c r="L6">
+        <v>3.6</v>
+      </c>
+      <c r="M6">
+        <f>L6-K6</f>
+        <v>1.7422710000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.47409800000000002</v>
+      </c>
+      <c r="C7">
+        <v>0.96557700000000002</v>
+      </c>
+      <c r="D7">
+        <v>1.289107</v>
+      </c>
+      <c r="E7">
+        <v>3.1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F10" si="9">E7-D7</f>
+        <v>1.8108930000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.50989899999999999</v>
+      </c>
+      <c r="J7">
+        <v>1.0646149999999901</v>
+      </c>
+      <c r="K7">
+        <v>1.3850290000000001</v>
+      </c>
+      <c r="L7">
+        <v>3.26</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M10" si="10">L7-K7</f>
+        <v>1.8749709999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.45488800000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.88311899999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.25692</v>
+      </c>
+      <c r="E8">
+        <v>2.87</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="9"/>
+        <v>1.6130800000000001</v>
+      </c>
+      <c r="I8">
+        <v>0.60211199999999898</v>
+      </c>
+      <c r="J8">
+        <v>1.1913959999999999</v>
+      </c>
+      <c r="K8">
+        <v>1.59188</v>
+      </c>
+      <c r="L8">
+        <v>4.16</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="10"/>
+        <v>2.5681200000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.58897699999999997</v>
+      </c>
+      <c r="C9">
+        <v>1.0756669999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.476818</v>
+      </c>
+      <c r="E9">
+        <v>3.55</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="9"/>
+        <v>2.0731820000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.44475300000000001</v>
+      </c>
+      <c r="J9">
+        <v>0.95806499999999895</v>
+      </c>
+      <c r="K9">
+        <v>1.3077430000000001</v>
+      </c>
+      <c r="L9">
+        <v>3.29</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="10"/>
+        <v>1.9822569999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.47200599999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.94247899999999996</v>
+      </c>
+      <c r="D10">
+        <v>1.354093</v>
+      </c>
+      <c r="E10">
+        <v>2.83</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="9"/>
+        <v>1.4759070000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.51471900000000004</v>
+      </c>
+      <c r="J10">
+        <v>0.97310799999999997</v>
+      </c>
+      <c r="K10">
+        <v>1.264273</v>
+      </c>
+      <c r="L10">
+        <v>3.03</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="10"/>
+        <v>1.7657269999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="5"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="5"/>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="P1:T1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -716,17 +1258,19 @@
     <col min="3" max="3" width="13.28515625" customWidth="1"/>
     <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="5.85546875" customWidth="1"/>
-    <col min="11" max="11" width="2.85546875" customWidth="1"/>
-    <col min="12" max="12" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.5703125" customWidth="1"/>
-    <col min="14" max="14" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="9" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:18">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -735,24 +1279,26 @@
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="6" t="s">
+      <c r="E1" s="6"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="6"/>
-      <c r="H1" s="6"/>
       <c r="I1" s="6"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="6" t="s">
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="6"/>
-      <c r="N1" s="6"/>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
-    </row>
-    <row r="2" spans="1:16">
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+    </row>
+    <row r="2" spans="1:18">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -766,36 +1312,39 @@
         <v>20</v>
       </c>
       <c r="E2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" s="2" t="str">
-        <f t="array" ref="F2:I2">B2:E2</f>
+      <c r="H2" s="2" t="str">
+        <f t="array" ref="H2:K2">B2:F2</f>
         <v>@terms</v>
       </c>
-      <c r="G2" t="str">
+      <c r="I2" t="str">
         <v>total Sinatra time</v>
       </c>
-      <c r="H2" t="str">
+      <c r="J2" t="str">
         <v>onload</v>
       </c>
-      <c r="I2" t="str">
-        <v>file size (k)</v>
-      </c>
-      <c r="M2" s="2" t="str">
-        <f t="array" ref="M2:P2">B2:E2</f>
+      <c r="K2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="O2" s="2" t="str">
+        <f t="array" ref="O2:R2">B2:F2</f>
         <v>@terms</v>
       </c>
-      <c r="N2" t="str">
+      <c r="P2" t="str">
         <v>total Sinatra time</v>
       </c>
-      <c r="O2" t="str">
+      <c r="Q2" t="str">
         <v>onload</v>
       </c>
-      <c r="P2" t="str">
-        <v>file size (k)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="R2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -804,7 +1353,7 @@
         <v>0.45378159999999956</v>
       </c>
       <c r="C3">
-        <f t="shared" ref="C3:I3" si="0">AVERAGE(C6:C32)</f>
+        <f t="shared" ref="C3:L3" si="0">AVERAGE(C6:C32)</f>
         <v>1.1975714</v>
       </c>
       <c r="D3">
@@ -812,46 +1361,54 @@
         <v>2.5720000000000001</v>
       </c>
       <c r="E3">
+        <f t="shared" ref="E3" si="1">AVERAGE(E6:E32)</f>
+        <v>1.3744286000000001</v>
+      </c>
+      <c r="F3">
         <f t="shared" si="0"/>
         <v>134.80000000000001</v>
       </c>
-      <c r="F3">
+      <c r="H3">
         <f t="shared" si="0"/>
         <v>0.43725959999999964</v>
       </c>
-      <c r="G3">
+      <c r="I3">
         <f t="shared" si="0"/>
         <v>1.1572868000000001</v>
       </c>
-      <c r="H3">
+      <c r="J3">
         <f t="shared" si="0"/>
         <v>2.4740000000000002</v>
       </c>
-      <c r="I3">
+      <c r="K3">
+        <f t="shared" ref="K3" si="2">AVERAGE(K6:K32)</f>
+        <v>1.3167132000000001</v>
+      </c>
+      <c r="L3">
         <f t="shared" si="0"/>
         <v>69.7</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>16</v>
       </c>
-      <c r="M3">
-        <f>B3-F3</f>
+      <c r="O3">
+        <f>B3-H3</f>
         <v>1.6521999999999926E-2</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:P3" si="1">C3-G3</f>
+      <c r="P3">
+        <f>C3-I3</f>
         <v>4.0284599999999893E-2</v>
       </c>
-      <c r="O3">
-        <f t="shared" si="1"/>
+      <c r="Q3">
+        <f>D3-J3</f>
         <v>9.7999999999999865E-2</v>
       </c>
-      <c r="P3">
-        <f t="shared" si="1"/>
-        <v>65.100000000000009</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="R3">
+        <f>E3-K3</f>
+        <v>5.7715399999999972E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -860,42 +1417,54 @@
         <v>2.0870108895260892E-2</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:H4" si="2">STDEVA(C6:C32)</f>
+        <f t="shared" ref="C4:J4" si="3">STDEVA(C6:C32)</f>
         <v>4.3157184561784891E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.8337398253059706E-2</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="2"/>
+      <c r="E4">
+        <f t="shared" ref="E4" si="4">STDEVA(E6:E32)</f>
+        <v>2.7504719218717954E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
         <v>2.5346738297066202E-2</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="2"/>
+      <c r="I4">
+        <f t="shared" si="3"/>
         <v>3.5277761461013364E-2</v>
       </c>
-      <c r="H4">
-        <f t="shared" si="2"/>
+      <c r="J4">
+        <f t="shared" si="3"/>
         <v>0.11458621208504334</v>
       </c>
-      <c r="L4" t="s">
+      <c r="K4">
+        <f t="shared" ref="K4" si="5">STDEVA(K6:K32)</f>
+        <v>9.4835850044695941E-2</v>
+      </c>
+      <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="M4" s="7">
-        <f>M3*1000</f>
+      <c r="O4" s="7">
+        <f>O3*1000</f>
         <v>16.521999999999927</v>
       </c>
-      <c r="N4" s="7">
-        <f t="shared" ref="N4:P4" si="3">N3*1000</f>
+      <c r="P4" s="7">
+        <f t="shared" ref="P4:R4" si="6">P3*1000</f>
         <v>40.284599999999891</v>
       </c>
-      <c r="O4" s="7">
-        <f t="shared" si="3"/>
+      <c r="Q4" s="7">
+        <f t="shared" si="6"/>
         <v>97.999999999999858</v>
       </c>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="R4" s="7">
+        <f t="shared" si="6"/>
+        <v>57.715399999999974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -904,28 +1473,37 @@
         <v>4.5991527411558583E-2</v>
       </c>
       <c r="C5" s="1">
-        <f t="shared" ref="C5:H5" si="4">C4/C3</f>
+        <f t="shared" ref="C5:K5" si="7">C4/C3</f>
         <v>3.6037253863765363E-2</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>2.656975048719273E-2</v>
       </c>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1">
-        <f t="shared" si="4"/>
+      <c r="E5" s="1">
+        <f t="shared" si="7"/>
+        <v>2.0011748313966946E-2</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <f t="shared" si="7"/>
         <v>5.7967253999834933E-2</v>
       </c>
-      <c r="G5" s="1">
-        <f t="shared" si="4"/>
+      <c r="I5" s="1">
+        <f t="shared" si="7"/>
         <v>3.0483162394156195E-2</v>
       </c>
-      <c r="H5" s="1">
-        <f t="shared" si="4"/>
+      <c r="J5" s="1">
+        <f t="shared" si="7"/>
         <v>4.6316173033566423E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="K5" s="1">
+        <f t="shared" si="7"/>
+        <v>7.2024682402132778E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
       <c r="A6">
         <v>1</v>
       </c>
@@ -939,22 +1517,30 @@
         <v>2.59</v>
       </c>
       <c r="E6">
+        <f>D6-C6</f>
+        <v>1.3830999999999998</v>
+      </c>
+      <c r="F6">
         <v>134.80000000000001</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.44712800000000003</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>1.1972499999999999</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>2.67</v>
       </c>
-      <c r="I6">
+      <c r="K6">
+        <f>J6-I6</f>
+        <v>1.47275</v>
+      </c>
+      <c r="L6">
         <v>69.7</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:18">
       <c r="A7">
         <v>2</v>
       </c>
@@ -967,17 +1553,25 @@
       <c r="D7">
         <v>2.66</v>
       </c>
-      <c r="F7">
+      <c r="E7">
+        <f t="shared" ref="E7:E10" si="8">D7-C7</f>
+        <v>1.4011990000000001</v>
+      </c>
+      <c r="H7">
         <v>0.440271999999999</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>1.1428370000000001</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>2.37</v>
       </c>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="K7">
+        <f t="shared" ref="K7:K10" si="9">J7-I7</f>
+        <v>1.227163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
       <c r="A8">
         <v>3</v>
       </c>
@@ -990,17 +1584,25 @@
       <c r="D8">
         <v>2.4700000000000002</v>
       </c>
-      <c r="F8">
+      <c r="E8">
+        <f t="shared" si="8"/>
+        <v>1.3317610000000002</v>
+      </c>
+      <c r="H8">
         <v>0.44775199999999898</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>1.18065</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>2.44</v>
       </c>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="K8">
+        <f t="shared" si="9"/>
+        <v>1.25935</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1013,17 +1615,25 @@
       <c r="D9">
         <v>2.56</v>
       </c>
-      <c r="F9">
+      <c r="E9">
+        <f t="shared" si="8"/>
+        <v>1.3641210000000001</v>
+      </c>
+      <c r="H9">
         <v>0.39332299999999998</v>
       </c>
-      <c r="G9">
+      <c r="I9">
         <v>1.1060909999999999</v>
       </c>
-      <c r="H9">
+      <c r="J9">
         <v>2.4300000000000002</v>
       </c>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="K9">
+        <f t="shared" si="9"/>
+        <v>1.3239090000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1036,27 +1646,36 @@
       <c r="D10">
         <v>2.58</v>
       </c>
-      <c r="F10">
+      <c r="E10">
+        <f t="shared" si="8"/>
+        <v>1.3919620000000001</v>
+      </c>
+      <c r="H10">
         <v>0.45782299999999998</v>
       </c>
-      <c r="G10">
+      <c r="I10">
         <v>1.1596059999999999</v>
       </c>
-      <c r="H10">
+      <c r="J10">
         <v>2.46</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="K10">
+        <f t="shared" si="9"/>
+        <v>1.300394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
       <c r="A16" s="5"/>
     </row>
     <row r="17" spans="1:1">
       <c r="A17" s="5"/>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:K1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1070,7 +1689,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -1249,7 +1868,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
@@ -1265,7 +1883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1409,7 +2027,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1421,7 +2038,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1549,7 +2166,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1561,7 +2177,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1683,7 +2299,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -1695,7 +2310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1884,7 +2499,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>

<commit_message>
Using @orbital_hash (loading table of orbitals [e.g., 11 = 5s] into memory rather than querying database table each time in pt_element.erb) cuts processing (e config) time considerably.
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -7,13 +7,14 @@
     <workbookView xWindow="25520" yWindow="-520" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="term_spans" sheetId="8" r:id="rId1"/>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId2"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId3"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId4"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId5"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId6"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId7"/>
+    <sheet name="@orbital_hash" sheetId="9" r:id="rId1"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId2"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId3"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId4"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId5"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId6"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId7"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId8"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -136,6 +137,30 @@
   </si>
   <si>
     <t>term_spans = false</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>orbitals</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>database query</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@orbital_hash (in memory)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>e config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>onload</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>non-Sinatra</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -179,17 +204,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -322,24 +350,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="460167944"/>
-        <c:axId val="460171112"/>
+        <c:axId val="515131336"/>
+        <c:axId val="515134856"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="460167944"/>
+        <c:axId val="515131336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="460171112"/>
+        <c:crossAx val="515134856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="460171112"/>
+        <c:axId val="515134856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -347,14 +375,13 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="460167944"/>
+        <c:crossAx val="515131336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -724,10 +751,480 @@
   <dimension ref="A1:V17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="K6" activePane="bottomRight" state="frozenSplit"/>
+      <pane xSplit="1" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="U4" sqref="U4"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="20" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f t="array" ref="I2:N2">B2:G2</f>
+        <v>orbitals</v>
+      </c>
+      <c r="J2" t="str">
+        <v>e config</v>
+      </c>
+      <c r="K2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="L2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="M2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="2" t="str">
+        <f t="array" ref="Q2:V2">B2:G2</f>
+        <v>orbitals</v>
+      </c>
+      <c r="R2" t="str">
+        <v>e config</v>
+      </c>
+      <c r="S2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="T2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="U2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.33251599999999915</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:E3" si="0">AVERAGE(C6:C32)</f>
+        <v>1.1246306000000001</v>
+      </c>
+      <c r="D3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E3" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3" si="1">AVERAGE(F6:F32)</f>
+        <v>0</v>
+      </c>
+      <c r="I3" t="e">
+        <f t="shared" ref="D3:M3" si="2">AVERAGE(I6:I32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J3">
+        <f t="shared" ref="J3:M3" si="3">AVERAGE(J6:J32)</f>
+        <v>0.22558519999999943</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="3"/>
+        <v>0.67792579999999991</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="3"/>
+        <v>2.028</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="3"/>
+        <v>1.3500742000000001</v>
+      </c>
+      <c r="P3" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q3" t="e">
+        <f>B3-I3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:U3" si="4">C3-J3</f>
+        <v>0.89904540000000077</v>
+      </c>
+      <c r="S3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T3" t="e">
+        <f t="shared" si="4"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="4"/>
+        <v>-1.3500742000000001</v>
+      </c>
+      <c r="V3">
+        <f>G3-N3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>6.3322111414576526E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:E4" si="5">STDEVA(C6:C32)</f>
+        <v>0.13060297172844007</v>
+      </c>
+      <c r="D4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E4" t="e">
+        <f t="shared" si="5"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F4">
+        <f t="shared" ref="F4" si="6">STDEVA(F6:F32)</f>
+        <v>0</v>
+      </c>
+      <c r="I4" t="e">
+        <f t="shared" ref="D4:M4" si="7">STDEVA(I6:I32)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J4">
+        <f t="shared" ref="J4:M4" si="8">STDEVA(J6:J32)</f>
+        <v>2.4286952519819566E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="8"/>
+        <v>4.520142942651436E-2</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="8"/>
+        <v>0.17064583206160919</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="8"/>
+        <v>0.13967913309510532</v>
+      </c>
+      <c r="P4" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="5" t="e">
+        <f>Q3*1000</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:U4" si="9">R3*1000</f>
+        <v>899.04540000000077</v>
+      </c>
+      <c r="S4" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="T4" s="5" t="e">
+        <f t="shared" si="9"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="U4" s="5">
+        <f t="shared" si="9"/>
+        <v>-1350.0742</v>
+      </c>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>0.19043327663804654</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:F5" si="10">C4/C3</f>
+        <v>0.11612966224504299</v>
+      </c>
+      <c r="D5" s="1" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="E5" s="1" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="F5" s="1" t="e">
+        <f t="shared" si="10"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1" t="e">
+        <f t="shared" ref="D5:M5" si="11">I4/I3</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" ref="J5:M5" si="12">J4/J3</f>
+        <v>0.10766199431443033</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="12"/>
+        <v>6.6676071963206546E-2</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" si="12"/>
+        <v>8.4144887604343785E-2</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" si="12"/>
+        <v>0.10346033802816565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.26496499999999901</v>
+      </c>
+      <c r="C6">
+        <v>1.025873</v>
+      </c>
+      <c r="F6">
+        <f>E6-D6</f>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0.23085899999999901</v>
+      </c>
+      <c r="K6">
+        <v>0.65015699999999998</v>
+      </c>
+      <c r="L6">
+        <v>1.99</v>
+      </c>
+      <c r="M6">
+        <f>L6-K6</f>
+        <v>1.3398430000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.409718999999999</v>
+      </c>
+      <c r="C7">
+        <v>1.1971369999999999</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F10" si="13">E7-D7</f>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0.186167</v>
+      </c>
+      <c r="K7">
+        <v>0.632552</v>
+      </c>
+      <c r="L7">
+        <v>1.93</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M10" si="14">L7-K7</f>
+        <v>1.2974479999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.38972899999999899</v>
+      </c>
+      <c r="C8">
+        <v>1.320954</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0.220945999999999</v>
+      </c>
+      <c r="K8">
+        <v>0.65561400000000003</v>
+      </c>
+      <c r="L8">
+        <v>1.93</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="14"/>
+        <v>1.2743859999999998</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.30088999999999999</v>
+      </c>
+      <c r="C9">
+        <v>1.0499179999999999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0.24352599999999999</v>
+      </c>
+      <c r="K9">
+        <v>0.71362800000000004</v>
+      </c>
+      <c r="L9">
+        <v>1.96</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="14"/>
+        <v>1.246372</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.29727699999999901</v>
+      </c>
+      <c r="C10">
+        <v>1.029271</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0.24642799999999901</v>
+      </c>
+      <c r="K10">
+        <v>0.73767799999999994</v>
+      </c>
+      <c r="L10">
+        <v>2.33</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="14"/>
+        <v>1.5923220000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="P1:T1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:V17"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -761,17 +1258,17 @@
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="4"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="3"/>
       <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
       <c r="L1" s="6"/>
-      <c r="M1" s="4"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="4"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
       <c r="P1" s="6" t="s">
         <v>15</v>
       </c>
@@ -854,7 +1351,7 @@
         <v>0.95898819999999974</v>
       </c>
       <c r="D3">
-        <f t="shared" ref="D3:M3" si="0">AVERAGE(D6:D32)</f>
+        <f t="shared" ref="D3:K3" si="0">AVERAGE(D6:D32)</f>
         <v>1.3245984</v>
       </c>
       <c r="E3">
@@ -932,7 +1429,7 @@
         <v>7.1833464563531013E-2</v>
       </c>
       <c r="D4">
-        <f t="shared" ref="D4:L4" si="3">STDEVA(D6:D32)</f>
+        <f t="shared" ref="D4:K4" si="3">STDEVA(D6:D32)</f>
         <v>9.4934143127222176E-2</v>
       </c>
       <c r="E4">
@@ -966,27 +1463,27 @@
       <c r="P4" t="s">
         <v>23</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="5">
         <f>Q3*1000</f>
         <v>-52.486200000000039</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="5">
         <f t="shared" ref="R4:U4" si="5">R3*1000</f>
         <v>-162.11299999999807</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="5">
         <f t="shared" si="5"/>
         <v>-156.7324000000001</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="5">
         <f t="shared" si="5"/>
         <v>-417.99999999999972</v>
       </c>
-      <c r="U4" s="7">
+      <c r="U4" s="5">
         <f t="shared" si="5"/>
         <v>-261.26760000000002</v>
       </c>
-      <c r="V4" s="7"/>
+      <c r="V4" s="5"/>
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
@@ -1001,7 +1498,7 @@
         <v>7.4905472834317491E-2</v>
       </c>
       <c r="D5" s="1">
-        <f t="shared" ref="D5:M5" si="6">D4/D3</f>
+        <f t="shared" ref="D5:K5" si="6">D4/D3</f>
         <v>7.1670132718884588E-2</v>
       </c>
       <c r="E5" s="1">
@@ -1221,10 +1718,10 @@
       </c>
     </row>
     <row r="16" spans="1:22">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
@@ -1244,7 +1741,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R17"/>
   <sheetViews>
@@ -1280,16 +1777,16 @@
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="6" t="s">
         <v>14</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="4"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
       <c r="N1" s="6" t="s">
         <v>15</v>
       </c>
@@ -1447,19 +1944,19 @@
       <c r="N4" t="s">
         <v>23</v>
       </c>
-      <c r="O4" s="7">
+      <c r="O4" s="5">
         <f>O3*1000</f>
         <v>16.521999999999927</v>
       </c>
-      <c r="P4" s="7">
+      <c r="P4" s="5">
         <f t="shared" ref="P4:R4" si="6">P3*1000</f>
         <v>40.284599999999891</v>
       </c>
-      <c r="Q4" s="7">
+      <c r="Q4" s="5">
         <f t="shared" si="6"/>
         <v>97.999999999999858</v>
       </c>
-      <c r="R4" s="7">
+      <c r="R4" s="5">
         <f t="shared" si="6"/>
         <v>57.715399999999974</v>
       </c>
@@ -1665,10 +2162,10 @@
       </c>
     </row>
     <row r="16" spans="1:18">
-      <c r="A16" s="5"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" spans="1:1">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
     </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
@@ -1679,7 +2176,6 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <drawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
@@ -1689,7 +2185,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -1708,16 +2204,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="3" t="s">
+      <c r="C1" s="7"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="3"/>
       <c r="H1" t="s">
         <v>15</v>
       </c>
@@ -1868,13 +2364,13 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1883,7 +2379,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2027,9 +2523,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2038,7 +2534,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2166,9 +2662,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2177,7 +2673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2299,9 +2795,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -2310,7 +2806,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2499,9 +2995,9 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Set up @timing framework to track each step. Determined that second call on a page to element.property_name is very slow; not sure why.
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="-520" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="25560" yWindow="820" windowWidth="25600" windowHeight="14520" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="@orbital_hash" sheetId="9" r:id="rId1"/>
-    <sheet name="term_spans" sheetId="8" r:id="rId2"/>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId3"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId4"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId5"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId6"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId7"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId8"/>
+    <sheet name="@timing framework" sheetId="10" r:id="rId1"/>
+    <sheet name="@orbital_hash" sheetId="9" r:id="rId2"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId3"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId4"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId5"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId6"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId7"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId8"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId9"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,6 +162,18 @@
   </si>
   <si>
     <t>non-Sinatra</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@timing[pt_econfig]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>@time_in_e_config</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Delta</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -382,6 +395,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
+      <c:layout/>
     </c:legend>
     <c:plotVisOnly val="1"/>
   </c:chart>
@@ -748,13 +762,193 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2">
+        <f>AVERAGE(D5:D31)</f>
+        <v>2.249571428571997E-3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3">
+        <f>STDEVA(D5:D31)</f>
+        <v>2.2947247993547286E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="1">
+        <f t="shared" ref="D4" si="0">D3/D2</f>
+        <v>0.10200719880281349</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>0.206763</v>
+      </c>
+      <c r="C5">
+        <v>0.20448</v>
+      </c>
+      <c r="D5">
+        <f>B5-C5</f>
+        <v>2.2830000000000072E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6">
+        <v>0.21421599999999899</v>
+      </c>
+      <c r="C6">
+        <v>0.193188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0.18376999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.18155399999999899</v>
+      </c>
+      <c r="D7">
+        <f t="shared" ref="D6:D12" si="1">B7-C7</f>
+        <v>2.216000000000995E-3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8">
+        <v>0.19337399999999999</v>
+      </c>
+      <c r="C8">
+        <v>0.190662999999999</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>2.7110000000009904E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9">
+        <v>0.19017000000000001</v>
+      </c>
+      <c r="C9">
+        <v>0.18808</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>2.0900000000000085E-3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>0.189051</v>
+      </c>
+      <c r="C10">
+        <v>0.18693899999999899</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>2.112000000001002E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.17564399999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.17332999999999901</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.3140000000009819E-3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>0.17163300000000001</v>
+      </c>
+      <c r="C12">
+        <v>0.16961200000000001</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2.020999999999995E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="D6" activePane="bottomRight" state="frozenSplit"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomRight" activeCell="D3" sqref="D3:D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -1216,7 +1410,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -1724,7 +1918,6 @@
       <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:L1"/>
@@ -1741,12 +1934,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R17"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -2168,7 +2361,6 @@
       <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="N1:R1"/>
     <mergeCell ref="B1:F1"/>
@@ -2185,7 +2377,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -2364,7 +2556,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
@@ -2379,7 +2570,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2523,7 +2714,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2534,7 +2724,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2662,7 +2852,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2673,7 +2862,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2795,7 +2984,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2806,7 +2994,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2995,7 +3183,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
home.erb: output @timing in two loops, first for labels, second for times--so can copy into Excel en masse easily
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25560" yWindow="820" windowWidth="25600" windowHeight="14520" tabRatio="843"/>
+    <workbookView xWindow="25520" yWindow="-520" windowWidth="25160" windowHeight="8380" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="@timing framework" sheetId="10" r:id="rId1"/>
-    <sheet name="@orbital_hash" sheetId="9" r:id="rId2"/>
-    <sheet name="term_spans" sheetId="8" r:id="rId3"/>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId4"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId5"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId6"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId7"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId8"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId9"/>
+    <sheet name="Sheet3" sheetId="11" r:id="rId1"/>
+    <sheet name="@timing framework" sheetId="10" r:id="rId2"/>
+    <sheet name="@orbital_hash" sheetId="9" r:id="rId3"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId4"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId5"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId6"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId7"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId8"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId9"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId10"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -27,12 +28,59 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+  <si>
+    <t>pt_econfig_this_orbital</t>
+  </si>
+  <si>
+    <t>pt_econfig_orbital_hash_n</t>
+  </si>
+  <si>
+    <t>pt_econfig_orbital_hash_l</t>
+  </si>
+  <si>
+    <t>pt_econfig_rest</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>Step</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>Run</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>for loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.each loop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>StDev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RelStdDev</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Avg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>Total time</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -175,17 +223,45 @@
   <si>
     <t>Delta</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pt_init</t>
+  </si>
+  <si>
+    <t>pt_atomic_num</t>
+  </si>
+  <si>
+    <t>pt_symbol</t>
+  </si>
+  <si>
+    <t>pt_name</t>
+  </si>
+  <si>
+    <t>pt_econfig_Orb.all</t>
+  </si>
+  <si>
+    <t>pt_econfig_pre_terms</t>
+  </si>
+  <si>
+    <t>pt_econfig_last_orb</t>
+  </si>
+  <si>
+    <t>pt_econfig_for</t>
+  </si>
+  <si>
+    <t>pt_econfig_if_term_spans</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="2">
     <font>
@@ -217,7 +293,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -231,6 +307,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -762,10 +845,699 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R16" sqref="R16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="11" width="7.7109375" customWidth="1"/>
+    <col min="14" max="14" width="10.7109375" style="11"/>
+    <col min="17" max="17" width="10.7109375" style="11"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="10" t="str">
+        <f>B1</f>
+        <v>for loop</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10" t="str">
+        <f>G1</f>
+        <v>.each loop</v>
+      </c>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f t="array" ref="G2:K2">B2:F2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="array" ref="O2:Q2">L2:N2</f>
+        <v>Avg</v>
+      </c>
+      <c r="P2" t="str">
+        <v>StDev</v>
+      </c>
+      <c r="Q2" s="11" t="str">
+        <v>RelStdDev</v>
+      </c>
+      <c r="R2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B3">
+        <v>5.3610000000000003E-3</v>
+      </c>
+      <c r="C3">
+        <v>5.731E-3</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(B3:F3)</f>
+        <v>5.5460000000000006E-3</v>
+      </c>
+      <c r="M3">
+        <f>STDEVA(B3:F3)</f>
+        <v>2.6162950903903102E-4</v>
+      </c>
+      <c r="N3" s="11">
+        <f>M3/L3</f>
+        <v>4.7174451683921925E-2</v>
+      </c>
+      <c r="R3">
+        <f t="array" ref="R3:R16">O3:O16-L3:L16</f>
+        <v>-5.5460000000000006E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4">
+        <v>3.5630000000000002E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.7069999999999998E-3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L16" si="0">AVERAGE(B4:F4)</f>
+        <v>3.6350000000000002E-3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M16" si="1">STDEVA(B4:F4)</f>
+        <v>1.0182337649085403E-4</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" ref="N4:N16" si="2">M4/L4</f>
+        <v>2.8011933009863554E-2</v>
+      </c>
+      <c r="R4">
+        <v>-3.6350000000000002E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5">
+        <v>0.27063799999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.28170800000000001</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.276173</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>7.8276720677375299E-3</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="2"/>
+        <v>2.8343364730576595E-2</v>
+      </c>
+      <c r="R5">
+        <v>-0.276173</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6">
+        <v>4.0070000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>4.5849999999999997E-3</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>4.2959999999999995E-3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>4.0870771952583503E-4</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="2"/>
+        <v>9.5136806221097547E-2</v>
+      </c>
+      <c r="R6">
+        <v>-4.2959999999999995E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>54</v>
+      </c>
+      <c r="B7">
+        <v>4.6899000000000003E-2</v>
+      </c>
+      <c r="C7">
+        <v>5.1619999999999999E-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>4.9259499999999998E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>3.3382511139819393E-3</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="2"/>
+        <v>6.7768676376778886E-2</v>
+      </c>
+      <c r="R7">
+        <v>-4.9259499999999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8">
+        <v>2.0709999999999999E-3</v>
+      </c>
+      <c r="C8">
+        <v>2.421E-3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2.2459999999999997E-3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>2.4748737341529604E-4</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="2"/>
+        <v>0.11019028201927697</v>
+      </c>
+      <c r="R8">
+        <v>-2.2459999999999997E-3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9">
+        <v>0.124172</v>
+      </c>
+      <c r="C9">
+        <v>0.15309</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.138631</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>2.0448113898352698E-2</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="2"/>
+        <v>0.1475002986226219</v>
+      </c>
+      <c r="R9">
+        <v>-0.138631</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10">
+        <v>3.503E-3</v>
+      </c>
+      <c r="C10">
+        <v>3.4680000000000002E-3</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>3.4854999999999999E-3</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>2.4748737341573409E-5</v>
+      </c>
+      <c r="N10" s="11">
+        <f t="shared" si="2"/>
+        <v>7.1004841031626484E-3</v>
+      </c>
+      <c r="R10">
+        <v>-3.4854999999999999E-3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11">
+        <v>1.0169999999999999E-3</v>
+      </c>
+      <c r="C11">
+        <v>9.0200000000000002E-4</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>9.5949999999999996E-4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>8.1317279836452277E-5</v>
+      </c>
+      <c r="N11" s="11">
+        <f t="shared" si="2"/>
+        <v>8.4749640267276993E-2</v>
+      </c>
+      <c r="R11">
+        <v>-9.5949999999999996E-4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="C12">
+        <v>4.8469999999999997E-3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>4.6235E-3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>3.1607673119038324E-4</v>
+      </c>
+      <c r="N12" s="11">
+        <f t="shared" si="2"/>
+        <v>6.8363086663865744E-2</v>
+      </c>
+      <c r="R12">
+        <v>-4.6235E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2.532E-3</v>
+      </c>
+      <c r="C13">
+        <v>2.539E-3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>2.5355E-3</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>4.9497474683420624E-6</v>
+      </c>
+      <c r="N13" s="11">
+        <f t="shared" si="2"/>
+        <v>1.9521780589004387E-3</v>
+      </c>
+      <c r="R13">
+        <v>-2.5355E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>1.658E-3</v>
+      </c>
+      <c r="C14">
+        <v>1.8810000000000001E-3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1.7695E-3</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>1.5768481220459723E-4</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="2"/>
+        <v>8.9112637583835669E-2</v>
+      </c>
+      <c r="R14">
+        <v>-1.7695E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1.8220000000000001E-3</v>
+      </c>
+      <c r="C15">
+        <v>1.8710000000000001E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1.8465000000000001E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>3.4648232278137748E-5</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="2"/>
+        <v>1.8764274182582044E-2</v>
+      </c>
+      <c r="R15">
+        <v>-1.8465000000000001E-3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0.60263599999999995</v>
+      </c>
+      <c r="C16">
+        <v>0.65221099999999999</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.62742349999999991</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>3.505481867732517E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="2"/>
+        <v>5.5871064245003856E-2</v>
+      </c>
+      <c r="R16">
+        <v>-0.62742349999999991</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.28515625" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>1.5002987999999939</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(C6:C32)</f>
+        <v>1.5571221999999998</v>
+      </c>
+      <c r="E3">
+        <f>AVERAGE(E6:E32)</f>
+        <v>1.571066199999994</v>
+      </c>
+      <c r="F3">
+        <f>AVERAGE(F6:F32)</f>
+        <v>1.6217526</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>5.0955876149856638E-2</v>
+      </c>
+      <c r="C4">
+        <f>STDEVA(C6:C32)</f>
+        <v>5.4136191191293544E-2</v>
+      </c>
+      <c r="E4">
+        <f>STDEVA(E6:E32)</f>
+        <v>6.8393520144085576E-2</v>
+      </c>
+      <c r="F4">
+        <f>STDEVA(F6:F32)</f>
+        <v>6.2694297067597771E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>3.3963818507257916E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C4/C3</f>
+        <v>3.4766822534091128E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f>E4/E3</f>
+        <v>4.3533187935738057E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f>F4/F3</f>
+        <v>3.8658360755887036E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>1.46162699999999</v>
+      </c>
+      <c r="C6">
+        <v>1.5232589999999999</v>
+      </c>
+      <c r="E6">
+        <v>1.5305409999999899</v>
+      </c>
+      <c r="F6">
+        <v>1.5778160000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>1.47313899999999</v>
+      </c>
+      <c r="C7">
+        <v>1.5372840000000001</v>
+      </c>
+      <c r="E7">
+        <v>1.4889460000000001</v>
+      </c>
+      <c r="F7">
+        <v>1.554457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>1.5873329999999899</v>
+      </c>
+      <c r="C8">
+        <v>1.6517569999999999</v>
+      </c>
+      <c r="E8">
+        <v>1.64681999999999</v>
+      </c>
+      <c r="F8">
+        <v>1.6936720000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>1.47641</v>
+      </c>
+      <c r="C9">
+        <v>1.522707</v>
+      </c>
+      <c r="E9">
+        <v>1.55275899999999</v>
+      </c>
+      <c r="F9">
+        <v>1.600678</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>1.502985</v>
+      </c>
+      <c r="C10">
+        <v>1.5506040000000001</v>
+      </c>
+      <c r="E10">
+        <v>1.6362650000000001</v>
+      </c>
+      <c r="F10">
+        <v>1.68214</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -776,16 +1548,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>47</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -940,7 +1712,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -973,10 +1745,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -985,7 +1757,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="3"/>
       <c r="I1" s="8" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -994,7 +1766,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -1003,22 +1775,22 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>41</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="F2" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -1061,7 +1833,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1104,7 +1876,7 @@
         <v>1.3500742000000001</v>
       </c>
       <c r="P3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="Q3" t="e">
         <f>B3-I3</f>
@@ -1133,7 +1905,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1176,7 +1948,7 @@
         <v>0.13967913309510532</v>
       </c>
       <c r="P4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="5" t="e">
         <f>Q3*1000</f>
@@ -1202,7 +1974,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1410,7 +2182,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -1443,10 +2215,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1455,7 +2227,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="3"/>
       <c r="I1" s="6" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -1464,7 +2236,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -1473,25 +2245,25 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="G2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -1534,7 +2306,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1583,7 +2355,7 @@
         <v>106.7</v>
       </c>
       <c r="P3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="Q3">
         <f>B3-I3</f>
@@ -1612,7 +2384,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1655,7 +2427,7 @@
         <v>0.33879452626806195</v>
       </c>
       <c r="P4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="Q4" s="5">
         <f>Q3*1000</f>
@@ -1681,7 +2453,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1934,7 +2706,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R17"/>
   <sheetViews>
@@ -1962,10 +2734,10 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1973,7 +2745,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" s="6" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -1981,7 +2753,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="6" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -1990,22 +2762,22 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="D2" t="s">
-        <v>20</v>
+        <v>33</v>
       </c>
       <c r="E2" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="H2" s="2" t="str">
         <f t="array" ref="H2:K2">B2:F2</f>
@@ -2036,7 +2808,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2079,7 +2851,7 @@
         <v>69.7</v>
       </c>
       <c r="N3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="O3">
         <f>B3-H3</f>
@@ -2100,7 +2872,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2135,7 +2907,7 @@
         <v>9.4835850044695941E-2</v>
       </c>
       <c r="N4" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="O4" s="5">
         <f>O3*1000</f>
@@ -2156,7 +2928,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2377,7 +3149,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -2397,45 +3169,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="7" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="3"/>
       <c r="E1" s="7" t="s">
-        <v>14</v>
+        <v>27</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2450,12 +3222,12 @@
         <v>1.3408000000000531E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2474,12 +3246,12 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>17</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2570,7 +3342,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2586,26 +3358,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2618,7 +3390,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2631,7 +3403,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2724,7 +3496,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2740,26 +3512,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2772,7 +3544,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2785,7 +3557,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2862,7 +3634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2878,20 +3650,20 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2904,7 +3676,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2917,7 +3689,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2981,205 +3753,6 @@
       </c>
       <c r="D10">
         <v>0.33001699999999901</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:F10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" width="23.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <f>AVERAGE(B6:B32)</f>
-        <v>1.5002987999999939</v>
-      </c>
-      <c r="C3">
-        <f>AVERAGE(C6:C32)</f>
-        <v>1.5571221999999998</v>
-      </c>
-      <c r="E3">
-        <f>AVERAGE(E6:E32)</f>
-        <v>1.571066199999994</v>
-      </c>
-      <c r="F3">
-        <f>AVERAGE(F6:F32)</f>
-        <v>1.6217526</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <f>STDEVA(B6:B32)</f>
-        <v>5.0955876149856638E-2</v>
-      </c>
-      <c r="C4">
-        <f>STDEVA(C6:C32)</f>
-        <v>5.4136191191293544E-2</v>
-      </c>
-      <c r="E4">
-        <f>STDEVA(E6:E32)</f>
-        <v>6.8393520144085576E-2</v>
-      </c>
-      <c r="F4">
-        <f>STDEVA(F6:F32)</f>
-        <v>6.2694297067597771E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" s="1">
-        <f>B4/B3</f>
-        <v>3.3963818507257916E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <f>C4/C3</f>
-        <v>3.4766822534091128E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <f>E4/E3</f>
-        <v>4.3533187935738057E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <f>F4/F3</f>
-        <v>3.8658360755887036E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>1.46162699999999</v>
-      </c>
-      <c r="C6">
-        <v>1.5232589999999999</v>
-      </c>
-      <c r="E6">
-        <v>1.5305409999999899</v>
-      </c>
-      <c r="F6">
-        <v>1.5778160000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>1.47313899999999</v>
-      </c>
-      <c r="C7">
-        <v>1.5372840000000001</v>
-      </c>
-      <c r="E7">
-        <v>1.4889460000000001</v>
-      </c>
-      <c r="F7">
-        <v>1.554457</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>1.5873329999999899</v>
-      </c>
-      <c r="C8">
-        <v>1.6517569999999999</v>
-      </c>
-      <c r="E8">
-        <v>1.64681999999999</v>
-      </c>
-      <c r="F8">
-        <v>1.6936720000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>1.47641</v>
-      </c>
-      <c r="C9">
-        <v>1.522707</v>
-      </c>
-      <c r="E9">
-        <v>1.55275899999999</v>
-      </c>
-      <c r="F9">
-        <v>1.600678</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>1.502985</v>
-      </c>
-      <c r="C10">
-        <v>1.5506040000000001</v>
-      </c>
-      <c r="E10">
-        <v>1.6362650000000001</v>
-      </c>
-      <c r="F10">
-        <v>1.68214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
home.erb: putting most frequent case first in if..else block sped up code.
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,19 +4,21 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="-520" windowWidth="25160" windowHeight="8380" tabRatio="843"/>
+    <workbookView xWindow="25520" yWindow="-520" windowWidth="25600" windowHeight="14620" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet3" sheetId="11" r:id="rId1"/>
-    <sheet name="@timing framework" sheetId="10" r:id="rId2"/>
-    <sheet name="@orbital_hash" sheetId="9" r:id="rId3"/>
-    <sheet name="term_spans" sheetId="8" r:id="rId4"/>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId5"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId6"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId7"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId8"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId9"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId10"/>
+    <sheet name="storing element.group" sheetId="13" r:id="rId1"/>
+    <sheet name="if else pos neg" sheetId="12" r:id="rId2"/>
+    <sheet name="for vs .each" sheetId="11" r:id="rId3"/>
+    <sheet name="@timing framework" sheetId="10" r:id="rId4"/>
+    <sheet name="@orbital_hash" sheetId="9" r:id="rId5"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId6"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId7"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId8"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId9"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId10"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId11"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId12"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="66">
   <si>
     <t>pt_econfig_this_orbital</t>
   </si>
@@ -74,6 +76,33 @@
   </si>
   <si>
     <t>Avg</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sum of pt steps</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>non-pt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>if element.group == @main_pauses_group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>lastGroup</t>
+  </si>
+  <si>
+    <t>if element.group != @main_pauses_group</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>calling each time</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>storing element.group</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -281,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -289,11 +318,51 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -314,6 +383,23 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -845,17 +931,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="M21" sqref="M21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
   <cols>
-    <col min="2" max="11" width="7.7109375" customWidth="1"/>
-    <col min="14" max="14" width="10.7109375" style="11"/>
-    <col min="17" max="17" width="10.7109375" style="11"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="14" customWidth="1"/>
+    <col min="8" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="14"/>
+    <col min="14" max="14" width="8.5703125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="14"/>
+    <col min="17" max="17" width="8.5703125" style="11" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -863,33 +958,33 @@
         <v>5</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
-      <c r="G1" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
-      <c r="J1" s="6"/>
-      <c r="K1" s="6"/>
-      <c r="L1" s="10" t="str">
+      <c r="G1" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="13" t="str">
         <f>B1</f>
-        <v>for loop</v>
-      </c>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10" t="str">
+        <v>calling each time</v>
+      </c>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="12" t="str">
         <f>G1</f>
-        <v>.each loop</v>
-      </c>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" t="s">
-        <v>49</v>
+        <v>storing element.group</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:18">
@@ -911,7 +1006,7 @@
       <c r="F2">
         <v>5</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="14">
         <f t="array" ref="G2:K2">B2:F2</f>
         <v>1</v>
       </c>
@@ -927,7 +1022,7 @@
       <c r="K2">
         <v>5</v>
       </c>
-      <c r="L2" t="s">
+      <c r="L2" s="14" t="s">
         <v>9</v>
       </c>
       <c r="M2" t="s">
@@ -936,7 +1031,7 @@
       <c r="N2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="O2" t="str">
+      <c r="O2" s="14" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
         <v>Avg</v>
       </c>
@@ -946,373 +1041,1023 @@
       <c r="Q2" s="11" t="str">
         <v>RelStdDev</v>
       </c>
-      <c r="R2" t="s">
+      <c r="R2" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B3">
-        <v>5.3610000000000003E-3</v>
+        <v>16</v>
+      </c>
+      <c r="B3" s="14">
+        <v>8.8199999999999997E-4</v>
       </c>
       <c r="C3">
-        <v>5.731E-3</v>
-      </c>
-      <c r="L3">
+        <v>7.7800000000000005E-4</v>
+      </c>
+      <c r="D3">
+        <v>3.7859999999999999E-3</v>
+      </c>
+      <c r="E3">
+        <v>9.3300000000000002E-4</v>
+      </c>
+      <c r="F3">
+        <v>8.7000000000000001E-4</v>
+      </c>
+      <c r="G3" s="14">
+        <v>5.8900000000000001E-4</v>
+      </c>
+      <c r="H3">
+        <v>6.1300000000000005E-4</v>
+      </c>
+      <c r="I3">
+        <v>7.2900000000000005E-4</v>
+      </c>
+      <c r="J3">
+        <v>5.62E-4</v>
+      </c>
+      <c r="K3">
+        <v>6.6600000000000003E-4</v>
+      </c>
+      <c r="L3" s="14">
         <f>AVERAGE(B3:F3)</f>
-        <v>5.5460000000000006E-3</v>
+        <v>1.4497999999999998E-3</v>
       </c>
       <c r="M3">
         <f>STDEVA(B3:F3)</f>
-        <v>2.6162950903903102E-4</v>
+        <v>1.3071718326218634E-3</v>
       </c>
       <c r="N3" s="11">
         <f>M3/L3</f>
-        <v>4.7174451683921925E-2</v>
-      </c>
-      <c r="R3">
+        <v>0.90162217728091021</v>
+      </c>
+      <c r="O3" s="14">
+        <f>AVERAGE(E3:I3)</f>
+        <v>7.4679999999999994E-4</v>
+      </c>
+      <c r="P3">
+        <f>STDEVA(E3:I3)</f>
+        <v>1.5245392746662887E-4</v>
+      </c>
+      <c r="Q3" s="11">
+        <f>P3/O3</f>
+        <v>0.20414291305119026</v>
+      </c>
+      <c r="R3" s="14">
         <f t="array" ref="R3:R16">O3:O16-L3:L16</f>
-        <v>-5.5460000000000006E-3</v>
+        <v>-7.0299999999999985E-4</v>
       </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4">
-        <v>3.5630000000000002E-3</v>
+        <v>57</v>
+      </c>
+      <c r="B4" s="14">
+        <v>5.5449999999999996E-3</v>
       </c>
       <c r="C4">
-        <v>3.7069999999999998E-3</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:L16" si="0">AVERAGE(B4:F4)</f>
-        <v>3.6350000000000002E-3</v>
+        <v>5.5370000000000003E-3</v>
+      </c>
+      <c r="D4">
+        <v>5.4060000000000002E-3</v>
+      </c>
+      <c r="E4">
+        <v>5.9839999999999997E-3</v>
+      </c>
+      <c r="F4">
+        <v>5.4660000000000004E-3</v>
+      </c>
+      <c r="G4" s="14">
+        <v>5.6940000000000003E-3</v>
+      </c>
+      <c r="H4">
+        <v>8.9409999999999993E-3</v>
+      </c>
+      <c r="I4">
+        <v>7.1890000000000001E-3</v>
+      </c>
+      <c r="J4">
+        <v>5.8830000000000002E-3</v>
+      </c>
+      <c r="K4">
+        <v>5.7710000000000001E-3</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" ref="L4:L18" si="0">AVERAGE(B4:F4)</f>
+        <v>5.5875999999999999E-3</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M16" si="1">STDEVA(B4:F4)</f>
-        <v>1.0182337649085403E-4</v>
+        <f t="shared" ref="M4:M18" si="1">STDEVA(B4:F4)</f>
+        <v>2.2873193917774225E-4</v>
       </c>
       <c r="N4" s="11">
-        <f t="shared" ref="N4:N16" si="2">M4/L4</f>
-        <v>2.8011933009863554E-2</v>
-      </c>
-      <c r="R4">
-        <v>-3.6350000000000002E-3</v>
+        <f t="shared" ref="N4:N18" si="2">M4/L4</f>
+        <v>4.0935632324744481E-2</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" ref="O4:O18" si="3">AVERAGE(E4:I4)</f>
+        <v>6.6547999999999998E-3</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P18" si="4">STDEVA(E4:I4)</f>
+        <v>1.4403502004720953E-3</v>
+      </c>
+      <c r="Q4" s="11">
+        <f t="shared" ref="Q4:Q18" si="5">P4/O4</f>
+        <v>0.21643778933583208</v>
+      </c>
+      <c r="R4" s="14">
+        <v>1.0671999999999999E-3</v>
       </c>
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>52</v>
-      </c>
-      <c r="B5">
-        <v>0.27063799999999999</v>
+        <v>58</v>
+      </c>
+      <c r="B5" s="14">
+        <v>3.5990000000000002E-3</v>
       </c>
       <c r="C5">
-        <v>0.28170800000000001</v>
-      </c>
-      <c r="L5">
+        <v>3.542E-3</v>
+      </c>
+      <c r="D5">
+        <v>3.2940000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>4.0099999999999997E-3</v>
+      </c>
+      <c r="F5">
+        <v>3.4259999999999998E-3</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3.6219999999999998E-3</v>
+      </c>
+      <c r="H5">
+        <v>4.3369999999999997E-3</v>
+      </c>
+      <c r="I5">
+        <v>4.1539999999999997E-3</v>
+      </c>
+      <c r="J5">
+        <v>3.5439999999999998E-3</v>
+      </c>
+      <c r="K5">
+        <v>3.7130000000000002E-3</v>
+      </c>
+      <c r="L5" s="14">
         <f t="shared" si="0"/>
-        <v>0.276173</v>
+        <v>3.5741999999999996E-3</v>
       </c>
       <c r="M5">
         <f t="shared" si="1"/>
-        <v>7.8276720677375299E-3</v>
+        <v>2.7020769789182577E-4</v>
       </c>
       <c r="N5" s="11">
         <f t="shared" si="2"/>
-        <v>2.8343364730576595E-2</v>
-      </c>
-      <c r="R5">
-        <v>-0.276173</v>
+        <v>7.5599490205311898E-2</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" si="3"/>
+        <v>3.9097999999999997E-3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>3.7718191897280007E-4</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="5"/>
+        <v>9.647089850447596E-2</v>
+      </c>
+      <c r="R5" s="14">
+        <v>3.3560000000000013E-4</v>
       </c>
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6">
-        <v>4.0070000000000001E-3</v>
+        <v>59</v>
+      </c>
+      <c r="B6" s="14">
+        <v>0.237287</v>
       </c>
       <c r="C6">
-        <v>4.5849999999999997E-3</v>
-      </c>
-      <c r="L6">
+        <v>0.203294</v>
+      </c>
+      <c r="D6">
+        <v>0.207894</v>
+      </c>
+      <c r="E6">
+        <v>0.24184900000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.23368</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.25685000000000002</v>
+      </c>
+      <c r="H6">
+        <v>0.310392</v>
+      </c>
+      <c r="I6">
+        <v>0.244006</v>
+      </c>
+      <c r="J6">
+        <v>0.23882800000000001</v>
+      </c>
+      <c r="K6">
+        <v>0.240255</v>
+      </c>
+      <c r="L6" s="14">
         <f t="shared" si="0"/>
-        <v>4.2959999999999995E-3</v>
+        <v>0.2248008</v>
       </c>
       <c r="M6">
         <f t="shared" si="1"/>
-        <v>4.0870771952583503E-4</v>
+        <v>1.7844949136940558E-2</v>
       </c>
       <c r="N6" s="11">
         <f t="shared" si="2"/>
-        <v>9.5136806221097547E-2</v>
-      </c>
-      <c r="R6">
-        <v>-4.2959999999999995E-3</v>
+        <v>7.9381163843458558E-2</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="3"/>
+        <v>0.25735540000000001</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>3.0790890922479056E-2</v>
+      </c>
+      <c r="Q6" s="11">
+        <f t="shared" si="5"/>
+        <v>0.11964346161953103</v>
+      </c>
+      <c r="R6" s="14">
+        <v>3.2554600000000017E-2</v>
       </c>
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>54</v>
-      </c>
-      <c r="B7">
-        <v>4.6899000000000003E-2</v>
+        <v>60</v>
+      </c>
+      <c r="B7" s="14">
+        <v>3.7789999999999998E-3</v>
       </c>
       <c r="C7">
-        <v>5.1619999999999999E-2</v>
-      </c>
-      <c r="L7">
+        <v>4.2139999999999999E-3</v>
+      </c>
+      <c r="D7">
+        <v>3.8270000000000001E-3</v>
+      </c>
+      <c r="E7">
+        <v>4.2430000000000002E-3</v>
+      </c>
+      <c r="F7">
+        <v>3.725E-3</v>
+      </c>
+      <c r="G7" s="14">
+        <v>4.0590000000000001E-3</v>
+      </c>
+      <c r="H7">
+        <v>4.5739999999999999E-3</v>
+      </c>
+      <c r="I7">
+        <v>4.3E-3</v>
+      </c>
+      <c r="J7">
+        <v>3.8920000000000001E-3</v>
+      </c>
+      <c r="K7">
+        <v>5.0049999999999999E-3</v>
+      </c>
+      <c r="L7" s="14">
         <f t="shared" si="0"/>
-        <v>4.9259499999999998E-2</v>
+        <v>3.9576000000000004E-3</v>
       </c>
       <c r="M7">
         <f t="shared" si="1"/>
-        <v>3.3382511139819393E-3</v>
+        <v>2.5012556846511561E-4</v>
       </c>
       <c r="N7" s="11">
         <f t="shared" si="2"/>
-        <v>6.7768676376778886E-2</v>
-      </c>
-      <c r="R7">
-        <v>-4.9259499999999998E-2</v>
+        <v>6.3201326173720332E-2</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="3"/>
+        <v>4.1801999999999994E-3</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>3.1435282724989814E-4</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="5"/>
+        <v>7.5200427551288973E-2</v>
+      </c>
+      <c r="R7" s="14">
+        <v>2.2259999999999901E-4</v>
       </c>
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8">
-        <v>2.0709999999999999E-3</v>
+        <v>61</v>
+      </c>
+      <c r="B8" s="14">
+        <v>4.7253000000000003E-2</v>
       </c>
       <c r="C8">
-        <v>2.421E-3</v>
-      </c>
-      <c r="L8">
+        <v>4.7164999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>6.4308000000000004E-2</v>
+      </c>
+      <c r="E8">
+        <v>5.2380000000000003E-2</v>
+      </c>
+      <c r="F8">
+        <v>4.4886000000000002E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>8.9952000000000004E-2</v>
+      </c>
+      <c r="H8">
+        <v>5.8425999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>5.4385999999999997E-2</v>
+      </c>
+      <c r="J8">
+        <v>4.9264000000000002E-2</v>
+      </c>
+      <c r="K8">
+        <v>4.9154999999999997E-2</v>
+      </c>
+      <c r="L8" s="14">
         <f t="shared" si="0"/>
-        <v>2.2459999999999997E-3</v>
+        <v>5.1198399999999998E-2</v>
       </c>
       <c r="M8">
         <f t="shared" si="1"/>
-        <v>2.4748737341529604E-4</v>
+        <v>7.8252584813538438E-3</v>
       </c>
       <c r="N8" s="11">
         <f t="shared" si="2"/>
-        <v>0.11019028201927697</v>
-      </c>
-      <c r="R8">
-        <v>-2.2459999999999997E-3</v>
+        <v>0.15284185602194295</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="3"/>
+        <v>6.0006000000000004E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>1.7447163035863446E-2</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="5"/>
+        <v>0.29075697490023406</v>
+      </c>
+      <c r="R8" s="14">
+        <v>8.8076000000000057E-3</v>
       </c>
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>56</v>
-      </c>
-      <c r="B9">
-        <v>0.124172</v>
+        <v>62</v>
+      </c>
+      <c r="B9" s="14">
+        <v>1.936E-3</v>
       </c>
       <c r="C9">
-        <v>0.15309</v>
-      </c>
-      <c r="L9">
+        <v>1.8860000000000001E-3</v>
+      </c>
+      <c r="D9">
+        <v>1.885E-3</v>
+      </c>
+      <c r="E9">
+        <v>2.2529999999999998E-3</v>
+      </c>
+      <c r="F9">
+        <v>2.0470000000000002E-3</v>
+      </c>
+      <c r="G9" s="14">
+        <v>2.0579999999999999E-3</v>
+      </c>
+      <c r="H9">
+        <v>2.4060000000000002E-3</v>
+      </c>
+      <c r="I9">
+        <v>2.63E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.9369999999999999E-3</v>
+      </c>
+      <c r="K9">
+        <v>2.026E-3</v>
+      </c>
+      <c r="L9" s="14">
         <f t="shared" si="0"/>
-        <v>0.138631</v>
+        <v>2.0014E-3</v>
       </c>
       <c r="M9">
         <f t="shared" si="1"/>
-        <v>2.0448113898352698E-2</v>
+        <v>1.5534252476382342E-4</v>
       </c>
       <c r="N9" s="11">
         <f t="shared" si="2"/>
-        <v>0.1475002986226219</v>
-      </c>
-      <c r="R9">
-        <v>-0.138631</v>
+        <v>7.7616930530540335E-2</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="3"/>
+        <v>2.2788000000000001E-3</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>2.463081403445663E-4</v>
+      </c>
+      <c r="Q9" s="11">
+        <f t="shared" si="5"/>
+        <v>0.10808677389177036</v>
+      </c>
+      <c r="R9" s="14">
+        <v>2.7740000000000013E-4</v>
       </c>
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="B10">
-        <v>3.503E-3</v>
+        <v>64</v>
+      </c>
+      <c r="B10" s="14">
+        <v>0.142016</v>
       </c>
       <c r="C10">
-        <v>3.4680000000000002E-3</v>
-      </c>
-      <c r="L10">
+        <v>0.140565</v>
+      </c>
+      <c r="D10">
+        <v>0.124282</v>
+      </c>
+      <c r="E10">
+        <v>0.19983100000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.122373</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.15872</v>
+      </c>
+      <c r="H10">
+        <v>0.149228</v>
+      </c>
+      <c r="I10">
+        <v>0.161359</v>
+      </c>
+      <c r="J10">
+        <v>0.13034799999999999</v>
+      </c>
+      <c r="K10">
+        <v>0.13450000000000001</v>
+      </c>
+      <c r="L10" s="14">
         <f t="shared" si="0"/>
-        <v>3.4854999999999999E-3</v>
+        <v>0.14581339999999998</v>
       </c>
       <c r="M10">
         <f t="shared" si="1"/>
-        <v>2.4748737341573409E-5</v>
+        <v>3.1515554085245132E-2</v>
       </c>
       <c r="N10" s="11">
         <f t="shared" si="2"/>
-        <v>7.1004841031626484E-3</v>
-      </c>
-      <c r="R10">
-        <v>-3.4854999999999999E-3</v>
+        <v>0.21613619931532449</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="3"/>
+        <v>0.1583022</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>2.7872066351456511E-2</v>
+      </c>
+      <c r="Q10" s="11">
+        <f t="shared" si="5"/>
+        <v>0.17606872394354917</v>
+      </c>
+      <c r="R10" s="14">
+        <v>1.2488800000000022E-2</v>
       </c>
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B11">
-        <v>1.0169999999999999E-3</v>
+        <v>65</v>
+      </c>
+      <c r="B11" s="14">
+        <v>8.6300000000000005E-4</v>
       </c>
       <c r="C11">
-        <v>9.0200000000000002E-4</v>
-      </c>
-      <c r="L11">
+        <v>8.7699999999999996E-4</v>
+      </c>
+      <c r="D11">
+        <v>8.8199999999999997E-4</v>
+      </c>
+      <c r="E11">
+        <v>9.1E-4</v>
+      </c>
+      <c r="F11">
+        <v>9.3300000000000002E-4</v>
+      </c>
+      <c r="G11" s="14">
+        <v>8.4599999999999996E-4</v>
+      </c>
+      <c r="H11">
+        <v>9.9700000000000006E-4</v>
+      </c>
+      <c r="I11">
+        <v>1.0510000000000001E-3</v>
+      </c>
+      <c r="J11">
+        <v>1.1199999999999999E-3</v>
+      </c>
+      <c r="K11">
+        <v>8.3299999999999997E-4</v>
+      </c>
+      <c r="L11" s="14">
         <f t="shared" si="0"/>
-        <v>9.5949999999999996E-4</v>
+        <v>8.9300000000000002E-4</v>
       </c>
       <c r="M11">
         <f t="shared" si="1"/>
-        <v>8.1317279836452277E-5</v>
+        <v>2.8133609793269177E-5</v>
       </c>
       <c r="N11" s="11">
         <f t="shared" si="2"/>
-        <v>8.4749640267276993E-2</v>
-      </c>
-      <c r="R11">
-        <v>-9.5949999999999996E-4</v>
+        <v>3.1504602232104342E-2</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="3"/>
+        <v>9.4739999999999993E-4</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>7.9185225894734296E-5</v>
+      </c>
+      <c r="Q11" s="11">
+        <f t="shared" si="5"/>
+        <v>8.3581619057139858E-2</v>
+      </c>
+      <c r="R11" s="14">
+        <v>5.4399999999999913E-5</v>
       </c>
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
         <v>0</v>
       </c>
-      <c r="B12">
-        <v>4.4000000000000003E-3</v>
+      <c r="B12" s="14">
+        <v>4.8430000000000001E-3</v>
       </c>
       <c r="C12">
-        <v>4.8469999999999997E-3</v>
-      </c>
-      <c r="L12">
+        <v>4.6100000000000004E-3</v>
+      </c>
+      <c r="D12">
+        <v>5.1659999999999996E-3</v>
+      </c>
+      <c r="E12">
+        <v>6.2249999999999996E-3</v>
+      </c>
+      <c r="F12">
+        <v>4.8710000000000003E-3</v>
+      </c>
+      <c r="G12" s="14">
+        <v>5.6990000000000001E-3</v>
+      </c>
+      <c r="H12">
+        <v>5.8669999999999998E-3</v>
+      </c>
+      <c r="I12">
+        <v>5.5160000000000001E-3</v>
+      </c>
+      <c r="J12">
+        <v>5.1879999999999999E-3</v>
+      </c>
+      <c r="K12">
+        <v>5.4180000000000001E-3</v>
+      </c>
+      <c r="L12" s="14">
         <f t="shared" si="0"/>
-        <v>4.6235E-3</v>
+        <v>5.143E-3</v>
       </c>
       <c r="M12">
         <f t="shared" si="1"/>
-        <v>3.1607673119038324E-4</v>
+        <v>6.3626370319231317E-4</v>
       </c>
       <c r="N12" s="11">
         <f t="shared" si="2"/>
-        <v>6.8363086663865744E-2</v>
-      </c>
-      <c r="R12">
-        <v>-4.6235E-3</v>
+        <v>0.12371450577334497</v>
+      </c>
+      <c r="O12" s="14">
+        <f t="shared" si="3"/>
+        <v>5.6356000000000002E-3</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>5.0096786324074739E-4</v>
+      </c>
+      <c r="Q12" s="11">
+        <f t="shared" si="5"/>
+        <v>8.8893438718281523E-2</v>
+      </c>
+      <c r="R12" s="14">
+        <v>4.9260000000000016E-4</v>
       </c>
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
         <v>1</v>
       </c>
-      <c r="B13">
-        <v>2.532E-3</v>
+      <c r="B13" s="14">
+        <v>2.7299999999999998E-3</v>
       </c>
       <c r="C13">
-        <v>2.539E-3</v>
-      </c>
-      <c r="L13">
+        <v>2.771E-3</v>
+      </c>
+      <c r="D13">
+        <v>2.8549999999999999E-3</v>
+      </c>
+      <c r="E13">
+        <v>2.7560000000000002E-3</v>
+      </c>
+      <c r="F13">
+        <v>2.6129999999999999E-3</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2.885E-3</v>
+      </c>
+      <c r="H13">
+        <v>3.3679999999999999E-3</v>
+      </c>
+      <c r="I13">
+        <v>2.6540000000000001E-3</v>
+      </c>
+      <c r="J13">
+        <v>2.6779999999999998E-3</v>
+      </c>
+      <c r="K13">
+        <v>2.9510000000000001E-3</v>
+      </c>
+      <c r="L13" s="14">
         <f t="shared" si="0"/>
-        <v>2.5355E-3</v>
+        <v>2.7449999999999996E-3</v>
       </c>
       <c r="M13">
         <f t="shared" si="1"/>
-        <v>4.9497474683420624E-6</v>
+        <v>8.7387069981793955E-5</v>
       </c>
       <c r="N13" s="11">
         <f t="shared" si="2"/>
-        <v>1.9521780589004387E-3</v>
-      </c>
-      <c r="R13">
-        <v>-2.5355E-3</v>
+        <v>3.1834998171873942E-2</v>
+      </c>
+      <c r="O13" s="14">
+        <f t="shared" si="3"/>
+        <v>2.8552E-3</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>3.0530099901572409E-4</v>
+      </c>
+      <c r="Q13" s="11">
+        <f t="shared" si="5"/>
+        <v>0.10692806073680446</v>
+      </c>
+      <c r="R13" s="14">
+        <v>1.102000000000004E-4</v>
       </c>
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
         <v>2</v>
       </c>
-      <c r="B14">
-        <v>1.658E-3</v>
+      <c r="B14" s="14">
+        <v>1.7639999999999999E-3</v>
       </c>
       <c r="C14">
-        <v>1.8810000000000001E-3</v>
-      </c>
-      <c r="L14">
+        <v>1.719E-3</v>
+      </c>
+      <c r="D14">
+        <v>1.5759999999999999E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.704E-3</v>
+      </c>
+      <c r="F14">
+        <v>1.6670000000000001E-3</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1.7229999999999999E-3</v>
+      </c>
+      <c r="H14">
+        <v>1.6919999999999999E-3</v>
+      </c>
+      <c r="I14">
+        <v>1.8450000000000001E-3</v>
+      </c>
+      <c r="J14">
+        <v>1.916E-3</v>
+      </c>
+      <c r="K14">
+        <v>1.9530000000000001E-3</v>
+      </c>
+      <c r="L14" s="14">
         <f t="shared" si="0"/>
-        <v>1.7695E-3</v>
+        <v>1.686E-3</v>
       </c>
       <c r="M14">
         <f t="shared" si="1"/>
-        <v>1.5768481220459723E-4</v>
+        <v>7.0636392886383684E-5</v>
       </c>
       <c r="N14" s="11">
         <f t="shared" si="2"/>
-        <v>8.9112637583835669E-2</v>
-      </c>
-      <c r="R14">
-        <v>-1.7695E-3</v>
+        <v>4.1895843942101829E-2</v>
+      </c>
+      <c r="O14" s="14">
+        <f t="shared" si="3"/>
+        <v>1.7262E-3</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>6.9445662211542746E-5</v>
+      </c>
+      <c r="Q14" s="11">
+        <f t="shared" si="5"/>
+        <v>4.0230368561894769E-2</v>
+      </c>
+      <c r="R14" s="14">
+        <v>4.0200000000000001E-5</v>
       </c>
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
         <v>3</v>
       </c>
-      <c r="B15">
-        <v>1.8220000000000001E-3</v>
+      <c r="B15" s="14">
+        <v>1.934E-3</v>
       </c>
       <c r="C15">
-        <v>1.8710000000000001E-3</v>
-      </c>
-      <c r="L15">
+        <v>1.8439999999999999E-3</v>
+      </c>
+      <c r="D15">
+        <v>1.9430000000000001E-3</v>
+      </c>
+      <c r="E15">
+        <v>1.8799999999999999E-3</v>
+      </c>
+      <c r="F15">
+        <v>1.789E-3</v>
+      </c>
+      <c r="G15" s="14">
+        <v>2.0999999999999999E-3</v>
+      </c>
+      <c r="H15">
+        <v>1.9300000000000001E-3</v>
+      </c>
+      <c r="I15">
+        <v>2.0070000000000001E-3</v>
+      </c>
+      <c r="J15">
+        <v>1.864E-3</v>
+      </c>
+      <c r="K15">
+        <v>2.1549999999999998E-3</v>
+      </c>
+      <c r="L15" s="14">
         <f t="shared" si="0"/>
-        <v>1.8465000000000001E-3</v>
+        <v>1.8780000000000001E-3</v>
       </c>
       <c r="M15">
         <f t="shared" si="1"/>
-        <v>3.4648232278137748E-5</v>
+        <v>6.4113181172043094E-5</v>
       </c>
       <c r="N15" s="11">
         <f t="shared" si="2"/>
-        <v>1.8764274182582044E-2</v>
-      </c>
-      <c r="R15">
-        <v>-1.8465000000000001E-3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
+        <v>3.4139074106519215E-2</v>
+      </c>
+      <c r="O15" s="14">
+        <f t="shared" si="3"/>
+        <v>1.9411999999999999E-3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>1.1893569691223808E-4</v>
+      </c>
+      <c r="Q15" s="11">
+        <f t="shared" si="5"/>
+        <v>6.1269161813434003E-2</v>
+      </c>
+      <c r="R15" s="14">
+        <v>6.3199999999999801E-5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" ht="14" thickBot="1">
       <c r="A16" t="s">
         <v>4</v>
       </c>
-      <c r="B16">
-        <v>0.60263599999999995</v>
+      <c r="B16" s="14">
+        <v>0.59009500000000004</v>
       </c>
       <c r="C16">
-        <v>0.65221099999999999</v>
-      </c>
-      <c r="L16">
+        <v>0.57384800000000002</v>
+      </c>
+      <c r="D16">
+        <v>0.57799500000000004</v>
+      </c>
+      <c r="E16">
+        <v>0.66256300000000001</v>
+      </c>
+      <c r="F16">
+        <v>0.57065900000000003</v>
+      </c>
+      <c r="G16" s="20">
+        <v>0.66956300000000002</v>
+      </c>
+      <c r="H16">
+        <v>0.74128700000000003</v>
+      </c>
+      <c r="I16">
+        <v>0.66476400000000002</v>
+      </c>
+      <c r="J16">
+        <v>0.61994099999999996</v>
+      </c>
+      <c r="K16">
+        <v>0.62372499999999997</v>
+      </c>
+      <c r="L16" s="14">
         <f t="shared" si="0"/>
-        <v>0.62742349999999991</v>
+        <v>0.59503200000000001</v>
       </c>
       <c r="M16">
         <f t="shared" si="1"/>
-        <v>3.505481867732517E-2</v>
+        <v>3.8463860583668637E-2</v>
       </c>
       <c r="N16" s="11">
         <f t="shared" si="2"/>
-        <v>5.5871064245003856E-2</v>
-      </c>
-      <c r="R16">
-        <v>-0.62742349999999991</v>
+        <v>6.4641667311453224E-2</v>
+      </c>
+      <c r="O16" s="14">
+        <f t="shared" si="3"/>
+        <v>0.66176720000000011</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>6.0610418462505145E-2</v>
+      </c>
+      <c r="Q16" s="11">
+        <f t="shared" si="5"/>
+        <v>9.1588731600032655E-2</v>
+      </c>
+      <c r="R16" s="14">
+        <v>6.6735200000000106E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" s="17" customFormat="1">
+      <c r="A17" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="17">
+        <f>SUM(B3:B15)</f>
+        <v>0.45443099999999992</v>
+      </c>
+      <c r="C17" s="17">
+        <f t="shared" ref="C17:K17" si="6">SUM(C3:C15)</f>
+        <v>0.41880200000000006</v>
+      </c>
+      <c r="D17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.42710399999999998</v>
+      </c>
+      <c r="E17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.52495800000000004</v>
+      </c>
+      <c r="F17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.428346</v>
+      </c>
+      <c r="G17" s="19">
+        <f t="shared" si="6"/>
+        <v>0.53479700000000008</v>
+      </c>
+      <c r="H17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.55277100000000001</v>
+      </c>
+      <c r="I17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.4918260000000001</v>
+      </c>
+      <c r="J17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.44702400000000003</v>
+      </c>
+      <c r="K17" s="17">
+        <f t="shared" si="6"/>
+        <v>0.45440099999999989</v>
+      </c>
+      <c r="L17" s="19">
+        <f t="shared" si="0"/>
+        <v>0.45072820000000002</v>
+      </c>
+      <c r="M17" s="17">
+        <f t="shared" si="1"/>
+        <v>4.3595073932727532E-2</v>
+      </c>
+      <c r="N17" s="18">
+        <f t="shared" si="2"/>
+        <v>9.6721425312921466E-2</v>
+      </c>
+      <c r="O17" s="19">
+        <f t="shared" si="3"/>
+        <v>0.50653960000000009</v>
+      </c>
+      <c r="P17" s="17">
+        <f t="shared" si="4"/>
+        <v>4.9004565004701281E-2</v>
+      </c>
+      <c r="Q17" s="18">
+        <f t="shared" si="5"/>
+        <v>9.6743798519802346E-2</v>
+      </c>
+      <c r="R17" s="19">
+        <f t="array" ref="R17">O17:O30-L17:L30</f>
+        <v>5.5811400000000067E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f>B16-B17</f>
+        <v>0.13566400000000012</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:K18" si="7">C16-C17</f>
+        <v>0.15504599999999996</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="7"/>
+        <v>0.15089100000000005</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>0.13760499999999998</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>0.14231300000000002</v>
+      </c>
+      <c r="G18" s="14">
+        <f t="shared" si="7"/>
+        <v>0.13476599999999994</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>0.18851600000000002</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>0.17293799999999993</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="7"/>
+        <v>0.17291699999999993</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="7"/>
+        <v>0.16932400000000009</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="0"/>
+        <v>0.14430380000000004</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>8.4004377088338026E-3</v>
+      </c>
+      <c r="N18" s="11">
+        <f t="shared" si="2"/>
+        <v>5.8213558539926186E-2</v>
+      </c>
+      <c r="O18" s="14">
+        <f t="shared" si="3"/>
+        <v>0.15522759999999997</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>2.4071746099940394E-2</v>
+      </c>
+      <c r="Q18" s="11">
+        <f t="shared" si="5"/>
+        <v>0.15507387925820151</v>
+      </c>
+      <c r="R18" s="14">
+        <f t="array" ref="R18">O18:O31-L18:L31</f>
+        <v>1.0923799999999928E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1335,6 +2080,278 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.44118779999999946</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(D6:D32)</f>
+        <v>0.45040099999999939</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.1336102659575439E-2</v>
+      </c>
+      <c r="D4">
+        <f>STDEVA(D6:D32)</f>
+        <v>3.2935379806523481E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>4.8360590795066105E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D4/D3</f>
+        <v>7.3124570785863097E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.42475299999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.39991199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.438661999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.45086799999999899</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.446709999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.484957999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.42122699999999902</v>
+      </c>
+      <c r="D9">
+        <v>0.44270900000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.47458699999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.47355799999999898</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="4.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.24570099999999978</v>
+      </c>
+      <c r="D3">
+        <f>AVERAGE(D6:D32)</f>
+        <v>0.3320297999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.0237555966569346E-2</v>
+      </c>
+      <c r="D4">
+        <f>STDEVA(D6:D32)</f>
+        <v>3.7396661477998347E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>8.2366599918475558E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f>D4/D3</f>
+        <v>0.11263043702100954</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.275005</v>
+      </c>
+      <c r="D6">
+        <v>0.32842199999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.23533599999999999</v>
+      </c>
+      <c r="D7">
+        <v>0.37503599999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.224244999999999</v>
+      </c>
+      <c r="D8">
+        <v>0.27442299999999997</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.23674799999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.35225099999999898</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.25717099999999998</v>
+      </c>
+      <c r="D10">
+        <v>0.33001699999999901</v>
+      </c>
+    </row>
+  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1350,32 +2367,32 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1396,7 +2413,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1417,7 +2434,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1522,6 +2539,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1533,6 +2551,2299 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="K25" sqref="K25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="14" customWidth="1"/>
+    <col min="8" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="14"/>
+    <col min="14" max="14" width="8.5703125" style="11" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="14"/>
+    <col min="17" max="17" width="8.5703125" style="11" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="14"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="13" t="str">
+        <f>B1</f>
+        <v>if element.group == @main_pauses_group</v>
+      </c>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="12" t="str">
+        <f>G1</f>
+        <v>if element.group != @main_pauses_group</v>
+      </c>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="14">
+        <f t="array" ref="G2:K2">B2:F2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" s="14" t="str">
+        <f t="array" ref="O2:Q2">L2:N2</f>
+        <v>Avg</v>
+      </c>
+      <c r="P2" t="str">
+        <v>StDev</v>
+      </c>
+      <c r="Q2" s="11" t="str">
+        <v>RelStdDev</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>7.2000000000000005E-4</v>
+      </c>
+      <c r="C3">
+        <v>1.4450000000000001E-3</v>
+      </c>
+      <c r="D3">
+        <v>7.3399999999999995E-4</v>
+      </c>
+      <c r="E3">
+        <v>7.4700000000000005E-4</v>
+      </c>
+      <c r="F3">
+        <v>6.6200000000000005E-4</v>
+      </c>
+      <c r="G3" s="14">
+        <v>8.8199999999999997E-4</v>
+      </c>
+      <c r="H3">
+        <v>7.7800000000000005E-4</v>
+      </c>
+      <c r="I3">
+        <v>3.7859999999999999E-3</v>
+      </c>
+      <c r="J3">
+        <v>9.3300000000000002E-4</v>
+      </c>
+      <c r="K3">
+        <v>8.7000000000000001E-4</v>
+      </c>
+      <c r="L3" s="14">
+        <f>AVERAGE(B3:F3)</f>
+        <v>8.6160000000000002E-4</v>
+      </c>
+      <c r="M3">
+        <f>STDEVA(B3:F3)</f>
+        <v>3.2774273447324509E-4</v>
+      </c>
+      <c r="N3" s="11">
+        <f>M3/L3</f>
+        <v>0.38038850333477842</v>
+      </c>
+      <c r="O3" s="14">
+        <f>AVERAGE(E3:I3)</f>
+        <v>1.371E-3</v>
+      </c>
+      <c r="P3">
+        <f>STDEVA(E3:I3)</f>
+        <v>1.3523176402014429E-3</v>
+      </c>
+      <c r="Q3" s="11">
+        <f>P3/O3</f>
+        <v>0.98637318760134418</v>
+      </c>
+      <c r="R3" s="14">
+        <f t="array" ref="R3:R16">O3:O16-L3:L16</f>
+        <v>5.0940000000000002E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B4">
+        <v>5.7739999999999996E-3</v>
+      </c>
+      <c r="C4">
+        <v>8.2579999999999997E-3</v>
+      </c>
+      <c r="D4">
+        <v>5.9410000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>4.0212999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>5.3889999999999997E-3</v>
+      </c>
+      <c r="G4" s="14">
+        <v>5.5449999999999996E-3</v>
+      </c>
+      <c r="H4">
+        <v>5.5370000000000003E-3</v>
+      </c>
+      <c r="I4">
+        <v>5.4060000000000002E-3</v>
+      </c>
+      <c r="J4">
+        <v>5.9839999999999997E-3</v>
+      </c>
+      <c r="K4">
+        <v>5.4660000000000004E-3</v>
+      </c>
+      <c r="L4" s="14">
+        <f t="shared" ref="L4:L18" si="0">AVERAGE(B4:F4)</f>
+        <v>1.3114999999999998E-2</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M18" si="1">STDEVA(B4:F4)</f>
+        <v>1.5189961207982067E-2</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" ref="N4:N18" si="2">M4/L4</f>
+        <v>1.1582128256181525</v>
+      </c>
+      <c r="O4" s="14">
+        <f t="shared" ref="O4:O18" si="3">AVERAGE(E4:I4)</f>
+        <v>1.2418E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P18" si="4">STDEVA(E4:I4)</f>
+        <v>1.5538044439375245E-2</v>
+      </c>
+      <c r="Q4" s="11">
+        <f t="shared" ref="Q4:Q18" si="5">P4/O4</f>
+        <v>1.2512517667398328</v>
+      </c>
+      <c r="R4" s="14">
+        <v>-6.9699999999999797E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>3.506E-3</v>
+      </c>
+      <c r="C5">
+        <v>5.2750000000000002E-3</v>
+      </c>
+      <c r="D5">
+        <v>3.4009999999999999E-3</v>
+      </c>
+      <c r="E5">
+        <v>3.8579999999999999E-3</v>
+      </c>
+      <c r="F5">
+        <v>3.3219999999999999E-3</v>
+      </c>
+      <c r="G5" s="14">
+        <v>3.5990000000000002E-3</v>
+      </c>
+      <c r="H5">
+        <v>3.542E-3</v>
+      </c>
+      <c r="I5">
+        <v>3.2940000000000001E-3</v>
+      </c>
+      <c r="J5">
+        <v>4.0099999999999997E-3</v>
+      </c>
+      <c r="K5">
+        <v>3.4259999999999998E-3</v>
+      </c>
+      <c r="L5" s="14">
+        <f t="shared" si="0"/>
+        <v>3.8723999999999994E-3</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>8.1038589573116746E-4</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.20927225899472357</v>
+      </c>
+      <c r="O5" s="14">
+        <f t="shared" si="3"/>
+        <v>3.5229999999999997E-3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>2.2978468182192511E-4</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="5"/>
+        <v>6.5224150389419561E-2</v>
+      </c>
+      <c r="R5" s="14">
+        <v>-3.4939999999999971E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6">
+        <v>0.23477999999999999</v>
+      </c>
+      <c r="C6">
+        <v>0.34004899999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.214394</v>
+      </c>
+      <c r="E6">
+        <v>0.219911</v>
+      </c>
+      <c r="F6">
+        <v>0.225803</v>
+      </c>
+      <c r="G6" s="14">
+        <v>0.237287</v>
+      </c>
+      <c r="H6">
+        <v>0.203294</v>
+      </c>
+      <c r="I6">
+        <v>0.207894</v>
+      </c>
+      <c r="J6">
+        <v>0.24184900000000001</v>
+      </c>
+      <c r="K6">
+        <v>0.23368</v>
+      </c>
+      <c r="L6" s="14">
+        <f t="shared" si="0"/>
+        <v>0.2469874</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>5.2568341169376795E-2</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="2"/>
+        <v>0.21283814951441571</v>
+      </c>
+      <c r="O6" s="14">
+        <f t="shared" si="3"/>
+        <v>0.21883779999999997</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>1.3705977042882206E-2</v>
+      </c>
+      <c r="Q6" s="11">
+        <f t="shared" si="5"/>
+        <v>6.2630756856823677E-2</v>
+      </c>
+      <c r="R6" s="14">
+        <v>-2.8149600000000025E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>4.3759999999999997E-3</v>
+      </c>
+      <c r="C7">
+        <v>7.0219999999999996E-3</v>
+      </c>
+      <c r="D7">
+        <v>3.7650000000000001E-3</v>
+      </c>
+      <c r="E7">
+        <v>4.326E-3</v>
+      </c>
+      <c r="F7">
+        <v>3.8730000000000001E-3</v>
+      </c>
+      <c r="G7" s="14">
+        <v>3.7789999999999998E-3</v>
+      </c>
+      <c r="H7">
+        <v>4.2139999999999999E-3</v>
+      </c>
+      <c r="I7">
+        <v>3.8270000000000001E-3</v>
+      </c>
+      <c r="J7">
+        <v>4.2430000000000002E-3</v>
+      </c>
+      <c r="K7">
+        <v>3.725E-3</v>
+      </c>
+      <c r="L7" s="14">
+        <f t="shared" si="0"/>
+        <v>4.6724000000000002E-3</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>1.3407909232986319E-3</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="2"/>
+        <v>0.28695979010757466</v>
+      </c>
+      <c r="O7" s="14">
+        <f t="shared" si="3"/>
+        <v>4.0038000000000001E-3</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>2.4844456122041271E-4</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="5"/>
+        <v>6.2052190723915455E-2</v>
+      </c>
+      <c r="R7" s="14">
+        <v>-6.686000000000001E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>61</v>
+      </c>
+      <c r="B8">
+        <v>8.2308000000000006E-2</v>
+      </c>
+      <c r="C8">
+        <v>8.2173999999999997E-2</v>
+      </c>
+      <c r="D8">
+        <v>7.6700000000000004E-2</v>
+      </c>
+      <c r="E8">
+        <v>6.8422999999999998E-2</v>
+      </c>
+      <c r="F8">
+        <v>4.8003999999999998E-2</v>
+      </c>
+      <c r="G8" s="14">
+        <v>4.7253000000000003E-2</v>
+      </c>
+      <c r="H8">
+        <v>4.7164999999999999E-2</v>
+      </c>
+      <c r="I8">
+        <v>6.4308000000000004E-2</v>
+      </c>
+      <c r="J8">
+        <v>5.2380000000000003E-2</v>
+      </c>
+      <c r="K8">
+        <v>4.4886000000000002E-2</v>
+      </c>
+      <c r="L8" s="14">
+        <f t="shared" si="0"/>
+        <v>7.1521799999999996E-2</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>1.4311836961061314E-2</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="2"/>
+        <v>0.20010454100793484</v>
+      </c>
+      <c r="O8" s="14">
+        <f t="shared" si="3"/>
+        <v>5.5030599999999999E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>1.0454166169523086E-2</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="5"/>
+        <v>0.18997005610556827</v>
+      </c>
+      <c r="R8" s="14">
+        <v>-1.6491199999999998E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9">
+        <v>2.1540000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <v>4.2300000000000003E-3</v>
+      </c>
+      <c r="D9">
+        <v>1.9530000000000001E-3</v>
+      </c>
+      <c r="E9">
+        <v>2.2629999999999998E-3</v>
+      </c>
+      <c r="F9">
+        <v>1.954E-3</v>
+      </c>
+      <c r="G9" s="14">
+        <v>1.936E-3</v>
+      </c>
+      <c r="H9">
+        <v>1.8860000000000001E-3</v>
+      </c>
+      <c r="I9">
+        <v>1.885E-3</v>
+      </c>
+      <c r="J9">
+        <v>2.2529999999999998E-3</v>
+      </c>
+      <c r="K9">
+        <v>2.0470000000000002E-3</v>
+      </c>
+      <c r="L9" s="14">
+        <f t="shared" si="0"/>
+        <v>2.5107999999999997E-3</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>9.7024826719762909E-4</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="2"/>
+        <v>0.38642992958325206</v>
+      </c>
+      <c r="O9" s="14">
+        <f t="shared" si="3"/>
+        <v>1.9848000000000001E-3</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>1.5846671574813319E-4</v>
+      </c>
+      <c r="Q9" s="11">
+        <f t="shared" si="5"/>
+        <v>7.9840142960566893E-2</v>
+      </c>
+      <c r="R9" s="14">
+        <v>-5.2599999999999956E-4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>0.131187</v>
+      </c>
+      <c r="C10">
+        <v>0.21551400000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.15320800000000001</v>
+      </c>
+      <c r="E10">
+        <v>0.134462</v>
+      </c>
+      <c r="F10">
+        <v>0.15776599999999999</v>
+      </c>
+      <c r="G10" s="14">
+        <v>0.142016</v>
+      </c>
+      <c r="H10">
+        <v>0.140565</v>
+      </c>
+      <c r="I10">
+        <v>0.124282</v>
+      </c>
+      <c r="J10">
+        <v>0.19983100000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.122373</v>
+      </c>
+      <c r="L10" s="14">
+        <f t="shared" si="0"/>
+        <v>0.1584274</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>3.392248249760043E-2</v>
+      </c>
+      <c r="N10" s="11">
+        <f t="shared" si="2"/>
+        <v>0.21412004803209816</v>
+      </c>
+      <c r="O10" s="14">
+        <f t="shared" si="3"/>
+        <v>0.13981819999999998</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>1.2222662852259474E-2</v>
+      </c>
+      <c r="Q10" s="11">
+        <f t="shared" si="5"/>
+        <v>8.7418253505333901E-2</v>
+      </c>
+      <c r="R10" s="14">
+        <v>-1.860920000000002E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>8.6600000000000002E-4</v>
+      </c>
+      <c r="C11">
+        <v>1.126E-3</v>
+      </c>
+      <c r="D11">
+        <v>1.0449999999999999E-3</v>
+      </c>
+      <c r="E11">
+        <v>9.3499999999999996E-4</v>
+      </c>
+      <c r="F11">
+        <v>8.1800000000000004E-4</v>
+      </c>
+      <c r="G11" s="14">
+        <v>8.6300000000000005E-4</v>
+      </c>
+      <c r="H11">
+        <v>8.7699999999999996E-4</v>
+      </c>
+      <c r="I11">
+        <v>8.8199999999999997E-4</v>
+      </c>
+      <c r="J11">
+        <v>9.1E-4</v>
+      </c>
+      <c r="K11">
+        <v>9.3300000000000002E-4</v>
+      </c>
+      <c r="L11" s="14">
+        <f t="shared" si="0"/>
+        <v>9.5799999999999998E-4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>1.2687198272274365E-4</v>
+      </c>
+      <c r="N11" s="11">
+        <f t="shared" si="2"/>
+        <v>0.13243421996111029</v>
+      </c>
+      <c r="O11" s="14">
+        <f t="shared" si="3"/>
+        <v>8.7500000000000013E-4</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>4.1970227542864399E-5</v>
+      </c>
+      <c r="Q11" s="11">
+        <f t="shared" si="5"/>
+        <v>4.7965974334702163E-2</v>
+      </c>
+      <c r="R11" s="14">
+        <v>-8.2999999999999849E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>4.7499999999999999E-3</v>
+      </c>
+      <c r="C12">
+        <v>1.0744E-2</v>
+      </c>
+      <c r="D12">
+        <v>4.8840000000000003E-3</v>
+      </c>
+      <c r="E12">
+        <v>5.0109999999999998E-3</v>
+      </c>
+      <c r="F12">
+        <v>4.7590000000000002E-3</v>
+      </c>
+      <c r="G12" s="14">
+        <v>4.8430000000000001E-3</v>
+      </c>
+      <c r="H12">
+        <v>4.6100000000000004E-3</v>
+      </c>
+      <c r="I12">
+        <v>5.1659999999999996E-3</v>
+      </c>
+      <c r="J12">
+        <v>6.2249999999999996E-3</v>
+      </c>
+      <c r="K12">
+        <v>4.8710000000000003E-3</v>
+      </c>
+      <c r="L12" s="14">
+        <f t="shared" si="0"/>
+        <v>6.0296000000000004E-3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>2.6375800082651508E-3</v>
+      </c>
+      <c r="N12" s="11">
+        <f t="shared" si="2"/>
+        <v>0.43743863743285633</v>
+      </c>
+      <c r="O12" s="14">
+        <f t="shared" si="3"/>
+        <v>4.8777999999999998E-3</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>2.1670417624032191E-4</v>
+      </c>
+      <c r="Q12" s="11">
+        <f t="shared" si="5"/>
+        <v>4.442662188698223E-2</v>
+      </c>
+      <c r="R12" s="14">
+        <v>-1.1518000000000006E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2.6059999999999998E-3</v>
+      </c>
+      <c r="C13">
+        <v>3.3349999999999999E-3</v>
+      </c>
+      <c r="D13">
+        <v>3.0049999999999999E-3</v>
+      </c>
+      <c r="E13">
+        <v>2.9529999999999999E-3</v>
+      </c>
+      <c r="F13">
+        <v>2.7899999999999999E-3</v>
+      </c>
+      <c r="G13" s="14">
+        <v>2.7299999999999998E-3</v>
+      </c>
+      <c r="H13">
+        <v>2.771E-3</v>
+      </c>
+      <c r="I13">
+        <v>2.8549999999999999E-3</v>
+      </c>
+      <c r="J13">
+        <v>2.7560000000000002E-3</v>
+      </c>
+      <c r="K13">
+        <v>2.6129999999999999E-3</v>
+      </c>
+      <c r="L13" s="14">
+        <f t="shared" si="0"/>
+        <v>2.9378E-3</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>2.7131660472591704E-4</v>
+      </c>
+      <c r="N13" s="11">
+        <f t="shared" si="2"/>
+        <v>9.2353667617236387E-2</v>
+      </c>
+      <c r="O13" s="14">
+        <f t="shared" si="3"/>
+        <v>2.8197999999999999E-3</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>8.7055729277280274E-5</v>
+      </c>
+      <c r="Q13" s="11">
+        <f t="shared" si="5"/>
+        <v>3.0873015560422823E-2</v>
+      </c>
+      <c r="R13" s="14">
+        <v>-1.1800000000000005E-4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>1.586E-3</v>
+      </c>
+      <c r="C14">
+        <v>9.2029999999999994E-3</v>
+      </c>
+      <c r="D14">
+        <v>1.787E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.8090000000000001E-3</v>
+      </c>
+      <c r="F14">
+        <v>1.8060000000000001E-3</v>
+      </c>
+      <c r="G14" s="14">
+        <v>1.7639999999999999E-3</v>
+      </c>
+      <c r="H14">
+        <v>1.719E-3</v>
+      </c>
+      <c r="I14">
+        <v>1.5759999999999999E-3</v>
+      </c>
+      <c r="J14">
+        <v>1.704E-3</v>
+      </c>
+      <c r="K14">
+        <v>1.6670000000000001E-3</v>
+      </c>
+      <c r="L14" s="14">
+        <f t="shared" si="0"/>
+        <v>3.2382000000000001E-3</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>3.335730609626622E-3</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="2"/>
+        <v>1.0301187726596943</v>
+      </c>
+      <c r="O14" s="14">
+        <f t="shared" si="3"/>
+        <v>1.7347999999999999E-3</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>9.6040095793373012E-5</v>
+      </c>
+      <c r="Q14" s="11">
+        <f t="shared" si="5"/>
+        <v>5.5360903731480872E-2</v>
+      </c>
+      <c r="R14" s="14">
+        <v>-1.5034000000000002E-3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1.9009999999999999E-3</v>
+      </c>
+      <c r="C15">
+        <v>3.604E-3</v>
+      </c>
+      <c r="D15">
+        <v>1.823E-3</v>
+      </c>
+      <c r="E15">
+        <v>1.8829999999999999E-3</v>
+      </c>
+      <c r="F15">
+        <v>1.8060000000000001E-3</v>
+      </c>
+      <c r="G15" s="14">
+        <v>1.934E-3</v>
+      </c>
+      <c r="H15">
+        <v>1.8439999999999999E-3</v>
+      </c>
+      <c r="I15">
+        <v>1.9430000000000001E-3</v>
+      </c>
+      <c r="J15">
+        <v>1.8799999999999999E-3</v>
+      </c>
+      <c r="K15">
+        <v>1.789E-3</v>
+      </c>
+      <c r="L15" s="14">
+        <f t="shared" si="0"/>
+        <v>2.2033999999999999E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>7.8396638958567642E-4</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="2"/>
+        <v>0.35579848851124463</v>
+      </c>
+      <c r="O15" s="14">
+        <f t="shared" si="3"/>
+        <v>1.882E-3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>5.840804739075316E-5</v>
+      </c>
+      <c r="Q15" s="11">
+        <f t="shared" si="5"/>
+        <v>3.1035094256510711E-2</v>
+      </c>
+      <c r="R15" s="14">
+        <v>-3.213999999999999E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0.64971699999999999</v>
+      </c>
+      <c r="C16">
+        <v>0.95032899999999998</v>
+      </c>
+      <c r="D16">
+        <v>0.73780299999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.61542200000000002</v>
+      </c>
+      <c r="F16">
+        <v>0.60846999999999996</v>
+      </c>
+      <c r="G16" s="14">
+        <v>0.59009500000000004</v>
+      </c>
+      <c r="H16">
+        <v>0.57384800000000002</v>
+      </c>
+      <c r="I16">
+        <v>0.57799500000000004</v>
+      </c>
+      <c r="J16">
+        <v>0.66256300000000001</v>
+      </c>
+      <c r="K16">
+        <v>0.57065900000000003</v>
+      </c>
+      <c r="L16" s="14">
+        <f t="shared" si="0"/>
+        <v>0.71234819999999999</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>0.1426454029287304</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="2"/>
+        <v>0.20024673738030138</v>
+      </c>
+      <c r="O16" s="14">
+        <f t="shared" si="3"/>
+        <v>0.59316599999999997</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>1.8318824730315368E-2</v>
+      </c>
+      <c r="Q16" s="11">
+        <f t="shared" si="5"/>
+        <v>3.0883133440411905E-2</v>
+      </c>
+      <c r="R16" s="14">
+        <v>-0.11918220000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B3:B15)</f>
+        <v>0.47651399999999988</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:K17" si="6">SUM(C3:C15)</f>
+        <v>0.6919789999999999</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>0.47264</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
+        <v>0.48679400000000006</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>0.45875199999999994</v>
+      </c>
+      <c r="G17" s="14">
+        <f t="shared" si="6"/>
+        <v>0.45443099999999992</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>0.41880200000000006</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>0.42710399999999998</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>0.52495800000000004</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>0.428346</v>
+      </c>
+      <c r="L17" s="14">
+        <f t="shared" si="0"/>
+        <v>0.5173357999999999</v>
+      </c>
+      <c r="M17">
+        <f t="shared" si="1"/>
+        <v>9.8144338054724153E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" si="2"/>
+        <v>0.18971108911218626</v>
+      </c>
+      <c r="O17" s="14">
+        <f t="shared" si="3"/>
+        <v>0.44917660000000004</v>
+      </c>
+      <c r="P17">
+        <f t="shared" si="4"/>
+        <v>2.7130157496777843E-2</v>
+      </c>
+      <c r="Q17" s="11">
+        <f t="shared" si="5"/>
+        <v>6.0399757014897575E-2</v>
+      </c>
+      <c r="R17" s="14">
+        <f t="array" ref="R17">O17:O30-L17:L30</f>
+        <v>-6.8159199999999864E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f>B16-B17</f>
+        <v>0.17320300000000011</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:K18" si="7">C16-C17</f>
+        <v>0.25835000000000008</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="7"/>
+        <v>0.26516299999999998</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="7"/>
+        <v>0.12862799999999996</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="7"/>
+        <v>0.14971800000000002</v>
+      </c>
+      <c r="G18" s="14">
+        <f t="shared" si="7"/>
+        <v>0.13566400000000012</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="7"/>
+        <v>0.15504599999999996</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="7"/>
+        <v>0.15089100000000005</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="7"/>
+        <v>0.13760499999999998</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="7"/>
+        <v>0.14231300000000002</v>
+      </c>
+      <c r="L18" s="14">
+        <f t="shared" si="0"/>
+        <v>0.19501240000000003</v>
+      </c>
+      <c r="M18">
+        <f t="shared" si="1"/>
+        <v>6.2981901005765242E-2</v>
+      </c>
+      <c r="N18" s="11">
+        <f t="shared" si="2"/>
+        <v>0.32296357055123281</v>
+      </c>
+      <c r="O18" s="14">
+        <f t="shared" si="3"/>
+        <v>0.14398940000000002</v>
+      </c>
+      <c r="P18">
+        <f t="shared" si="4"/>
+        <v>1.1269230665843868E-2</v>
+      </c>
+      <c r="Q18" s="11">
+        <f t="shared" si="5"/>
+        <v>7.8264307413211429E-2</v>
+      </c>
+      <c r="R18" s="14">
+        <f t="array" ref="R18">O18:O31-L18:L31</f>
+        <v>-5.1023000000000013E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="B17" sqref="B17:K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="11" width="7.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" style="11" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="10" t="str">
+        <f>B1</f>
+        <v>for loop</v>
+      </c>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10" t="str">
+        <f>G1</f>
+        <v>.each loop</v>
+      </c>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
+        <f t="array" ref="G2:K2">B2:F2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M2" t="s">
+        <v>10</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="str">
+        <f t="array" ref="O2:Q2">L2:N2</f>
+        <v>Avg</v>
+      </c>
+      <c r="P2" t="str">
+        <v>StDev</v>
+      </c>
+      <c r="Q2" s="11" t="str">
+        <v>RelStdDev</v>
+      </c>
+      <c r="R2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3">
+        <v>5.3610000000000003E-3</v>
+      </c>
+      <c r="C3">
+        <v>5.731E-3</v>
+      </c>
+      <c r="D3">
+        <v>5.0509999999999999E-3</v>
+      </c>
+      <c r="E3">
+        <v>5.9129999999999999E-3</v>
+      </c>
+      <c r="F3">
+        <v>6.9189999999999998E-3</v>
+      </c>
+      <c r="G3">
+        <v>5.2180000000000004E-3</v>
+      </c>
+      <c r="H3">
+        <v>5.0699999999999999E-3</v>
+      </c>
+      <c r="I3">
+        <v>7.6099999999999996E-3</v>
+      </c>
+      <c r="J3">
+        <v>5.3990000000000002E-3</v>
+      </c>
+      <c r="K3">
+        <v>6.0400000000000002E-3</v>
+      </c>
+      <c r="L3">
+        <f>AVERAGE(B3:F3)</f>
+        <v>5.7949999999999998E-3</v>
+      </c>
+      <c r="M3">
+        <f>STDEVA(B3:F3)</f>
+        <v>7.1121164219942624E-4</v>
+      </c>
+      <c r="N3" s="11">
+        <f>M3/L3</f>
+        <v>0.12272849735969392</v>
+      </c>
+      <c r="O3">
+        <f>AVERAGE(E3:I3)</f>
+        <v>6.1460000000000004E-3</v>
+      </c>
+      <c r="P3">
+        <f>STDEVA(E3:I3)</f>
+        <v>1.0970499077070271E-3</v>
+      </c>
+      <c r="Q3" s="11">
+        <f>P3/O3</f>
+        <v>0.1784981952012735</v>
+      </c>
+      <c r="R3">
+        <f t="array" ref="R3:R16">O3:O16-L3:L16</f>
+        <v>3.5100000000000062E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>3.5630000000000002E-3</v>
+      </c>
+      <c r="C4">
+        <v>3.7069999999999998E-3</v>
+      </c>
+      <c r="D4">
+        <v>3.4550000000000002E-3</v>
+      </c>
+      <c r="E4">
+        <v>2.1857999999999999E-2</v>
+      </c>
+      <c r="F4">
+        <v>3.882E-3</v>
+      </c>
+      <c r="G4">
+        <v>3.264E-3</v>
+      </c>
+      <c r="H4">
+        <v>3.3080000000000002E-3</v>
+      </c>
+      <c r="I4">
+        <v>5.1739999999999998E-3</v>
+      </c>
+      <c r="J4">
+        <v>3.6099999999999999E-3</v>
+      </c>
+      <c r="K4">
+        <v>4.0889999999999998E-3</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:L16" si="0">AVERAGE(B4:F4)</f>
+        <v>7.2929999999999991E-3</v>
+      </c>
+      <c r="M4">
+        <f t="shared" ref="M4:M16" si="1">STDEVA(B4:F4)</f>
+        <v>8.14365836095793E-3</v>
+      </c>
+      <c r="N4" s="11">
+        <f t="shared" ref="N4:N16" si="2">M4/L4</f>
+        <v>1.1166403895458565</v>
+      </c>
+      <c r="O4">
+        <f t="shared" ref="O4:O16" si="3">AVERAGE(E4:I4)</f>
+        <v>7.4971999999999999E-3</v>
+      </c>
+      <c r="P4">
+        <f t="shared" ref="P4:P16" si="4">STDEVA(E4:I4)</f>
+        <v>8.0648757708969097E-3</v>
+      </c>
+      <c r="Q4" s="11">
+        <f t="shared" ref="Q4:Q16" si="5">P4/O4</f>
+        <v>1.0757183709780864</v>
+      </c>
+      <c r="R4">
+        <v>2.0420000000000074E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B5">
+        <v>0.27063799999999999</v>
+      </c>
+      <c r="C5">
+        <v>0.28170800000000001</v>
+      </c>
+      <c r="D5">
+        <v>0.22800799999999999</v>
+      </c>
+      <c r="E5">
+        <v>0.229348</v>
+      </c>
+      <c r="F5">
+        <v>0.371834</v>
+      </c>
+      <c r="G5">
+        <v>0.219108</v>
+      </c>
+      <c r="H5">
+        <v>0.20186899999999999</v>
+      </c>
+      <c r="I5">
+        <v>0.22290299999999999</v>
+      </c>
+      <c r="J5">
+        <v>0.206928</v>
+      </c>
+      <c r="K5">
+        <v>0.24981</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>0.27630719999999998</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="1"/>
+        <v>5.857614098931424E-2</v>
+      </c>
+      <c r="N5" s="11">
+        <f t="shared" si="2"/>
+        <v>0.21199643364094112</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="3"/>
+        <v>0.24901240000000002</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="4"/>
+        <v>6.9408767683196773E-2</v>
+      </c>
+      <c r="Q5" s="11">
+        <f t="shared" si="5"/>
+        <v>0.27873619017846807</v>
+      </c>
+      <c r="R5">
+        <v>-2.7294799999999952E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B6">
+        <v>4.0070000000000001E-3</v>
+      </c>
+      <c r="C6">
+        <v>4.5849999999999997E-3</v>
+      </c>
+      <c r="D6">
+        <v>3.565E-3</v>
+      </c>
+      <c r="E6">
+        <v>4.2640000000000004E-3</v>
+      </c>
+      <c r="F6">
+        <v>4.4400000000000004E-3</v>
+      </c>
+      <c r="G6">
+        <v>3.6600000000000001E-3</v>
+      </c>
+      <c r="H6">
+        <v>3.9490000000000003E-3</v>
+      </c>
+      <c r="I6">
+        <v>3.8570000000000002E-3</v>
+      </c>
+      <c r="J6">
+        <v>3.5130000000000001E-3</v>
+      </c>
+      <c r="K6">
+        <v>2.1189E-2</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>4.1721999999999992E-3</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="1"/>
+        <v>4.0203569493268569E-4</v>
+      </c>
+      <c r="N6" s="11">
+        <f t="shared" si="2"/>
+        <v>9.636059990716786E-2</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="3"/>
+        <v>4.0340000000000003E-3</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="4"/>
+        <v>3.1470859537038995E-4</v>
+      </c>
+      <c r="Q6" s="11">
+        <f t="shared" si="5"/>
+        <v>7.8014029591073356E-2</v>
+      </c>
+      <c r="R6">
+        <v>-1.3819999999999891E-4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7">
+        <v>4.6899000000000003E-2</v>
+      </c>
+      <c r="C7">
+        <v>5.1619999999999999E-2</v>
+      </c>
+      <c r="D7">
+        <v>4.5069999999999999E-2</v>
+      </c>
+      <c r="E7">
+        <v>5.2664999999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>5.7401000000000001E-2</v>
+      </c>
+      <c r="G7">
+        <v>4.5416999999999999E-2</v>
+      </c>
+      <c r="H7">
+        <v>4.6365000000000003E-2</v>
+      </c>
+      <c r="I7">
+        <v>5.0300999999999998E-2</v>
+      </c>
+      <c r="J7">
+        <v>4.6940999999999997E-2</v>
+      </c>
+      <c r="K7">
+        <v>5.1693000000000003E-2</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>5.0730999999999991E-2</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="1"/>
+        <v>4.8926148938988083E-3</v>
+      </c>
+      <c r="N7" s="11">
+        <f t="shared" si="2"/>
+        <v>9.6442311286960819E-2</v>
+      </c>
+      <c r="O7">
+        <f t="shared" si="3"/>
+        <v>5.042979999999999E-2</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="4"/>
+        <v>4.8800896713073576E-3</v>
+      </c>
+      <c r="Q7" s="11">
+        <f t="shared" si="5"/>
+        <v>9.6769958859788424E-2</v>
+      </c>
+      <c r="R7">
+        <v>-3.0120000000000147E-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8">
+        <v>2.0709999999999999E-3</v>
+      </c>
+      <c r="C8">
+        <v>2.421E-3</v>
+      </c>
+      <c r="D8">
+        <v>1.9589999999999998E-3</v>
+      </c>
+      <c r="E8">
+        <v>2.1619999999999999E-3</v>
+      </c>
+      <c r="F8">
+        <v>2.542E-3</v>
+      </c>
+      <c r="G8">
+        <v>1.42E-3</v>
+      </c>
+      <c r="H8">
+        <v>1.526E-3</v>
+      </c>
+      <c r="I8">
+        <v>1.787E-3</v>
+      </c>
+      <c r="J8">
+        <v>1.634E-3</v>
+      </c>
+      <c r="K8">
+        <v>1.438E-3</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>2.2309999999999995E-3</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="1"/>
+        <v>2.4349845995406494E-4</v>
+      </c>
+      <c r="N8" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10914319137340431</v>
+      </c>
+      <c r="O8">
+        <f t="shared" si="3"/>
+        <v>1.8874000000000002E-3</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="4"/>
+        <v>4.6450489771368293E-4</v>
+      </c>
+      <c r="Q8" s="11">
+        <f t="shared" si="5"/>
+        <v>0.24610834889990615</v>
+      </c>
+      <c r="R8">
+        <v>-3.4359999999999924E-4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9">
+        <v>0.124172</v>
+      </c>
+      <c r="C9">
+        <v>0.15309</v>
+      </c>
+      <c r="D9">
+        <v>0.116609</v>
+      </c>
+      <c r="E9">
+        <v>0.13301099999999999</v>
+      </c>
+      <c r="F9">
+        <v>0.162052</v>
+      </c>
+      <c r="G9">
+        <v>1.2520000000000001E-3</v>
+      </c>
+      <c r="H9">
+        <v>1.2780000000000001E-3</v>
+      </c>
+      <c r="I9">
+        <v>1.3669999999999999E-3</v>
+      </c>
+      <c r="J9">
+        <v>1.3780000000000001E-3</v>
+      </c>
+      <c r="K9">
+        <v>1.312E-3</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>0.13778680000000001</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="1"/>
+        <v>1.9233162238695905E-2</v>
+      </c>
+      <c r="N9" s="11">
+        <f t="shared" si="2"/>
+        <v>0.13958639172036727</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="3"/>
+        <v>5.9791999999999991E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="4"/>
+        <v>8.075027860942649E-2</v>
+      </c>
+      <c r="Q9" s="11">
+        <f t="shared" si="5"/>
+        <v>1.3505197787233494</v>
+      </c>
+      <c r="R9">
+        <v>-7.7994800000000031E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10">
+        <v>3.503E-3</v>
+      </c>
+      <c r="C10">
+        <v>3.4680000000000002E-3</v>
+      </c>
+      <c r="D10">
+        <v>3.2789999999999998E-3</v>
+      </c>
+      <c r="E10">
+        <v>3.441E-3</v>
+      </c>
+      <c r="F10">
+        <v>3.8089999999999999E-3</v>
+      </c>
+      <c r="G10">
+        <v>0.19350899999999999</v>
+      </c>
+      <c r="H10">
+        <v>0.15874099999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.172538</v>
+      </c>
+      <c r="J10">
+        <v>0.17712700000000001</v>
+      </c>
+      <c r="K10">
+        <v>0.201511</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="0"/>
+        <v>3.4999999999999996E-3</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="1"/>
+        <v>1.9289634522199107E-4</v>
+      </c>
+      <c r="N10" s="11">
+        <f t="shared" si="2"/>
+        <v>5.511324149199745E-2</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="3"/>
+        <v>0.1064076</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="4"/>
+        <v>9.4640453664381799E-2</v>
+      </c>
+      <c r="Q10" s="11">
+        <f t="shared" si="5"/>
+        <v>0.88941441837220081</v>
+      </c>
+      <c r="R10">
+        <v>0.1029076</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18">
+      <c r="A11" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11">
+        <v>1.0169999999999999E-3</v>
+      </c>
+      <c r="C11">
+        <v>9.0200000000000002E-4</v>
+      </c>
+      <c r="D11">
+        <v>8.8699999999999998E-4</v>
+      </c>
+      <c r="E11">
+        <v>8.8500000000000004E-4</v>
+      </c>
+      <c r="F11">
+        <v>1.029E-3</v>
+      </c>
+      <c r="G11">
+        <v>8.7399999999999999E-4</v>
+      </c>
+      <c r="H11">
+        <v>8.8800000000000001E-4</v>
+      </c>
+      <c r="I11">
+        <v>9.0700000000000004E-4</v>
+      </c>
+      <c r="J11">
+        <v>9.1E-4</v>
+      </c>
+      <c r="K11">
+        <v>7.9100000000000004E-4</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="0"/>
+        <v>9.4400000000000007E-4</v>
+      </c>
+      <c r="M11">
+        <f t="shared" si="1"/>
+        <v>7.2539644333286966E-5</v>
+      </c>
+      <c r="N11" s="11">
+        <f t="shared" si="2"/>
+        <v>7.6842843573397199E-2</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="3"/>
+        <v>9.1659999999999984E-4</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="4"/>
+        <v>6.3947634827257266E-5</v>
+      </c>
+      <c r="Q11" s="11">
+        <f t="shared" si="5"/>
+        <v>6.9766130075558888E-2</v>
+      </c>
+      <c r="R11">
+        <v>-2.7400000000000232E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>4.4000000000000003E-3</v>
+      </c>
+      <c r="C12">
+        <v>4.8469999999999997E-3</v>
+      </c>
+      <c r="D12">
+        <v>4.1669999999999997E-3</v>
+      </c>
+      <c r="E12">
+        <v>4.6810000000000003E-3</v>
+      </c>
+      <c r="F12">
+        <v>6.0610000000000004E-3</v>
+      </c>
+      <c r="G12">
+        <v>2.6480000000000002E-3</v>
+      </c>
+      <c r="H12">
+        <v>2.5170000000000001E-3</v>
+      </c>
+      <c r="I12">
+        <v>2.8240000000000001E-3</v>
+      </c>
+      <c r="J12">
+        <v>2.6129999999999999E-3</v>
+      </c>
+      <c r="K12">
+        <v>2.8600000000000001E-3</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="0"/>
+        <v>4.8311999999999999E-3</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>7.3524023284910031E-4</v>
+      </c>
+      <c r="N12" s="11">
+        <f t="shared" si="2"/>
+        <v>0.15218584054667583</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>3.7462000000000007E-3</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>1.5652139470372711E-3</v>
+      </c>
+      <c r="Q12" s="11">
+        <f t="shared" si="5"/>
+        <v>0.41781377049737622</v>
+      </c>
+      <c r="R12">
+        <v>-1.0849999999999992E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18">
+      <c r="A13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>2.532E-3</v>
+      </c>
+      <c r="C13">
+        <v>2.539E-3</v>
+      </c>
+      <c r="D13">
+        <v>2.562E-3</v>
+      </c>
+      <c r="E13">
+        <v>2.7469999999999999E-3</v>
+      </c>
+      <c r="F13">
+        <v>2.8519999999999999E-3</v>
+      </c>
+      <c r="G13">
+        <v>2.826E-3</v>
+      </c>
+      <c r="H13">
+        <v>2.4979999999999998E-3</v>
+      </c>
+      <c r="I13">
+        <v>2.5500000000000002E-3</v>
+      </c>
+      <c r="J13">
+        <v>2.7130000000000001E-3</v>
+      </c>
+      <c r="K13">
+        <v>3.1979999999999999E-3</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="0"/>
+        <v>2.6464000000000001E-3</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="1"/>
+        <v>1.4503206542002976E-4</v>
+      </c>
+      <c r="N13" s="11">
+        <f t="shared" si="2"/>
+        <v>5.4803531370930227E-2</v>
+      </c>
+      <c r="O13">
+        <f t="shared" si="3"/>
+        <v>2.6946000000000001E-3</v>
+      </c>
+      <c r="P13">
+        <f t="shared" si="4"/>
+        <v>1.6151408607300845E-4</v>
+      </c>
+      <c r="Q13" s="11">
+        <f t="shared" si="5"/>
+        <v>5.9939911702296608E-2</v>
+      </c>
+      <c r="R13">
+        <v>4.8199999999999979E-5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18">
+      <c r="A14" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>1.658E-3</v>
+      </c>
+      <c r="C14">
+        <v>1.8810000000000001E-3</v>
+      </c>
+      <c r="D14">
+        <v>1.8010000000000001E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.887E-3</v>
+      </c>
+      <c r="F14">
+        <v>1.751E-3</v>
+      </c>
+      <c r="G14">
+        <v>1.6639999999999999E-3</v>
+      </c>
+      <c r="H14">
+        <v>1.913E-3</v>
+      </c>
+      <c r="I14">
+        <v>1.6900000000000001E-3</v>
+      </c>
+      <c r="J14">
+        <v>1.766E-3</v>
+      </c>
+      <c r="K14">
+        <v>1.884E-3</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="0"/>
+        <v>1.7956000000000001E-3</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="1"/>
+        <v>9.5654586926084505E-5</v>
+      </c>
+      <c r="N14" s="11">
+        <f t="shared" si="2"/>
+        <v>5.32716567866365E-2</v>
+      </c>
+      <c r="O14">
+        <f t="shared" si="3"/>
+        <v>1.781E-3</v>
+      </c>
+      <c r="P14">
+        <f t="shared" si="4"/>
+        <v>1.1350110131624256E-4</v>
+      </c>
+      <c r="Q14" s="11">
+        <f t="shared" si="5"/>
+        <v>6.3728860929950906E-2</v>
+      </c>
+      <c r="R14">
+        <v>-1.460000000000003E-5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>1.8220000000000001E-3</v>
+      </c>
+      <c r="C15">
+        <v>1.8710000000000001E-3</v>
+      </c>
+      <c r="D15">
+        <v>1.848E-3</v>
+      </c>
+      <c r="E15">
+        <v>2.1429999999999999E-3</v>
+      </c>
+      <c r="F15">
+        <v>2.2620000000000001E-3</v>
+      </c>
+      <c r="G15">
+        <v>1.5280000000000001E-3</v>
+      </c>
+      <c r="H15">
+        <v>1.665E-3</v>
+      </c>
+      <c r="I15">
+        <v>1.6260000000000001E-3</v>
+      </c>
+      <c r="J15">
+        <v>1.3699999999999999E-3</v>
+      </c>
+      <c r="K15">
+        <v>1.6479999999999999E-3</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="0"/>
+        <v>1.9892E-3</v>
+      </c>
+      <c r="M15">
+        <f t="shared" si="1"/>
+        <v>1.9996174634164516E-4</v>
+      </c>
+      <c r="N15" s="11">
+        <f t="shared" si="2"/>
+        <v>0.10052370115707077</v>
+      </c>
+      <c r="O15">
+        <f t="shared" si="3"/>
+        <v>1.8448E-3</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="4"/>
+        <v>3.3299504500818071E-4</v>
+      </c>
+      <c r="Q15" s="11">
+        <f t="shared" si="5"/>
+        <v>0.18050468614927404</v>
+      </c>
+      <c r="R15">
+        <v>-1.4440000000000004E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>0.60263599999999995</v>
+      </c>
+      <c r="C16">
+        <v>0.65221099999999999</v>
+      </c>
+      <c r="D16">
+        <v>0.58568500000000001</v>
+      </c>
+      <c r="E16">
+        <v>0.63578100000000004</v>
+      </c>
+      <c r="F16">
+        <v>0.81640100000000004</v>
+      </c>
+      <c r="G16">
+        <v>0.63617199999999996</v>
+      </c>
+      <c r="H16">
+        <v>0.61492800000000003</v>
+      </c>
+      <c r="I16">
+        <v>0.64525399999999999</v>
+      </c>
+      <c r="J16">
+        <v>0.60635399999999995</v>
+      </c>
+      <c r="K16">
+        <v>0.67732800000000004</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="0"/>
+        <v>0.65854279999999998</v>
+      </c>
+      <c r="M16">
+        <f t="shared" si="1"/>
+        <v>9.2075012686397353E-2</v>
+      </c>
+      <c r="N16" s="11">
+        <f t="shared" si="2"/>
+        <v>0.1398162924055921</v>
+      </c>
+      <c r="O16">
+        <f t="shared" si="3"/>
+        <v>0.66970719999999995</v>
+      </c>
+      <c r="P16">
+        <f t="shared" si="4"/>
+        <v>8.275473911928008E-2</v>
+      </c>
+      <c r="Q16" s="11">
+        <f t="shared" si="5"/>
+        <v>0.12356853729402952</v>
+      </c>
+      <c r="R16">
+        <v>1.1164399999999963E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <f>SUM(B3:B15)</f>
+        <v>0.47164299999999992</v>
+      </c>
+      <c r="C17">
+        <f t="shared" ref="C17:K17" si="6">SUM(C3:C15)</f>
+        <v>0.51837</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="6"/>
+        <v>0.41826099999999999</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="6"/>
+        <v>0.46500500000000006</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="6"/>
+        <v>0.62683399999999978</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="6"/>
+        <v>0.48238799999999987</v>
+      </c>
+      <c r="H17">
+        <f t="shared" si="6"/>
+        <v>0.431587</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>0.475134</v>
+      </c>
+      <c r="J17">
+        <f t="shared" si="6"/>
+        <v>0.45590199999999997</v>
+      </c>
+      <c r="K17">
+        <f t="shared" si="6"/>
+        <v>0.54746300000000003</v>
+      </c>
+      <c r="L17">
+        <f t="shared" ref="L17" si="7">AVERAGE(B17:F17)</f>
+        <v>0.50002259999999998</v>
+      </c>
+      <c r="M17">
+        <f t="shared" ref="M17" si="8">STDEVA(B17:F17)</f>
+        <v>7.9269085236931713E-2</v>
+      </c>
+      <c r="N17" s="11">
+        <f t="shared" ref="N17" si="9">M17/L17</f>
+        <v>0.1585310048724432</v>
+      </c>
+      <c r="O17">
+        <f t="shared" ref="O17" si="10">AVERAGE(E17:I17)</f>
+        <v>0.49618959999999995</v>
+      </c>
+      <c r="P17">
+        <f t="shared" ref="P17" si="11">STDEVA(E17:I17)</f>
+        <v>7.5577372455649786E-2</v>
+      </c>
+      <c r="Q17" s="11">
+        <f t="shared" ref="Q17" si="12">P17/O17</f>
+        <v>0.15231551095720222</v>
+      </c>
+      <c r="R17">
+        <f t="array" ref="R17">O17:O30-L17:L30</f>
+        <v>-3.8330000000000308E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <f>B16-B17</f>
+        <v>0.13099300000000003</v>
+      </c>
+      <c r="C18">
+        <f t="shared" ref="C18:K18" si="13">C16-C17</f>
+        <v>0.13384099999999999</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="13"/>
+        <v>0.16742400000000002</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="13"/>
+        <v>0.17077599999999998</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="13"/>
+        <v>0.18956700000000026</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="13"/>
+        <v>0.15378400000000009</v>
+      </c>
+      <c r="H18">
+        <f t="shared" si="13"/>
+        <v>0.18334100000000003</v>
+      </c>
+      <c r="I18">
+        <f t="shared" si="13"/>
+        <v>0.17011999999999999</v>
+      </c>
+      <c r="J18">
+        <f t="shared" si="13"/>
+        <v>0.15045199999999997</v>
+      </c>
+      <c r="K18">
+        <f t="shared" si="13"/>
+        <v>0.12986500000000001</v>
+      </c>
+      <c r="L18">
+        <f t="shared" ref="L18" si="14">AVERAGE(B18:F18)</f>
+        <v>0.15852020000000006</v>
+      </c>
+      <c r="M18">
+        <f t="shared" ref="M18" si="15">STDEVA(B18:F18)</f>
+        <v>2.5299188380262138E-2</v>
+      </c>
+      <c r="N18" s="11">
+        <f t="shared" ref="N18" si="16">M18/L18</f>
+        <v>0.1595959907965176</v>
+      </c>
+      <c r="O18">
+        <f t="shared" ref="O18" si="17">AVERAGE(E18:I18)</f>
+        <v>0.17351760000000011</v>
+      </c>
+      <c r="P18">
+        <f t="shared" ref="P18" si="18">STDEVA(E18:I18)</f>
+        <v>1.3807221418518414E-2</v>
+      </c>
+      <c r="Q18" s="11">
+        <f t="shared" ref="Q18" si="19">P18/O18</f>
+        <v>7.9572455004670459E-2</v>
+      </c>
+      <c r="R18">
+        <f t="array" ref="R18">O18:O31-L18:L31</f>
+        <v>1.499740000000005E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1548,16 +4859,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1712,7 +5023,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -1745,10 +5056,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -1757,7 +5068,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="3"/>
       <c r="I1" s="8" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -1766,7 +5077,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -1775,22 +5086,22 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="E2" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>53</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -1833,7 +5144,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1876,7 +5187,7 @@
         <v>1.3500742000000001</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="Q3" t="e">
         <f>B3-I3</f>
@@ -1905,7 +5216,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1948,7 +5259,7 @@
         <v>0.13967913309510532</v>
       </c>
       <c r="P4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="Q4" s="5" t="e">
         <f>Q3*1000</f>
@@ -1974,7 +5285,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2182,7 +5493,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -2215,10 +5526,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2227,7 +5538,7 @@
       <c r="G1" s="7"/>
       <c r="H1" s="3"/>
       <c r="I1" s="6" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
       <c r="J1" s="6"/>
       <c r="K1" s="6"/>
@@ -2236,7 +5547,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -2245,25 +5556,25 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
-        <v>32</v>
-      </c>
       <c r="E2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="F2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="G2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -2306,7 +5617,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2355,7 +5666,7 @@
         <v>106.7</v>
       </c>
       <c r="P3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="Q3">
         <f>B3-I3</f>
@@ -2384,7 +5695,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2427,7 +5738,7 @@
         <v>0.33879452626806195</v>
       </c>
       <c r="P4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="5">
         <f>Q3*1000</f>
@@ -2453,7 +5764,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2706,7 +6017,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R17"/>
   <sheetViews>
@@ -2734,10 +6045,10 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2745,7 +6056,7 @@
       <c r="F1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" s="6" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
@@ -2753,7 +6064,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="6" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
       <c r="O1" s="6"/>
       <c r="P1" s="6"/>
@@ -2762,22 +6073,22 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="D2" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F2" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="H2" s="2" t="str">
         <f t="array" ref="H2:K2">B2:F2</f>
@@ -2808,7 +6119,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2851,7 +6162,7 @@
         <v>69.7</v>
       </c>
       <c r="N3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="O3">
         <f>B3-H3</f>
@@ -2872,7 +6183,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2907,7 +6218,7 @@
         <v>9.4835850044695941E-2</v>
       </c>
       <c r="N4" t="s">
-        <v>36</v>
+        <v>43</v>
       </c>
       <c r="O4" s="5">
         <f>O3*1000</f>
@@ -2928,7 +6239,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -3149,7 +6460,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -3169,45 +6480,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="7" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C1" s="7"/>
       <c r="D1" s="3"/>
       <c r="E1" s="7" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="F1" s="7"/>
       <c r="G1" s="3"/>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="F2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="I2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -3222,12 +6533,12 @@
         <v>1.3408000000000531E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -3246,12 +6557,12 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -3328,6 +6639,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
@@ -3342,7 +6654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -3358,26 +6670,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>23</v>
+        <v>30</v>
       </c>
       <c r="D1" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -3390,7 +6702,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -3403,7 +6715,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -3486,276 +6798,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <f>AVERAGE(B6:B32)</f>
-        <v>0.44118779999999946</v>
-      </c>
-      <c r="D3">
-        <f>AVERAGE(D6:D32)</f>
-        <v>0.45040099999999939</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <f>STDEVA(B6:B32)</f>
-        <v>2.1336102659575439E-2</v>
-      </c>
-      <c r="D4">
-        <f>STDEVA(D6:D32)</f>
-        <v>3.2935379806523481E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1">
-        <f>B4/B3</f>
-        <v>4.8360590795066105E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <f>D4/D3</f>
-        <v>7.3124570785863097E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>0.42475299999999999</v>
-      </c>
-      <c r="D6">
-        <v>0.39991199999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>0.438661999999999</v>
-      </c>
-      <c r="D7">
-        <v>0.45086799999999899</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>0.446709999999999</v>
-      </c>
-      <c r="D8">
-        <v>0.484957999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>0.42122699999999902</v>
-      </c>
-      <c r="D9">
-        <v>0.44270900000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>0.47458699999999998</v>
-      </c>
-      <c r="D10">
-        <v>0.47355799999999898</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" width="23.7109375" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3">
-        <f>AVERAGE(B6:B32)</f>
-        <v>0.24570099999999978</v>
-      </c>
-      <c r="D3">
-        <f>AVERAGE(D6:D32)</f>
-        <v>0.3320297999999996</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4">
-        <f>STDEVA(B6:B32)</f>
-        <v>2.0237555966569346E-2</v>
-      </c>
-      <c r="D4">
-        <f>STDEVA(D6:D32)</f>
-        <v>3.7396661477998347E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1">
-        <f>B4/B3</f>
-        <v>8.2366599918475558E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <f>D4/D3</f>
-        <v>0.11263043702100954</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>0.275005</v>
-      </c>
-      <c r="D6">
-        <v>0.32842199999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>0.23533599999999999</v>
-      </c>
-      <c r="D7">
-        <v>0.37503599999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>0.224244999999999</v>
-      </c>
-      <c r="D8">
-        <v>0.27442299999999997</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>0.23674799999999999</v>
-      </c>
-      <c r="D9">
-        <v>0.35225099999999898</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>0.25717099999999998</v>
-      </c>
-      <c r="D10">
-        <v>0.33001699999999901</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>

</xml_diff>

<commit_message>
Tested how much quicker home page loading would be if make home_static.erb (so no computation required to created home page). About 200 ms; page computation took ~450 ms so this shows cutting computation by n ms doesn't cut onload time by as many as n ms.
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,23 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25520" yWindow="16580" windowWidth="25600" windowHeight="14620" tabRatio="843"/>
+    <workbookView xWindow="25540" yWindow="16660" windowWidth="25600" windowHeight="14620" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="storing properties" sheetId="15" r:id="rId1"/>
-    <sheet name="pt_main loop type" sheetId="14" r:id="rId2"/>
-    <sheet name="storing element.group" sheetId="13" r:id="rId3"/>
-    <sheet name="if else pos neg" sheetId="12" r:id="rId4"/>
-    <sheet name="for vs .each" sheetId="11" r:id="rId5"/>
-    <sheet name="@timing framework" sheetId="10" r:id="rId6"/>
-    <sheet name="@orbital_hash" sheetId="9" r:id="rId7"/>
-    <sheet name="term_spans" sheetId="8" r:id="rId8"/>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId9"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId10"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId11"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId12"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId13"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId14"/>
+    <sheet name="home_static" sheetId="16" r:id="rId1"/>
+    <sheet name="storing properties" sheetId="15" r:id="rId2"/>
+    <sheet name="pt_main loop type" sheetId="14" r:id="rId3"/>
+    <sheet name="storing element.group" sheetId="13" r:id="rId4"/>
+    <sheet name="if else pos neg" sheetId="12" r:id="rId5"/>
+    <sheet name="for vs .each" sheetId="11" r:id="rId6"/>
+    <sheet name="@timing framework" sheetId="10" r:id="rId7"/>
+    <sheet name="@orbital_hash" sheetId="9" r:id="rId8"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId9"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId10"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId11"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId12"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId13"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId14"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId15"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -32,7 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="74">
+  <si>
+    <t>computing home.erb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>using home_static.erb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
   <si>
     <t>pt_econfig_this_orbital</t>
   </si>
@@ -385,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -424,6 +433,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -960,7 +970,7 @@
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -978,17 +988,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>71</v>
+        <v>1</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -996,23 +1006,23 @@
       <c r="K1" s="16"/>
       <c r="L1" s="17" t="str">
         <f>B1</f>
-        <v>creating properties each time</v>
+        <v>computing home.erb</v>
       </c>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
       <c r="O1" s="18" t="str">
         <f>G1</f>
-        <v>storing properties</v>
+        <v>using home_static.erb</v>
       </c>
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1046,13 +1056,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -1065,70 +1075,70 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="B3">
-        <v>0.52637100000000003</v>
+        <v>1.81</v>
       </c>
       <c r="C3">
-        <v>0.52769900000000003</v>
+        <v>1.78</v>
       </c>
       <c r="D3">
-        <v>0.48954900000000001</v>
+        <v>1.83</v>
       </c>
       <c r="E3">
-        <v>0.502965</v>
+        <v>1.9</v>
       </c>
       <c r="F3">
-        <v>0.59748599999999996</v>
+        <v>2.21</v>
       </c>
       <c r="G3" s="8">
-        <v>0.33057700000000001</v>
-      </c>
-      <c r="H3">
-        <v>0.33275300000000002</v>
-      </c>
-      <c r="I3">
-        <v>0.30465599999999998</v>
-      </c>
-      <c r="J3">
-        <v>0.310811</v>
-      </c>
-      <c r="K3">
-        <v>0.32437100000000002</v>
+        <v>1.34</v>
+      </c>
+      <c r="H3" s="22">
+        <v>1.52</v>
+      </c>
+      <c r="I3" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="J3" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="K3" s="22">
+        <v>1.31</v>
       </c>
       <c r="L3" s="8">
-        <f>AVERAGE(B3:F3)</f>
-        <v>0.52881400000000001</v>
+        <f>AVERAGE(B3:K3)</f>
+        <v>1.6620000000000001</v>
       </c>
       <c r="M3">
         <f>STDEVA(B3:F3)</f>
-        <v>4.163221734426311E-2</v>
+        <v>0.17558473737770897</v>
       </c>
       <c r="N3" s="7">
         <f>M3/L3</f>
-        <v>7.8727524884483216E-2</v>
+        <v>0.10564665305517987</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" ref="O3:O20" si="0">AVERAGE(G3:K3)</f>
-        <v>0.32063359999999996</v>
+        <v>1.4179999999999999</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P20" si="1">STDEVA(G3:K3)</f>
-        <v>1.2364125436116804E-2</v>
+        <v>8.8994381845150045E-2</v>
       </c>
       <c r="Q3" s="7">
         <f>P3/O3</f>
-        <v>3.8561540138391005E-2</v>
+        <v>6.276049495426661E-2</v>
       </c>
       <c r="R3" s="8">
         <f>O3-L3</f>
-        <v>-0.20818040000000004</v>
+        <v>-0.24400000000000022</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="13" customFormat="1">
@@ -1181,6 +1191,449 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R17"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.85546875" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.85546875" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" customWidth="1"/>
+    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="5.85546875" customWidth="1"/>
+    <col min="13" max="13" width="2.85546875" customWidth="1"/>
+    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.5703125" customWidth="1"/>
+    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="20"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>46</v>
+      </c>
+      <c r="H2" s="2" t="str">
+        <f t="array" ref="H2:K2">B2:F2</f>
+        <v>@terms</v>
+      </c>
+      <c r="I2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="J2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="K2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="O2" s="2" t="str">
+        <f t="array" ref="O2:R2">B2:F2</f>
+        <v>@terms</v>
+      </c>
+      <c r="P2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="Q2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="R2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.45378159999999956</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:L3" si="0">AVERAGE(C6:C32)</f>
+        <v>1.1975714</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>2.5720000000000001</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3" si="1">AVERAGE(E6:E32)</f>
+        <v>1.3744286000000001</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>134.80000000000001</v>
+      </c>
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>0.43725959999999964</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>1.1572868000000001</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>2.4740000000000002</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3" si="2">AVERAGE(K6:K32)</f>
+        <v>1.3167132000000001</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>69.7</v>
+      </c>
+      <c r="N3" t="s">
+        <v>41</v>
+      </c>
+      <c r="O3">
+        <f>B3-H3</f>
+        <v>1.6521999999999926E-2</v>
+      </c>
+      <c r="P3">
+        <f>C3-I3</f>
+        <v>4.0284599999999893E-2</v>
+      </c>
+      <c r="Q3">
+        <f>D3-J3</f>
+        <v>9.7999999999999865E-2</v>
+      </c>
+      <c r="R3">
+        <f>E3-K3</f>
+        <v>5.7715399999999972E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>2.0870108895260892E-2</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:J4" si="3">STDEVA(C6:C32)</f>
+        <v>4.3157184561784891E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="3"/>
+        <v>6.8337398253059706E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4" si="4">STDEVA(E6:E32)</f>
+        <v>2.7504719218717954E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" si="3"/>
+        <v>2.5346738297066202E-2</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>3.5277761461013364E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.11458621208504334</v>
+      </c>
+      <c r="K4">
+        <f t="shared" ref="K4" si="5">STDEVA(K6:K32)</f>
+        <v>9.4835850044695941E-2</v>
+      </c>
+      <c r="N4" t="s">
+        <v>48</v>
+      </c>
+      <c r="O4" s="5">
+        <f>O3*1000</f>
+        <v>16.521999999999927</v>
+      </c>
+      <c r="P4" s="5">
+        <f t="shared" ref="P4:R4" si="6">P3*1000</f>
+        <v>40.284599999999891</v>
+      </c>
+      <c r="Q4" s="5">
+        <f t="shared" si="6"/>
+        <v>97.999999999999858</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" si="6"/>
+        <v>57.715399999999974</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18">
+      <c r="A5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>4.5991527411558583E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <f t="shared" ref="C5:K5" si="7">C4/C3</f>
+        <v>3.6037253863765363E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" si="7"/>
+        <v>2.656975048719273E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="7"/>
+        <v>2.0011748313966946E-2</v>
+      </c>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1">
+        <f t="shared" si="7"/>
+        <v>5.7967253999834933E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <f t="shared" si="7"/>
+        <v>3.0483162394156195E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="7"/>
+        <v>4.6316173033566423E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="7"/>
+        <v>7.2024682402132778E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.43260199999999999</v>
+      </c>
+      <c r="C6">
+        <v>1.2069000000000001</v>
+      </c>
+      <c r="D6">
+        <v>2.59</v>
+      </c>
+      <c r="E6">
+        <f>D6-C6</f>
+        <v>1.3830999999999998</v>
+      </c>
+      <c r="F6">
+        <v>134.80000000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.44712800000000003</v>
+      </c>
+      <c r="I6">
+        <v>1.1972499999999999</v>
+      </c>
+      <c r="J6">
+        <v>2.67</v>
+      </c>
+      <c r="K6">
+        <f>J6-I6</f>
+        <v>1.47275</v>
+      </c>
+      <c r="L6">
+        <v>69.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.46669099999999902</v>
+      </c>
+      <c r="C7">
+        <v>1.2588010000000001</v>
+      </c>
+      <c r="D7">
+        <v>2.66</v>
+      </c>
+      <c r="E7">
+        <f t="shared" ref="E7:E10" si="8">D7-C7</f>
+        <v>1.4011990000000001</v>
+      </c>
+      <c r="H7">
+        <v>0.440271999999999</v>
+      </c>
+      <c r="I7">
+        <v>1.1428370000000001</v>
+      </c>
+      <c r="J7">
+        <v>2.37</v>
+      </c>
+      <c r="K7">
+        <f t="shared" ref="K7:K10" si="9">J7-I7</f>
+        <v>1.227163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.44835399999999997</v>
+      </c>
+      <c r="C8">
+        <v>1.138239</v>
+      </c>
+      <c r="D8">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="8"/>
+        <v>1.3317610000000002</v>
+      </c>
+      <c r="H8">
+        <v>0.44775199999999898</v>
+      </c>
+      <c r="I8">
+        <v>1.18065</v>
+      </c>
+      <c r="J8">
+        <v>2.44</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="9"/>
+        <v>1.25935</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.43822799999999901</v>
+      </c>
+      <c r="C9">
+        <v>1.1958789999999999</v>
+      </c>
+      <c r="D9">
+        <v>2.56</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="8"/>
+        <v>1.3641210000000001</v>
+      </c>
+      <c r="H9">
+        <v>0.39332299999999998</v>
+      </c>
+      <c r="I9">
+        <v>1.1060909999999999</v>
+      </c>
+      <c r="J9">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="9"/>
+        <v>1.3239090000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.48303299999999999</v>
+      </c>
+      <c r="C10">
+        <v>1.1880379999999999</v>
+      </c>
+      <c r="D10">
+        <v>2.58</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="8"/>
+        <v>1.3919620000000001</v>
+      </c>
+      <c r="H10">
+        <v>0.45782299999999998</v>
+      </c>
+      <c r="I10">
+        <v>1.1596059999999999</v>
+      </c>
+      <c r="J10">
+        <v>2.46</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="9"/>
+        <v>1.300394</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="N1:R1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="H1:K1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
@@ -1199,45 +1652,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="3"/>
       <c r="E1" s="20" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="3"/>
       <c r="H1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="I2" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1252,12 +1705,12 @@
         <v>1.3408000000000531E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1276,12 +1729,12 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1358,6 +1811,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
@@ -1372,7 +1826,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1388,26 +1842,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1420,7 +1874,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1433,7 +1887,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1516,6 +1970,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1526,7 +1981,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1542,26 +1997,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="D1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1574,7 +2029,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1587,7 +2042,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1654,6 +2109,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1664,7 +2120,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1680,20 +2136,20 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1706,7 +2162,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1719,7 +2175,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1786,6 +2242,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1796,7 +2253,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -1813,32 +2270,32 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1859,7 +2316,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1880,7 +2337,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1985,6 +2442,7 @@
       </c>
     </row>
   </sheetData>
+  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1996,6 +2454,233 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="N4" sqref="N4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="8" customWidth="1"/>
+    <col min="8" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="8"/>
+    <col min="14" max="14" width="8.5703125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="8"/>
+    <col min="17" max="17" width="8.5703125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="str">
+        <f>B1</f>
+        <v>creating properties each time</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18" t="str">
+        <f>G1</f>
+        <v>storing properties</v>
+      </c>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="array" ref="G2:K2">B2:F2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="8" t="str">
+        <f t="array" ref="O2:Q2">L2:N2</f>
+        <v>Avg</v>
+      </c>
+      <c r="P2" t="str">
+        <v>StDev</v>
+      </c>
+      <c r="Q2" s="7" t="str">
+        <v>RelStdDev</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3">
+        <v>0.52637100000000003</v>
+      </c>
+      <c r="C3">
+        <v>0.52769900000000003</v>
+      </c>
+      <c r="D3">
+        <v>0.48954900000000001</v>
+      </c>
+      <c r="E3">
+        <v>0.502965</v>
+      </c>
+      <c r="F3">
+        <v>0.59748599999999996</v>
+      </c>
+      <c r="G3" s="8">
+        <v>0.33057700000000001</v>
+      </c>
+      <c r="H3">
+        <v>0.33275300000000002</v>
+      </c>
+      <c r="I3">
+        <v>0.30465599999999998</v>
+      </c>
+      <c r="J3">
+        <v>0.310811</v>
+      </c>
+      <c r="K3">
+        <v>0.32437100000000002</v>
+      </c>
+      <c r="L3" s="8">
+        <f>AVERAGE(B3:F3)</f>
+        <v>0.52881400000000001</v>
+      </c>
+      <c r="M3">
+        <f>STDEVA(B3:F3)</f>
+        <v>4.163221734426311E-2</v>
+      </c>
+      <c r="N3" s="7">
+        <f>M3/L3</f>
+        <v>7.8727524884483216E-2</v>
+      </c>
+      <c r="O3" s="8">
+        <f t="shared" ref="O3:O20" si="0">AVERAGE(G3:K3)</f>
+        <v>0.32063359999999996</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P20" si="1">STDEVA(G3:K3)</f>
+        <v>1.2364125436116804E-2</v>
+      </c>
+      <c r="Q3" s="7">
+        <f>P3/O3</f>
+        <v>3.8561540138391005E-2</v>
+      </c>
+      <c r="R3" s="8">
+        <f>O3-L3</f>
+        <v>-0.20818040000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="13" customFormat="1">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18" s="8"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18" s="8"/>
+      <c r="M18"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="8"/>
+      <c r="P18"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="8"/>
+    </row>
+    <row r="19" spans="1:18" ht="14" thickBot="1">
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:18" s="9" customFormat="1">
+      <c r="G20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="11"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R21"/>
   <sheetViews>
@@ -2021,17 +2706,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -2050,12 +2735,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2089,13 +2774,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -2108,12 +2793,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B3">
         <v>1.1590000000000001E-3</v>
@@ -2161,7 +2846,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>9.4499999999999998E-4</v>
@@ -2209,7 +2894,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B5">
         <v>6.3940000000000004E-3</v>
@@ -2257,7 +2942,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B6">
         <v>5.9379999999999997E-3</v>
@@ -2305,7 +2990,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B7">
         <v>2.4650000000000002E-3</v>
@@ -2353,7 +3038,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B8">
         <v>0.23839399999999999</v>
@@ -2401,7 +3086,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B9">
         <v>2.5820000000000001E-3</v>
@@ -2449,7 +3134,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B10">
         <v>5.2374999999999998E-2</v>
@@ -2497,7 +3182,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B11">
         <v>2.2130000000000001E-3</v>
@@ -2545,7 +3230,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B12">
         <v>0.16836200000000001</v>
@@ -2593,7 +3278,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B13">
         <v>8.6200000000000003E-4</v>
@@ -2641,7 +3326,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B14">
         <v>5.5449999999999996E-3</v>
@@ -2689,7 +3374,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B15">
         <v>3.1979999999999999E-3</v>
@@ -2737,7 +3422,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B16">
         <v>1.769E-3</v>
@@ -2785,7 +3470,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B17">
         <v>1.993E-3</v>
@@ -2833,7 +3518,7 @@
     </row>
     <row r="18" spans="1:18" s="13" customFormat="1">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B18">
         <v>0.49546000000000001</v>
@@ -2886,7 +3571,7 @@
     </row>
     <row r="19" spans="1:18" ht="14" thickBot="1">
       <c r="A19" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B19">
         <v>0.67658300000000005</v>
@@ -2935,7 +3620,7 @@
     </row>
     <row r="20" spans="1:18" s="9" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B20" s="9">
         <f>SUM(B3:B18)</f>
@@ -3008,7 +3693,7 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B21">
         <f>B19-B18</f>
@@ -3096,7 +3781,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -3122,17 +3807,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -3151,12 +3836,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3190,13 +3875,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -3209,12 +3894,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3" s="8">
         <v>8.8199999999999997E-4</v>
@@ -3277,7 +3962,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4" s="8">
         <v>5.5449999999999996E-3</v>
@@ -3339,7 +4024,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B5" s="8">
         <v>3.5990000000000002E-3</v>
@@ -3401,7 +4086,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6" s="8">
         <v>0.237287</v>
@@ -3463,7 +4148,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7" s="8">
         <v>3.7789999999999998E-3</v>
@@ -3525,7 +4210,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B8" s="8">
         <v>4.7253000000000003E-2</v>
@@ -3587,7 +4272,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9" s="8">
         <v>1.936E-3</v>
@@ -3649,7 +4334,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10" s="8">
         <v>0.142016</v>
@@ -3711,7 +4396,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B11" s="8">
         <v>8.6300000000000005E-4</v>
@@ -3773,7 +4458,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12" s="8">
         <v>4.8430000000000001E-3</v>
@@ -3835,7 +4520,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13" s="8">
         <v>2.7299999999999998E-3</v>
@@ -3897,7 +4582,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14" s="8">
         <v>1.7639999999999999E-3</v>
@@ -3959,7 +4644,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15" s="8">
         <v>1.934E-3</v>
@@ -4021,7 +4706,7 @@
     </row>
     <row r="16" spans="1:18" ht="14" thickBot="1">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16" s="8">
         <v>0.59009500000000004</v>
@@ -4083,7 +4768,7 @@
     </row>
     <row r="17" spans="1:18" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9">
         <f>SUM(B3:B15)</f>
@@ -4156,7 +4841,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <f>B16-B17</f>
@@ -4228,7 +4913,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -4245,7 +4929,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -4271,17 +4955,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -4300,12 +4984,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4339,13 +5023,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -4358,12 +5042,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B3">
         <v>7.2000000000000005E-4</v>
@@ -4426,7 +5110,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B4">
         <v>5.7739999999999996E-3</v>
@@ -4488,7 +5172,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B5">
         <v>3.506E-3</v>
@@ -4550,7 +5234,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B6">
         <v>0.23477999999999999</v>
@@ -4612,7 +5296,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>4.3759999999999997E-3</v>
@@ -4674,7 +5358,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>8.2308000000000006E-2</v>
@@ -4736,7 +5420,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9">
         <v>2.1540000000000001E-3</v>
@@ -4798,7 +5482,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>0.131187</v>
@@ -4860,7 +5544,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>8.6600000000000002E-4</v>
@@ -4922,7 +5606,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>4.7499999999999999E-3</v>
@@ -4984,7 +5668,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>2.6059999999999998E-3</v>
@@ -5046,7 +5730,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>1.586E-3</v>
@@ -5108,7 +5792,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>1.9009999999999999E-3</v>
@@ -5170,7 +5854,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>0.64971699999999999</v>
@@ -5232,7 +5916,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <f>SUM(B3:B15)</f>
@@ -5305,7 +5989,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <f>B16-B17</f>
@@ -5377,7 +6061,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -5394,7 +6077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -5415,17 +6098,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="14" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -5444,12 +6127,12 @@
       <c r="P1" s="19"/>
       <c r="Q1" s="19"/>
       <c r="R1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5483,13 +6166,13 @@
         <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="M2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="O2" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -5502,12 +6185,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B3">
         <v>5.3610000000000003E-3</v>
@@ -5570,7 +6253,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B4">
         <v>3.5630000000000002E-3</v>
@@ -5632,7 +6315,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>0.27063799999999999</v>
@@ -5694,7 +6377,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B6">
         <v>4.0070000000000001E-3</v>
@@ -5756,7 +6439,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B7">
         <v>4.6899000000000003E-2</v>
@@ -5818,7 +6501,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B8">
         <v>2.0709999999999999E-3</v>
@@ -5880,7 +6563,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B9">
         <v>0.124172</v>
@@ -5942,7 +6625,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B10">
         <v>3.503E-3</v>
@@ -6004,7 +6687,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B11">
         <v>1.0169999999999999E-3</v>
@@ -6066,7 +6749,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B12">
         <v>4.4000000000000003E-3</v>
@@ -6128,7 +6811,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B13">
         <v>2.532E-3</v>
@@ -6190,7 +6873,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>1.658E-3</v>
@@ -6252,7 +6935,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>1.8220000000000001E-3</v>
@@ -6314,7 +6997,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>0.60263599999999995</v>
@@ -6376,7 +7059,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17">
         <f>SUM(B3:B15)</f>
@@ -6449,7 +7132,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18">
         <f>B16-B17</f>
@@ -6521,7 +7204,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="4">
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="G1:K1"/>
@@ -6538,7 +7220,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -6554,16 +7236,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="D1" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -6707,7 +7389,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -6718,7 +7399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -6751,10 +7432,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -6763,7 +7444,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="3"/>
       <c r="I1" s="21" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
@@ -6772,7 +7453,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="14"/>
       <c r="R1" s="14"/>
@@ -6781,22 +7462,22 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="D2" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -6839,7 +7520,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -6882,7 +7563,7 @@
         <v>1.3500742000000001</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q3" t="e">
         <f>B3-I3</f>
@@ -6911,7 +7592,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -6954,7 +7635,7 @@
         <v>0.13967913309510532</v>
       </c>
       <c r="P4" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Q4" s="5" t="e">
         <f>Q3*1000</f>
@@ -6980,7 +7661,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -7172,7 +7853,6 @@
       <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:L1"/>
@@ -7188,7 +7868,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -7221,10 +7901,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -7233,7 +7913,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="3"/>
       <c r="I1" s="14" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
@@ -7242,7 +7922,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="Q1" s="14"/>
       <c r="R1" s="14"/>
@@ -7251,25 +7931,25 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="D2" t="s">
-        <v>42</v>
-      </c>
-      <c r="E2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" t="s">
-        <v>47</v>
-      </c>
       <c r="G2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -7312,7 +7992,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -7361,7 +8041,7 @@
         <v>106.7</v>
       </c>
       <c r="P3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="Q3">
         <f>B3-I3</f>
@@ -7390,7 +8070,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -7433,7 +8113,7 @@
         <v>0.33879452626806195</v>
       </c>
       <c r="P4" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="Q4" s="5">
         <f>Q3*1000</f>
@@ -7459,7 +8139,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -7696,7 +8376,6 @@
       <c r="A17" s="4"/>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="3">
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="I1:L1"/>
@@ -7710,448 +8389,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:R17"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
-    <col min="4" max="4" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.85546875" customWidth="1"/>
-    <col min="6" max="6" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="4.85546875" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="5.85546875" customWidth="1"/>
-    <col min="13" max="13" width="2.85546875" customWidth="1"/>
-    <col min="14" max="14" width="3.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="8.5703125" customWidth="1"/>
-    <col min="16" max="16" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:18">
-      <c r="A1" t="s">
-        <v>45</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="O1" s="14"/>
-      <c r="P1" s="14"/>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-    </row>
-    <row r="2" spans="1:18">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="2" t="str">
-        <f t="array" ref="H2:K2">B2:F2</f>
-        <v>@terms</v>
-      </c>
-      <c r="I2" t="str">
-        <v>total Sinatra time</v>
-      </c>
-      <c r="J2" t="str">
-        <v>onload</v>
-      </c>
-      <c r="K2" t="str">
-        <v>non-Sinatra</v>
-      </c>
-      <c r="O2" s="2" t="str">
-        <f t="array" ref="O2:R2">B2:F2</f>
-        <v>@terms</v>
-      </c>
-      <c r="P2" t="str">
-        <v>total Sinatra time</v>
-      </c>
-      <c r="Q2" t="str">
-        <v>onload</v>
-      </c>
-      <c r="R2" t="str">
-        <v>non-Sinatra</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3">
-        <f>AVERAGE(B6:B32)</f>
-        <v>0.45378159999999956</v>
-      </c>
-      <c r="C3">
-        <f t="shared" ref="C3:L3" si="0">AVERAGE(C6:C32)</f>
-        <v>1.1975714</v>
-      </c>
-      <c r="D3">
-        <f t="shared" si="0"/>
-        <v>2.5720000000000001</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3" si="1">AVERAGE(E6:E32)</f>
-        <v>1.3744286000000001</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>134.80000000000001</v>
-      </c>
-      <c r="H3">
-        <f t="shared" si="0"/>
-        <v>0.43725959999999964</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>1.1572868000000001</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>2.4740000000000002</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3" si="2">AVERAGE(K6:K32)</f>
-        <v>1.3167132000000001</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>69.7</v>
-      </c>
-      <c r="N3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3">
-        <f>B3-H3</f>
-        <v>1.6521999999999926E-2</v>
-      </c>
-      <c r="P3">
-        <f>C3-I3</f>
-        <v>4.0284599999999893E-2</v>
-      </c>
-      <c r="Q3">
-        <f>D3-J3</f>
-        <v>9.7999999999999865E-2</v>
-      </c>
-      <c r="R3">
-        <f>E3-K3</f>
-        <v>5.7715399999999972E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4">
-        <f>STDEVA(B6:B32)</f>
-        <v>2.0870108895260892E-2</v>
-      </c>
-      <c r="C4">
-        <f t="shared" ref="C4:J4" si="3">STDEVA(C6:C32)</f>
-        <v>4.3157184561784891E-2</v>
-      </c>
-      <c r="D4">
-        <f t="shared" si="3"/>
-        <v>6.8337398253059706E-2</v>
-      </c>
-      <c r="E4">
-        <f t="shared" ref="E4" si="4">STDEVA(E6:E32)</f>
-        <v>2.7504719218717954E-2</v>
-      </c>
-      <c r="H4">
-        <f t="shared" si="3"/>
-        <v>2.5346738297066202E-2</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="3"/>
-        <v>3.5277761461013364E-2</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="3"/>
-        <v>0.11458621208504334</v>
-      </c>
-      <c r="K4">
-        <f t="shared" ref="K4" si="5">STDEVA(K6:K32)</f>
-        <v>9.4835850044695941E-2</v>
-      </c>
-      <c r="N4" t="s">
-        <v>46</v>
-      </c>
-      <c r="O4" s="5">
-        <f>O3*1000</f>
-        <v>16.521999999999927</v>
-      </c>
-      <c r="P4" s="5">
-        <f t="shared" ref="P4:R4" si="6">P3*1000</f>
-        <v>40.284599999999891</v>
-      </c>
-      <c r="Q4" s="5">
-        <f t="shared" si="6"/>
-        <v>97.999999999999858</v>
-      </c>
-      <c r="R4" s="5">
-        <f t="shared" si="6"/>
-        <v>57.715399999999974</v>
-      </c>
-    </row>
-    <row r="5" spans="1:18">
-      <c r="A5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="1">
-        <f>B4/B3</f>
-        <v>4.5991527411558583E-2</v>
-      </c>
-      <c r="C5" s="1">
-        <f t="shared" ref="C5:K5" si="7">C4/C3</f>
-        <v>3.6037253863765363E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" si="7"/>
-        <v>2.656975048719273E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="7"/>
-        <v>2.0011748313966946E-2</v>
-      </c>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1">
-        <f t="shared" si="7"/>
-        <v>5.7967253999834933E-2</v>
-      </c>
-      <c r="I5" s="1">
-        <f t="shared" si="7"/>
-        <v>3.0483162394156195E-2</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="7"/>
-        <v>4.6316173033566423E-2</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="7"/>
-        <v>7.2024682402132778E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:18">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>0.43260199999999999</v>
-      </c>
-      <c r="C6">
-        <v>1.2069000000000001</v>
-      </c>
-      <c r="D6">
-        <v>2.59</v>
-      </c>
-      <c r="E6">
-        <f>D6-C6</f>
-        <v>1.3830999999999998</v>
-      </c>
-      <c r="F6">
-        <v>134.80000000000001</v>
-      </c>
-      <c r="H6">
-        <v>0.44712800000000003</v>
-      </c>
-      <c r="I6">
-        <v>1.1972499999999999</v>
-      </c>
-      <c r="J6">
-        <v>2.67</v>
-      </c>
-      <c r="K6">
-        <f>J6-I6</f>
-        <v>1.47275</v>
-      </c>
-      <c r="L6">
-        <v>69.7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:18">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>0.46669099999999902</v>
-      </c>
-      <c r="C7">
-        <v>1.2588010000000001</v>
-      </c>
-      <c r="D7">
-        <v>2.66</v>
-      </c>
-      <c r="E7">
-        <f t="shared" ref="E7:E10" si="8">D7-C7</f>
-        <v>1.4011990000000001</v>
-      </c>
-      <c r="H7">
-        <v>0.440271999999999</v>
-      </c>
-      <c r="I7">
-        <v>1.1428370000000001</v>
-      </c>
-      <c r="J7">
-        <v>2.37</v>
-      </c>
-      <c r="K7">
-        <f t="shared" ref="K7:K10" si="9">J7-I7</f>
-        <v>1.227163</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>0.44835399999999997</v>
-      </c>
-      <c r="C8">
-        <v>1.138239</v>
-      </c>
-      <c r="D8">
-        <v>2.4700000000000002</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="8"/>
-        <v>1.3317610000000002</v>
-      </c>
-      <c r="H8">
-        <v>0.44775199999999898</v>
-      </c>
-      <c r="I8">
-        <v>1.18065</v>
-      </c>
-      <c r="J8">
-        <v>2.44</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="9"/>
-        <v>1.25935</v>
-      </c>
-    </row>
-    <row r="9" spans="1:18">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>0.43822799999999901</v>
-      </c>
-      <c r="C9">
-        <v>1.1958789999999999</v>
-      </c>
-      <c r="D9">
-        <v>2.56</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="8"/>
-        <v>1.3641210000000001</v>
-      </c>
-      <c r="H9">
-        <v>0.39332299999999998</v>
-      </c>
-      <c r="I9">
-        <v>1.1060909999999999</v>
-      </c>
-      <c r="J9">
-        <v>2.4300000000000002</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="9"/>
-        <v>1.3239090000000002</v>
-      </c>
-    </row>
-    <row r="10" spans="1:18">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>0.48303299999999999</v>
-      </c>
-      <c r="C10">
-        <v>1.1880379999999999</v>
-      </c>
-      <c r="D10">
-        <v>2.58</v>
-      </c>
-      <c r="E10">
-        <f t="shared" si="8"/>
-        <v>1.3919620000000001</v>
-      </c>
-      <c r="H10">
-        <v>0.45782299999999998</v>
-      </c>
-      <c r="I10">
-        <v>1.1596059999999999</v>
-      </c>
-      <c r="J10">
-        <v>2.46</v>
-      </c>
-      <c r="K10">
-        <f t="shared" si="9"/>
-        <v>1.300394</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4"/>
-    </row>
-  </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
-  <mergeCells count="3">
-    <mergeCell ref="N1:R1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="H1:K1"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Trying to get to work on OpenShift hosting: added config.ru
</commit_message>
<xml_diff>
--- a/Utilities.xlsx
+++ b/Utilities.xlsx
@@ -4,24 +4,25 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="25540" yWindow="16660" windowWidth="25600" windowHeight="14620" tabRatio="843"/>
+    <workbookView xWindow="25500" yWindow="15400" windowWidth="25360" windowHeight="4680" tabRatio="843"/>
   </bookViews>
   <sheets>
-    <sheet name="home_static" sheetId="16" r:id="rId1"/>
-    <sheet name="storing properties" sheetId="15" r:id="rId2"/>
-    <sheet name="pt_main loop type" sheetId="14" r:id="rId3"/>
-    <sheet name="storing element.group" sheetId="13" r:id="rId4"/>
-    <sheet name="if else pos neg" sheetId="12" r:id="rId5"/>
-    <sheet name="for vs .each" sheetId="11" r:id="rId6"/>
-    <sheet name="@timing framework" sheetId="10" r:id="rId7"/>
-    <sheet name="@orbital_hash" sheetId="9" r:id="rId8"/>
-    <sheet name="term_spans" sheetId="8" r:id="rId9"/>
-    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId10"/>
-    <sheet name="custom pt_element_home" sheetId="6" r:id="rId11"/>
-    <sheet name="span_ec" sheetId="5" r:id="rId12"/>
-    <sheet name="ec_class accumulated" sheetId="4" r:id="rId13"/>
-    <sheet name="db query vs get" sheetId="2" r:id="rId14"/>
-    <sheet name="ec_class" sheetId="1" r:id="rId15"/>
+    <sheet name="home_static no blank lines" sheetId="17" r:id="rId1"/>
+    <sheet name="home_static" sheetId="16" r:id="rId2"/>
+    <sheet name="storing properties" sheetId="15" r:id="rId3"/>
+    <sheet name="pt_main loop type" sheetId="14" r:id="rId4"/>
+    <sheet name="storing element.group" sheetId="13" r:id="rId5"/>
+    <sheet name="if else pos neg" sheetId="12" r:id="rId6"/>
+    <sheet name="for vs .each" sheetId="11" r:id="rId7"/>
+    <sheet name="@timing framework" sheetId="10" r:id="rId8"/>
+    <sheet name="@orbital_hash" sheetId="9" r:id="rId9"/>
+    <sheet name="term_spans" sheetId="8" r:id="rId10"/>
+    <sheet name="custom pt_element_home total" sheetId="7" r:id="rId11"/>
+    <sheet name="custom pt_element_home" sheetId="6" r:id="rId12"/>
+    <sheet name="span_ec" sheetId="5" r:id="rId13"/>
+    <sheet name="ec_class accumulated" sheetId="4" r:id="rId14"/>
+    <sheet name="db query vs get" sheetId="2" r:id="rId15"/>
+    <sheet name="ec_class" sheetId="1" r:id="rId16"/>
   </sheets>
   <calcPr calcId="130407" concurrentCalc="0"/>
   <extLst>
@@ -33,13 +34,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="76">
   <si>
     <t>computing home.erb</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>using home_static.erb</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static home.erb with blank lines</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>static home.erb without blank lines</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
@@ -317,7 +326,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
   <fonts count="3">
@@ -988,41 +1001,41 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="15" t="s">
-        <v>1</v>
-      </c>
-      <c r="H1" s="16"/>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
+      <c r="G1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
       <c r="L1" s="17" t="str">
         <f>B1</f>
-        <v>computing home.erb</v>
+        <v>static home.erb with blank lines</v>
       </c>
       <c r="M1" s="17"/>
       <c r="N1" s="17"/>
       <c r="O1" s="18" t="str">
         <f>G1</f>
-        <v>using home_static.erb</v>
+        <v>static home.erb without blank lines</v>
       </c>
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1056,13 +1069,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -1075,70 +1088,70 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3">
-        <v>1.81</v>
-      </c>
-      <c r="C3">
-        <v>1.78</v>
-      </c>
-      <c r="D3">
-        <v>1.83</v>
-      </c>
-      <c r="E3">
-        <v>1.9</v>
-      </c>
-      <c r="F3">
-        <v>2.21</v>
+        <v>47</v>
+      </c>
+      <c r="B3" s="8">
+        <v>1.34</v>
+      </c>
+      <c r="C3" s="22">
+        <v>1.52</v>
+      </c>
+      <c r="D3" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="E3" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="F3" s="22">
+        <v>1.31</v>
       </c>
       <c r="G3" s="8">
-        <v>1.34</v>
+        <v>1.54</v>
       </c>
       <c r="H3" s="22">
-        <v>1.52</v>
+        <v>1.27</v>
       </c>
       <c r="I3" s="22">
-        <v>1.46</v>
+        <v>1.51</v>
       </c>
       <c r="J3" s="22">
-        <v>1.46</v>
+        <v>1.4</v>
       </c>
       <c r="K3" s="22">
-        <v>1.31</v>
+        <v>1.3</v>
       </c>
       <c r="L3" s="8">
         <f>AVERAGE(B3:K3)</f>
-        <v>1.6620000000000001</v>
+        <v>1.411</v>
       </c>
       <c r="M3">
         <f>STDEVA(B3:F3)</f>
-        <v>0.17558473737770897</v>
+        <v>8.8994381845150045E-2</v>
       </c>
       <c r="N3" s="7">
         <f>M3/L3</f>
-        <v>0.10564665305517987</v>
+        <v>6.3071851059638584E-2</v>
       </c>
       <c r="O3" s="8">
         <f t="shared" ref="O3:O20" si="0">AVERAGE(G3:K3)</f>
-        <v>1.4179999999999999</v>
+        <v>1.4040000000000001</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P20" si="1">STDEVA(G3:K3)</f>
-        <v>8.8994381845150045E-2</v>
+        <v>0.12095453691366452</v>
       </c>
       <c r="Q3" s="7">
         <f>P3/O3</f>
-        <v>6.276049495426661E-2</v>
+        <v>8.6149955066712608E-2</v>
       </c>
       <c r="R3" s="8">
         <f>O3-L3</f>
-        <v>-0.24400000000000022</v>
+        <v>-6.9999999999998952E-3</v>
       </c>
     </row>
     <row r="18" spans="1:18" s="13" customFormat="1">
@@ -1181,6 +1194,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -1190,6 +1204,529 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:V17"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="2" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" customWidth="1"/>
+    <col min="8" max="8" width="4.85546875" customWidth="1"/>
+    <col min="9" max="9" width="10.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" customWidth="1"/>
+    <col min="12" max="12" width="7.7109375" customWidth="1"/>
+    <col min="13" max="13" width="6.85546875" customWidth="1"/>
+    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.85546875" customWidth="1"/>
+    <col min="16" max="16" width="3.28515625" customWidth="1"/>
+    <col min="17" max="17" width="8.5703125" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" customWidth="1"/>
+    <col min="19" max="20" width="9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:22">
+      <c r="A1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="20"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+    </row>
+    <row r="2" spans="1:22">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="2" t="str">
+        <f t="array" ref="I2:N2">B2:G2</f>
+        <v>@terms</v>
+      </c>
+      <c r="J2" t="str">
+        <v>in e config</v>
+      </c>
+      <c r="K2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="L2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="M2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="N2" t="str">
+        <v>file size (k)</v>
+      </c>
+      <c r="Q2" s="2" t="str">
+        <f t="array" ref="Q2:V2">B2:G2</f>
+        <v>@terms</v>
+      </c>
+      <c r="R2" t="str">
+        <v>in e config</v>
+      </c>
+      <c r="S2" t="str">
+        <v>total Sinatra time</v>
+      </c>
+      <c r="T2" t="str">
+        <v>onload</v>
+      </c>
+      <c r="U2" t="str">
+        <v>non-Sinatra</v>
+      </c>
+      <c r="V2" t="str">
+        <v>file size (k)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <f>AVERAGE(B6:B32)</f>
+        <v>0.5009969999999998</v>
+      </c>
+      <c r="C3">
+        <f>AVERAGE(C6:C32)</f>
+        <v>0.95898819999999974</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:K3" si="0">AVERAGE(D6:D32)</f>
+        <v>1.3245984</v>
+      </c>
+      <c r="E3">
+        <f t="shared" si="0"/>
+        <v>3.0500000000000003</v>
+      </c>
+      <c r="F3">
+        <f t="shared" si="0"/>
+        <v>1.7254016000000001</v>
+      </c>
+      <c r="G3">
+        <v>67.3</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="0"/>
+        <v>0.55348319999999984</v>
+      </c>
+      <c r="J3">
+        <f t="shared" si="0"/>
+        <v>1.1211011999999978</v>
+      </c>
+      <c r="K3">
+        <f t="shared" si="0"/>
+        <v>1.4813308000000001</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:M3" si="1">AVERAGE(L6:L32)</f>
+        <v>3.468</v>
+      </c>
+      <c r="M3">
+        <f t="shared" si="1"/>
+        <v>1.9866692000000001</v>
+      </c>
+      <c r="N3">
+        <v>106.7</v>
+      </c>
+      <c r="P3" t="s">
+        <v>43</v>
+      </c>
+      <c r="Q3">
+        <f>B3-I3</f>
+        <v>-5.2486200000000038E-2</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:U3" si="2">C3-J3</f>
+        <v>-0.16211299999999806</v>
+      </c>
+      <c r="S3">
+        <f t="shared" si="2"/>
+        <v>-0.1567324000000001</v>
+      </c>
+      <c r="T3">
+        <f t="shared" si="2"/>
+        <v>-0.41799999999999971</v>
+      </c>
+      <c r="U3">
+        <f t="shared" si="2"/>
+        <v>-0.26126760000000004</v>
+      </c>
+      <c r="V3">
+        <f>G3-N3</f>
+        <v>-39.400000000000006</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <f>STDEVA(B6:B32)</f>
+        <v>5.3914485354123132E-2</v>
+      </c>
+      <c r="C4">
+        <f>STDEVA(C6:C32)</f>
+        <v>7.1833464563531013E-2</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:K4" si="3">STDEVA(D6:D32)</f>
+        <v>9.4934143127222176E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>0.29824486584013271</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="3"/>
+        <v>0.22816090053140187</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="3"/>
+        <v>9.7315476406376278E-2</v>
+      </c>
+      <c r="J4">
+        <f t="shared" si="3"/>
+        <v>0.19036480990902901</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="3"/>
+        <v>0.24516197712777557</v>
+      </c>
+      <c r="L4">
+        <f t="shared" ref="L4:M4" si="4">STDEVA(L6:L32)</f>
+        <v>0.43677225186589419</v>
+      </c>
+      <c r="M4">
+        <f t="shared" si="4"/>
+        <v>0.33879452626806195</v>
+      </c>
+      <c r="P4" t="s">
+        <v>50</v>
+      </c>
+      <c r="Q4" s="5">
+        <f>Q3*1000</f>
+        <v>-52.486200000000039</v>
+      </c>
+      <c r="R4" s="5">
+        <f t="shared" ref="R4:U4" si="5">R3*1000</f>
+        <v>-162.11299999999807</v>
+      </c>
+      <c r="S4" s="5">
+        <f t="shared" si="5"/>
+        <v>-156.7324000000001</v>
+      </c>
+      <c r="T4" s="5">
+        <f t="shared" si="5"/>
+        <v>-417.99999999999972</v>
+      </c>
+      <c r="U4" s="5">
+        <f t="shared" si="5"/>
+        <v>-261.26760000000002</v>
+      </c>
+      <c r="V4" s="5"/>
+    </row>
+    <row r="5" spans="1:22">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1">
+        <f>B4/B3</f>
+        <v>0.10761438761933335</v>
+      </c>
+      <c r="C5" s="1">
+        <f>C4/C3</f>
+        <v>7.4905472834317491E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <f t="shared" ref="D5:K5" si="6">D4/D3</f>
+        <v>7.1670132718884588E-2</v>
+      </c>
+      <c r="E5" s="1">
+        <f t="shared" si="6"/>
+        <v>9.7785201914797601E-2</v>
+      </c>
+      <c r="F5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.13223640254616773</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.17582372221302525</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.16980162888865821</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="6"/>
+        <v>0.16550116768501374</v>
+      </c>
+      <c r="L5" s="1">
+        <f t="shared" ref="L5" si="7">L4/L3</f>
+        <v>0.12594355590135356</v>
+      </c>
+      <c r="M5" s="1">
+        <f t="shared" ref="M5" si="8">M4/M3</f>
+        <v>0.17053394005809419</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0.51501599999999903</v>
+      </c>
+      <c r="C6">
+        <v>0.92809899999999901</v>
+      </c>
+      <c r="D6">
+        <v>1.246054</v>
+      </c>
+      <c r="E6">
+        <v>2.9</v>
+      </c>
+      <c r="F6">
+        <f>E6-D6</f>
+        <v>1.6539459999999999</v>
+      </c>
+      <c r="I6">
+        <v>0.69593300000000002</v>
+      </c>
+      <c r="J6">
+        <v>1.4183220000000001</v>
+      </c>
+      <c r="K6">
+        <v>1.857729</v>
+      </c>
+      <c r="L6">
+        <v>3.6</v>
+      </c>
+      <c r="M6">
+        <f>L6-K6</f>
+        <v>1.7422710000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7">
+        <v>0.47409800000000002</v>
+      </c>
+      <c r="C7">
+        <v>0.96557700000000002</v>
+      </c>
+      <c r="D7">
+        <v>1.289107</v>
+      </c>
+      <c r="E7">
+        <v>3.1</v>
+      </c>
+      <c r="F7">
+        <f t="shared" ref="F7:F10" si="9">E7-D7</f>
+        <v>1.8108930000000001</v>
+      </c>
+      <c r="I7">
+        <v>0.50989899999999999</v>
+      </c>
+      <c r="J7">
+        <v>1.0646149999999901</v>
+      </c>
+      <c r="K7">
+        <v>1.3850290000000001</v>
+      </c>
+      <c r="L7">
+        <v>3.26</v>
+      </c>
+      <c r="M7">
+        <f t="shared" ref="M7:M10" si="10">L7-K7</f>
+        <v>1.8749709999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>0.45488800000000001</v>
+      </c>
+      <c r="C8">
+        <v>0.88311899999999999</v>
+      </c>
+      <c r="D8">
+        <v>1.25692</v>
+      </c>
+      <c r="E8">
+        <v>2.87</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="9"/>
+        <v>1.6130800000000001</v>
+      </c>
+      <c r="I8">
+        <v>0.60211199999999898</v>
+      </c>
+      <c r="J8">
+        <v>1.1913959999999999</v>
+      </c>
+      <c r="K8">
+        <v>1.59188</v>
+      </c>
+      <c r="L8">
+        <v>4.16</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="10"/>
+        <v>2.5681200000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22">
+      <c r="A9">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>0.58897699999999997</v>
+      </c>
+      <c r="C9">
+        <v>1.0756669999999999</v>
+      </c>
+      <c r="D9">
+        <v>1.476818</v>
+      </c>
+      <c r="E9">
+        <v>3.55</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="9"/>
+        <v>2.0731820000000001</v>
+      </c>
+      <c r="I9">
+        <v>0.44475300000000001</v>
+      </c>
+      <c r="J9">
+        <v>0.95806499999999895</v>
+      </c>
+      <c r="K9">
+        <v>1.3077430000000001</v>
+      </c>
+      <c r="L9">
+        <v>3.29</v>
+      </c>
+      <c r="M9">
+        <f t="shared" si="10"/>
+        <v>1.9822569999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22">
+      <c r="A10">
+        <v>5</v>
+      </c>
+      <c r="B10">
+        <v>0.47200599999999998</v>
+      </c>
+      <c r="C10">
+        <v>0.94247899999999996</v>
+      </c>
+      <c r="D10">
+        <v>1.354093</v>
+      </c>
+      <c r="E10">
+        <v>2.83</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="9"/>
+        <v>1.4759070000000001</v>
+      </c>
+      <c r="I10">
+        <v>0.51471900000000004</v>
+      </c>
+      <c r="J10">
+        <v>0.97310799999999997</v>
+      </c>
+      <c r="K10">
+        <v>1.264273</v>
+      </c>
+      <c r="L10">
+        <v>3.03</v>
+      </c>
+      <c r="M10">
+        <f t="shared" si="10"/>
+        <v>1.7657269999999998</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22">
+      <c r="A16" s="4"/>
+    </row>
+    <row r="17" spans="1:1">
+      <c r="A17" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="P1:T1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R17"/>
   <sheetViews>
@@ -1217,10 +1754,10 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -1228,7 +1765,7 @@
       <c r="F1" s="20"/>
       <c r="G1" s="3"/>
       <c r="H1" s="14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="I1" s="14"/>
       <c r="J1" s="14"/>
@@ -1236,7 +1773,7 @@
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
       <c r="N1" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="O1" s="14"/>
       <c r="P1" s="14"/>
@@ -1245,22 +1782,22 @@
     </row>
     <row r="2" spans="1:18">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D2" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="E2" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="F2" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="H2" s="2" t="str">
         <f t="array" ref="H2:K2">B2:F2</f>
@@ -1291,7 +1828,7 @@
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1334,7 +1871,7 @@
         <v>69.7</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="O3">
         <f>B3-H3</f>
@@ -1355,7 +1892,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1390,7 +1927,7 @@
         <v>9.4835850044695941E-2</v>
       </c>
       <c r="N4" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="O4" s="5">
         <f>O3*1000</f>
@@ -1411,7 +1948,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1632,7 +2169,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:J12"/>
   <sheetViews>
@@ -1652,45 +2189,45 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="20" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C1" s="20"/>
       <c r="D1" s="3"/>
       <c r="E1" s="20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F1" s="20"/>
       <c r="G1" s="3"/>
       <c r="H1" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="C2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1705,12 +2242,12 @@
         <v>1.3408000000000531E-2</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:10">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1729,12 +2266,12 @@
         <v>0</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1811,7 +2348,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <mergeCells count="2">
     <mergeCell ref="E1:F1"/>
     <mergeCell ref="B1:C1"/>
@@ -1826,7 +2362,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -1842,26 +2378,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D1" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -1874,7 +2410,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -1887,7 +2423,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -1970,7 +2506,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -1981,7 +2516,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -1997,26 +2532,26 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2029,7 +2564,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2042,7 +2577,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2109,7 +2644,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2120,7 +2654,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -2136,20 +2670,20 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="B1" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2162,7 +2696,7 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2175,7 +2709,7 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2242,7 +2776,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2253,7 +2786,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:F10"/>
   <sheetViews>
@@ -2270,32 +2803,32 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="B1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="E2" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -2316,7 +2849,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -2337,7 +2870,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -2442,7 +2975,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetCalcPr fullCalcOnLoad="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <extLst>
@@ -2454,6 +2986,233 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
+  <dimension ref="A1:R20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozenSplit"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L3" sqref="L3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="2" max="6" width="7.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.7109375" style="8" customWidth="1"/>
+    <col min="8" max="11" width="7.7109375" customWidth="1"/>
+    <col min="12" max="12" width="10.7109375" style="8"/>
+    <col min="14" max="14" width="8.5703125" style="7" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" style="8"/>
+    <col min="17" max="17" width="8.5703125" style="7" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="17" t="str">
+        <f>B1</f>
+        <v>computing home.erb</v>
+      </c>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="18" t="str">
+        <f>G1</f>
+        <v>using home_static.erb</v>
+      </c>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18">
+      <c r="A2" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>3</v>
+      </c>
+      <c r="E2">
+        <v>4</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2" s="8">
+        <f t="array" ref="G2:K2">B2:F2</f>
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>2</v>
+      </c>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" s="8" t="str">
+        <f t="array" ref="O2:Q2">L2:N2</f>
+        <v>Avg</v>
+      </c>
+      <c r="P2" t="str">
+        <v>StDev</v>
+      </c>
+      <c r="Q2" s="7" t="str">
+        <v>RelStdDev</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3">
+        <v>1.81</v>
+      </c>
+      <c r="C3">
+        <v>1.78</v>
+      </c>
+      <c r="D3">
+        <v>1.83</v>
+      </c>
+      <c r="E3">
+        <v>1.9</v>
+      </c>
+      <c r="F3">
+        <v>2.21</v>
+      </c>
+      <c r="G3" s="8">
+        <v>1.34</v>
+      </c>
+      <c r="H3" s="22">
+        <v>1.52</v>
+      </c>
+      <c r="I3" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="J3" s="22">
+        <v>1.46</v>
+      </c>
+      <c r="K3" s="22">
+        <v>1.31</v>
+      </c>
+      <c r="L3" s="8">
+        <f>AVERAGE(B3:K3)</f>
+        <v>1.6620000000000001</v>
+      </c>
+      <c r="M3">
+        <f>STDEVA(B3:F3)</f>
+        <v>0.17558473737770897</v>
+      </c>
+      <c r="N3" s="7">
+        <f>M3/L3</f>
+        <v>0.10564665305517987</v>
+      </c>
+      <c r="O3" s="8">
+        <f t="shared" ref="O3:O20" si="0">AVERAGE(G3:K3)</f>
+        <v>1.4179999999999999</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P20" si="1">STDEVA(G3:K3)</f>
+        <v>8.8994381845150045E-2</v>
+      </c>
+      <c r="Q3" s="7">
+        <f>P3/O3</f>
+        <v>6.276049495426661E-2</v>
+      </c>
+      <c r="R3" s="8">
+        <f>O3-L3</f>
+        <v>-0.24400000000000022</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" s="13" customFormat="1">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18" s="8"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18" s="8"/>
+      <c r="M18"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="8"/>
+      <c r="P18"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="8"/>
+    </row>
+    <row r="19" spans="1:18" ht="14" thickBot="1">
+      <c r="G19" s="12"/>
+    </row>
+    <row r="20" spans="1:18" s="9" customFormat="1">
+      <c r="G20" s="11"/>
+      <c r="L20" s="11"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="11"/>
+      <c r="Q20" s="10"/>
+      <c r="R20" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R20"/>
   <sheetViews>
@@ -2479,17 +3238,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -2508,12 +3267,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2547,13 +3306,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -2566,12 +3325,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B3">
         <v>0.52637100000000003</v>
@@ -2680,7 +3439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R21"/>
   <sheetViews>
@@ -2706,17 +3465,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -2735,12 +3494,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -2774,13 +3533,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -2793,12 +3552,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B3">
         <v>1.1590000000000001E-3</v>
@@ -2846,7 +3605,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B4">
         <v>9.4499999999999998E-4</v>
@@ -2894,7 +3653,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B5">
         <v>6.3940000000000004E-3</v>
@@ -2942,7 +3701,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B6">
         <v>5.9379999999999997E-3</v>
@@ -2990,7 +3749,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B7">
         <v>2.4650000000000002E-3</v>
@@ -3038,7 +3797,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B8">
         <v>0.23839399999999999</v>
@@ -3086,7 +3845,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B9">
         <v>2.5820000000000001E-3</v>
@@ -3134,7 +3893,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B10">
         <v>5.2374999999999998E-2</v>
@@ -3182,7 +3941,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B11">
         <v>2.2130000000000001E-3</v>
@@ -3230,7 +3989,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B12">
         <v>0.16836200000000001</v>
@@ -3278,7 +4037,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>8.6200000000000003E-4</v>
@@ -3326,7 +4085,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B14">
         <v>5.5449999999999996E-3</v>
@@ -3374,7 +4133,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B15">
         <v>3.1979999999999999E-3</v>
@@ -3422,7 +4181,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B16">
         <v>1.769E-3</v>
@@ -3470,7 +4229,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B17">
         <v>1.993E-3</v>
@@ -3518,7 +4277,7 @@
     </row>
     <row r="18" spans="1:18" s="13" customFormat="1">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B18">
         <v>0.49546000000000001</v>
@@ -3571,7 +4330,7 @@
     </row>
     <row r="19" spans="1:18" ht="14" thickBot="1">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B19">
         <v>0.67658300000000005</v>
@@ -3620,7 +4379,7 @@
     </row>
     <row r="20" spans="1:18" s="9" customFormat="1">
       <c r="A20" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B20" s="9">
         <f>SUM(B3:B18)</f>
@@ -3693,7 +4452,7 @@
     </row>
     <row r="21" spans="1:18">
       <c r="A21" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <f>B19-B18</f>
@@ -3781,7 +4540,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -3807,17 +4566,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -3836,12 +4595,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -3875,13 +4634,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -3894,12 +4653,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="8">
         <v>8.8199999999999997E-4</v>
@@ -3962,7 +4721,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B4" s="8">
         <v>5.5449999999999996E-3</v>
@@ -4024,7 +4783,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5" s="8">
         <v>3.5990000000000002E-3</v>
@@ -4086,7 +4845,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B6" s="8">
         <v>0.237287</v>
@@ -4148,7 +4907,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B7" s="8">
         <v>3.7789999999999998E-3</v>
@@ -4210,7 +4969,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B8" s="8">
         <v>4.7253000000000003E-2</v>
@@ -4272,7 +5031,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B9" s="8">
         <v>1.936E-3</v>
@@ -4334,7 +5093,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10" s="8">
         <v>0.142016</v>
@@ -4396,7 +5155,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B11" s="8">
         <v>8.6300000000000005E-4</v>
@@ -4458,7 +5217,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12" s="8">
         <v>4.8430000000000001E-3</v>
@@ -4520,7 +5279,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13" s="8">
         <v>2.7299999999999998E-3</v>
@@ -4582,7 +5341,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14" s="8">
         <v>1.7639999999999999E-3</v>
@@ -4644,7 +5403,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B15" s="8">
         <v>1.934E-3</v>
@@ -4706,7 +5465,7 @@
     </row>
     <row r="16" spans="1:18" ht="14" thickBot="1">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16" s="8">
         <v>0.59009500000000004</v>
@@ -4768,7 +5527,7 @@
     </row>
     <row r="17" spans="1:18" s="9" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17" s="9">
         <f>SUM(B3:B15)</f>
@@ -4841,7 +5600,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <f>B16-B17</f>
@@ -4929,7 +5688,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -4955,17 +5714,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="15" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="H1" s="16"/>
       <c r="I1" s="16"/>
@@ -4984,12 +5743,12 @@
       <c r="P1" s="17"/>
       <c r="Q1" s="17"/>
       <c r="R1" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -5023,13 +5782,13 @@
         <v>5</v>
       </c>
       <c r="L2" s="8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O2" s="8" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -5042,12 +5801,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" s="8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3">
         <v>7.2000000000000005E-4</v>
@@ -5110,7 +5869,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B4">
         <v>5.7739999999999996E-3</v>
@@ -5172,7 +5931,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B5">
         <v>3.506E-3</v>
@@ -5234,7 +5993,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B6">
         <v>0.23477999999999999</v>
@@ -5296,7 +6055,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B7">
         <v>4.3759999999999997E-3</v>
@@ -5358,7 +6117,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B8">
         <v>8.2308000000000006E-2</v>
@@ -5420,7 +6179,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B9">
         <v>2.1540000000000001E-3</v>
@@ -5482,7 +6241,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>0.131187</v>
@@ -5544,7 +6303,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>8.6600000000000002E-4</v>
@@ -5606,7 +6365,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>4.7499999999999999E-3</v>
@@ -5668,7 +6427,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>2.6059999999999998E-3</v>
@@ -5730,7 +6489,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>1.586E-3</v>
@@ -5792,7 +6551,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>1.9009999999999999E-3</v>
@@ -5854,7 +6613,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>0.64971699999999999</v>
@@ -5916,7 +6675,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <f>SUM(B3:B15)</f>
@@ -5989,7 +6748,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <f>B16-B17</f>
@@ -6077,7 +6836,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:R18"/>
   <sheetViews>
@@ -6098,17 +6857,17 @@
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
       <c r="G1" s="14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H1" s="14"/>
       <c r="I1" s="14"/>
@@ -6127,12 +6886,12 @@
       <c r="P1" s="19"/>
       <c r="Q1" s="19"/>
       <c r="R1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:18">
       <c r="A2" s="6" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -6166,13 +6925,13 @@
         <v>5</v>
       </c>
       <c r="L2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="M2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="N2" s="7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O2" t="str">
         <f t="array" ref="O2:Q2">L2:N2</f>
@@ -6185,12 +6944,12 @@
         <v>RelStdDev</v>
       </c>
       <c r="R2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B3">
         <v>5.3610000000000003E-3</v>
@@ -6253,7 +7012,7 @@
     </row>
     <row r="4" spans="1:18">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B4">
         <v>3.5630000000000002E-3</v>
@@ -6315,7 +7074,7 @@
     </row>
     <row r="5" spans="1:18">
       <c r="A5" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B5">
         <v>0.27063799999999999</v>
@@ -6377,7 +7136,7 @@
     </row>
     <row r="6" spans="1:18">
       <c r="A6" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B6">
         <v>4.0070000000000001E-3</v>
@@ -6439,7 +7198,7 @@
     </row>
     <row r="7" spans="1:18">
       <c r="A7" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B7">
         <v>4.6899000000000003E-2</v>
@@ -6501,7 +7260,7 @@
     </row>
     <row r="8" spans="1:18">
       <c r="A8" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B8">
         <v>2.0709999999999999E-3</v>
@@ -6563,7 +7322,7 @@
     </row>
     <row r="9" spans="1:18">
       <c r="A9" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B9">
         <v>0.124172</v>
@@ -6625,7 +7384,7 @@
     </row>
     <row r="10" spans="1:18">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B10">
         <v>3.503E-3</v>
@@ -6687,7 +7446,7 @@
     </row>
     <row r="11" spans="1:18">
       <c r="A11" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B11">
         <v>1.0169999999999999E-3</v>
@@ -6749,7 +7508,7 @@
     </row>
     <row r="12" spans="1:18">
       <c r="A12" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B12">
         <v>4.4000000000000003E-3</v>
@@ -6811,7 +7570,7 @@
     </row>
     <row r="13" spans="1:18">
       <c r="A13" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B13">
         <v>2.532E-3</v>
@@ -6873,7 +7632,7 @@
     </row>
     <row r="14" spans="1:18">
       <c r="A14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B14">
         <v>1.658E-3</v>
@@ -6935,7 +7694,7 @@
     </row>
     <row r="15" spans="1:18">
       <c r="A15" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B15">
         <v>1.8220000000000001E-3</v>
@@ -6997,7 +7756,7 @@
     </row>
     <row r="16" spans="1:18">
       <c r="A16" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B16">
         <v>0.60263599999999995</v>
@@ -7059,7 +7818,7 @@
     </row>
     <row r="17" spans="1:18">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17">
         <f>SUM(B3:B15)</f>
@@ -7132,7 +7891,7 @@
     </row>
     <row r="18" spans="1:18">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18">
         <f>B16-B17</f>
@@ -7220,7 +7979,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -7236,16 +7995,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D1" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -7399,7 +8158,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
   <dimension ref="A1:V17"/>
   <sheetViews>
@@ -7432,10 +8191,10 @@
   <sheetData>
     <row r="1" spans="1:22">
       <c r="A1" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
@@ -7444,7 +8203,7 @@
       <c r="G1" s="20"/>
       <c r="H1" s="3"/>
       <c r="I1" s="21" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="J1" s="14"/>
       <c r="K1" s="14"/>
@@ -7453,7 +8212,7 @@
       <c r="N1" s="3"/>
       <c r="O1" s="3"/>
       <c r="P1" s="14" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="Q1" s="14"/>
       <c r="R1" s="14"/>
@@ -7462,22 +8221,22 @@
     </row>
     <row r="2" spans="1:22">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="I2" s="2" t="str">
         <f t="array" ref="I2:N2">B2:G2</f>
@@ -7520,7 +8279,7 @@
     </row>
     <row r="3" spans="1:22">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B3">
         <f>AVERAGE(B6:B32)</f>
@@ -7563,7 +8322,7 @@
         <v>1.3500742000000001</v>
       </c>
       <c r="P3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="Q3" t="e">
         <f>B3-I3</f>
@@ -7592,7 +8351,7 @@
     </row>
     <row r="4" spans="1:22">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4">
         <f>STDEVA(B6:B32)</f>
@@ -7635,7 +8394,7 @@
         <v>0.13967913309510532</v>
       </c>
       <c r="P4" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="5" t="e">
         <f>Q3*1000</f>
@@ -7661,7 +8420,7 @@
     </row>
     <row r="5" spans="1:22">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B5" s="1">
         <f>B4/B3</f>
@@ -7844,529 +8603,6 @@
       <c r="M10">
         <f t="shared" si="14"/>
         <v>1.5923220000000002</v>
-      </c>
-    </row>
-    <row r="16" spans="1:22">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" spans="1:1">
-      <c r="A17" s="4"/>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="I1:L1"/>
-    <mergeCell ref="P1:T1"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:V17"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozenSplit"/>
-      <selection pane="topRight" activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
-  <cols>
-    <col min="2" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="5" max="5" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" customWidth="1"/>
-    <col min="8" max="8" width="4.85546875" customWidth="1"/>
-    <col min="9" max="9" width="10.5703125" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" customWidth="1"/>
-    <col min="12" max="12" width="7.7109375" customWidth="1"/>
-    <col min="13" max="13" width="6.85546875" customWidth="1"/>
-    <col min="14" max="14" width="9.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="2.85546875" customWidth="1"/>
-    <col min="16" max="16" width="3.28515625" customWidth="1"/>
-    <col min="17" max="17" width="8.5703125" customWidth="1"/>
-    <col min="18" max="18" width="9.85546875" customWidth="1"/>
-    <col min="19" max="20" width="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:22">
-      <c r="A1" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-      <c r="F1" s="14"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="J1" s="14"/>
-      <c r="K1" s="14"/>
-      <c r="L1" s="14"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="14" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q1" s="14"/>
-      <c r="R1" s="14"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
-    </row>
-    <row r="2" spans="1:22">
-      <c r="A2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
-      </c>
-      <c r="D2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I2" s="2" t="str">
-        <f t="array" ref="I2:N2">B2:G2</f>
-        <v>@terms</v>
-      </c>
-      <c r="J2" t="str">
-        <v>in e config</v>
-      </c>
-      <c r="K2" t="str">
-        <v>total Sinatra time</v>
-      </c>
-      <c r="L2" t="str">
-        <v>onload</v>
-      </c>
-      <c r="M2" t="str">
-        <v>non-Sinatra</v>
-      </c>
-      <c r="N2" t="str">
-        <v>file size (k)</v>
-      </c>
-      <c r="Q2" s="2" t="str">
-        <f t="array" ref="Q2:V2">B2:G2</f>
-        <v>@terms</v>
-      </c>
-      <c r="R2" t="str">
-        <v>in e config</v>
-      </c>
-      <c r="S2" t="str">
-        <v>total Sinatra time</v>
-      </c>
-      <c r="T2" t="str">
-        <v>onload</v>
-      </c>
-      <c r="U2" t="str">
-        <v>non-Sinatra</v>
-      </c>
-      <c r="V2" t="str">
-        <v>file size (k)</v>
-      </c>
-    </row>
-    <row r="3" spans="1:22">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <f>AVERAGE(B6:B32)</f>
-        <v>0.5009969999999998</v>
-      </c>
-      <c r="C3">
-        <f>AVERAGE(C6:C32)</f>
-        <v>0.95898819999999974</v>
-      </c>
-      <c r="D3">
-        <f t="shared" ref="D3:K3" si="0">AVERAGE(D6:D32)</f>
-        <v>1.3245984</v>
-      </c>
-      <c r="E3">
-        <f t="shared" si="0"/>
-        <v>3.0500000000000003</v>
-      </c>
-      <c r="F3">
-        <f t="shared" si="0"/>
-        <v>1.7254016000000001</v>
-      </c>
-      <c r="G3">
-        <v>67.3</v>
-      </c>
-      <c r="I3">
-        <f t="shared" si="0"/>
-        <v>0.55348319999999984</v>
-      </c>
-      <c r="J3">
-        <f t="shared" si="0"/>
-        <v>1.1211011999999978</v>
-      </c>
-      <c r="K3">
-        <f t="shared" si="0"/>
-        <v>1.4813308000000001</v>
-      </c>
-      <c r="L3">
-        <f t="shared" ref="L3:M3" si="1">AVERAGE(L6:L32)</f>
-        <v>3.468</v>
-      </c>
-      <c r="M3">
-        <f t="shared" si="1"/>
-        <v>1.9866692000000001</v>
-      </c>
-      <c r="N3">
-        <v>106.7</v>
-      </c>
-      <c r="P3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3">
-        <f>B3-I3</f>
-        <v>-5.2486200000000038E-2</v>
-      </c>
-      <c r="R3">
-        <f t="shared" ref="R3:U3" si="2">C3-J3</f>
-        <v>-0.16211299999999806</v>
-      </c>
-      <c r="S3">
-        <f t="shared" si="2"/>
-        <v>-0.1567324000000001</v>
-      </c>
-      <c r="T3">
-        <f t="shared" si="2"/>
-        <v>-0.41799999999999971</v>
-      </c>
-      <c r="U3">
-        <f t="shared" si="2"/>
-        <v>-0.26126760000000004</v>
-      </c>
-      <c r="V3">
-        <f>G3-N3</f>
-        <v>-39.400000000000006</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22">
-      <c r="A4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B4">
-        <f>STDEVA(B6:B32)</f>
-        <v>5.3914485354123132E-2</v>
-      </c>
-      <c r="C4">
-        <f>STDEVA(C6:C32)</f>
-        <v>7.1833464563531013E-2</v>
-      </c>
-      <c r="D4">
-        <f t="shared" ref="D4:K4" si="3">STDEVA(D6:D32)</f>
-        <v>9.4934143127222176E-2</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="3"/>
-        <v>0.29824486584013271</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="3"/>
-        <v>0.22816090053140187</v>
-      </c>
-      <c r="I4">
-        <f t="shared" si="3"/>
-        <v>9.7315476406376278E-2</v>
-      </c>
-      <c r="J4">
-        <f t="shared" si="3"/>
-        <v>0.19036480990902901</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="3"/>
-        <v>0.24516197712777557</v>
-      </c>
-      <c r="L4">
-        <f t="shared" ref="L4:M4" si="4">STDEVA(L6:L32)</f>
-        <v>0.43677225186589419</v>
-      </c>
-      <c r="M4">
-        <f t="shared" si="4"/>
-        <v>0.33879452626806195</v>
-      </c>
-      <c r="P4" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q4" s="5">
-        <f>Q3*1000</f>
-        <v>-52.486200000000039</v>
-      </c>
-      <c r="R4" s="5">
-        <f t="shared" ref="R4:U4" si="5">R3*1000</f>
-        <v>-162.11299999999807</v>
-      </c>
-      <c r="S4" s="5">
-        <f t="shared" si="5"/>
-        <v>-156.7324000000001</v>
-      </c>
-      <c r="T4" s="5">
-        <f t="shared" si="5"/>
-        <v>-417.99999999999972</v>
-      </c>
-      <c r="U4" s="5">
-        <f t="shared" si="5"/>
-        <v>-261.26760000000002</v>
-      </c>
-      <c r="V4" s="5"/>
-    </row>
-    <row r="5" spans="1:22">
-      <c r="A5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B5" s="1">
-        <f>B4/B3</f>
-        <v>0.10761438761933335</v>
-      </c>
-      <c r="C5" s="1">
-        <f>C4/C3</f>
-        <v>7.4905472834317491E-2</v>
-      </c>
-      <c r="D5" s="1">
-        <f t="shared" ref="D5:K5" si="6">D4/D3</f>
-        <v>7.1670132718884588E-2</v>
-      </c>
-      <c r="E5" s="1">
-        <f t="shared" si="6"/>
-        <v>9.7785201914797601E-2</v>
-      </c>
-      <c r="F5" s="1">
-        <f t="shared" si="6"/>
-        <v>0.13223640254616773</v>
-      </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1">
-        <f t="shared" si="6"/>
-        <v>0.17582372221302525</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="6"/>
-        <v>0.16980162888865821</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="6"/>
-        <v>0.16550116768501374</v>
-      </c>
-      <c r="L5" s="1">
-        <f t="shared" ref="L5" si="7">L4/L3</f>
-        <v>0.12594355590135356</v>
-      </c>
-      <c r="M5" s="1">
-        <f t="shared" ref="M5" si="8">M4/M3</f>
-        <v>0.17053394005809419</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22">
-      <c r="A6">
-        <v>1</v>
-      </c>
-      <c r="B6">
-        <v>0.51501599999999903</v>
-      </c>
-      <c r="C6">
-        <v>0.92809899999999901</v>
-      </c>
-      <c r="D6">
-        <v>1.246054</v>
-      </c>
-      <c r="E6">
-        <v>2.9</v>
-      </c>
-      <c r="F6">
-        <f>E6-D6</f>
-        <v>1.6539459999999999</v>
-      </c>
-      <c r="I6">
-        <v>0.69593300000000002</v>
-      </c>
-      <c r="J6">
-        <v>1.4183220000000001</v>
-      </c>
-      <c r="K6">
-        <v>1.857729</v>
-      </c>
-      <c r="L6">
-        <v>3.6</v>
-      </c>
-      <c r="M6">
-        <f>L6-K6</f>
-        <v>1.7422710000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:22">
-      <c r="A7">
-        <v>2</v>
-      </c>
-      <c r="B7">
-        <v>0.47409800000000002</v>
-      </c>
-      <c r="C7">
-        <v>0.96557700000000002</v>
-      </c>
-      <c r="D7">
-        <v>1.289107</v>
-      </c>
-      <c r="E7">
-        <v>3.1</v>
-      </c>
-      <c r="F7">
-        <f t="shared" ref="F7:F10" si="9">E7-D7</f>
-        <v>1.8108930000000001</v>
-      </c>
-      <c r="I7">
-        <v>0.50989899999999999</v>
-      </c>
-      <c r="J7">
-        <v>1.0646149999999901</v>
-      </c>
-      <c r="K7">
-        <v>1.3850290000000001</v>
-      </c>
-      <c r="L7">
-        <v>3.26</v>
-      </c>
-      <c r="M7">
-        <f t="shared" ref="M7:M10" si="10">L7-K7</f>
-        <v>1.8749709999999997</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22">
-      <c r="A8">
-        <v>3</v>
-      </c>
-      <c r="B8">
-        <v>0.45488800000000001</v>
-      </c>
-      <c r="C8">
-        <v>0.88311899999999999</v>
-      </c>
-      <c r="D8">
-        <v>1.25692</v>
-      </c>
-      <c r="E8">
-        <v>2.87</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="9"/>
-        <v>1.6130800000000001</v>
-      </c>
-      <c r="I8">
-        <v>0.60211199999999898</v>
-      </c>
-      <c r="J8">
-        <v>1.1913959999999999</v>
-      </c>
-      <c r="K8">
-        <v>1.59188</v>
-      </c>
-      <c r="L8">
-        <v>4.16</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="10"/>
-        <v>2.5681200000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22">
-      <c r="A9">
-        <v>4</v>
-      </c>
-      <c r="B9">
-        <v>0.58897699999999997</v>
-      </c>
-      <c r="C9">
-        <v>1.0756669999999999</v>
-      </c>
-      <c r="D9">
-        <v>1.476818</v>
-      </c>
-      <c r="E9">
-        <v>3.55</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="9"/>
-        <v>2.0731820000000001</v>
-      </c>
-      <c r="I9">
-        <v>0.44475300000000001</v>
-      </c>
-      <c r="J9">
-        <v>0.95806499999999895</v>
-      </c>
-      <c r="K9">
-        <v>1.3077430000000001</v>
-      </c>
-      <c r="L9">
-        <v>3.29</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="10"/>
-        <v>1.9822569999999999</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22">
-      <c r="A10">
-        <v>5</v>
-      </c>
-      <c r="B10">
-        <v>0.47200599999999998</v>
-      </c>
-      <c r="C10">
-        <v>0.94247899999999996</v>
-      </c>
-      <c r="D10">
-        <v>1.354093</v>
-      </c>
-      <c r="E10">
-        <v>2.83</v>
-      </c>
-      <c r="F10">
-        <f t="shared" si="9"/>
-        <v>1.4759070000000001</v>
-      </c>
-      <c r="I10">
-        <v>0.51471900000000004</v>
-      </c>
-      <c r="J10">
-        <v>0.97310799999999997</v>
-      </c>
-      <c r="K10">
-        <v>1.264273</v>
-      </c>
-      <c r="L10">
-        <v>3.03</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="10"/>
-        <v>1.7657269999999998</v>
       </c>
     </row>
     <row r="16" spans="1:22">

</xml_diff>